<commit_message>
adding missing translations to add_n footnotes
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8204ED-2E00-42CC-9BA5-961C668B21E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3995A0B5-73F7-45FD-802D-381BDA293D26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="11720" yWindow="1240" windowWidth="14400" windowHeight="7360" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="223">
   <si>
     <t>context</t>
   </si>
@@ -1065,21 +1065,21 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>194</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>194</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>203</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>203</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>203</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>203</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>203</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>203</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>203</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>203</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>203</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>203</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
added range to translation excel file
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52730DF3-65D6-47CC-9E48-9011099271DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B6283-E8C8-40FA-BE5E-8F47F16F2646}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="624">
   <si>
     <t>context</t>
   </si>
@@ -2008,6 +2008,9 @@
   </si>
   <si>
     <t>提示された統計</t>
+  </si>
+  <si>
+    <t>range</t>
   </si>
 </sst>
 </file>
@@ -2453,27 +2456,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="51.81640625" customWidth="1"/>
     <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.26953125" style="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" style="22" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="38.453125" style="14" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3335,7 +3338,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="15.5">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -4312,86 +4315,57 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="2" customFormat="1">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:13" s="12" customFormat="1">
+      <c r="A52" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="B52" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:13" s="2" customFormat="1">
       <c r="A53" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>407</v>
+        <v>565</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>406</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="H53" s="22" t="s">
-        <v>622</v>
+        <v>376</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>252</v>
+        <v>114</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1">
@@ -4399,22 +4373,40 @@
         <v>80</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>274</v>
+        <v>91</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="4"/>
-      <c r="J54" s="6" t="s">
-        <v>312</v>
+        <v>568</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="2" customFormat="1">
@@ -4422,22 +4414,22 @@
         <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>574</v>
+        <v>569</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>571</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="12"/>
       <c r="H55" s="4"/>
       <c r="J55" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="2" customFormat="1">
@@ -4445,40 +4437,22 @@
         <v>80</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>86</v>
+        <v>278</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>90</v>
+        <v>572</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="F56" s="14"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="4"/>
+      <c r="J56" s="6" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="2" customFormat="1">
@@ -4486,81 +4460,81 @@
         <v>80</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="2" customFormat="1">
+      <c r="A58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C58" s="22" t="s">
         <v>577</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D58" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E58" s="22" t="s">
         <v>579</v>
       </c>
-      <c r="F57" s="20" t="s">
+      <c r="F58" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G58" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="H58" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="J58" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="K58" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="L58" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="M58" s="2" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>581</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="J58" t="s">
-        <v>196</v>
-      </c>
-      <c r="K58" t="s">
-        <v>197</v>
-      </c>
-      <c r="L58" t="s">
-        <v>195</v>
-      </c>
-      <c r="M58" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -4568,352 +4542,393 @@
         <v>194</v>
       </c>
       <c r="B59" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J59" t="s">
+        <v>196</v>
+      </c>
+      <c r="K59" t="s">
+        <v>197</v>
+      </c>
+      <c r="L59" t="s">
+        <v>195</v>
+      </c>
+      <c r="M59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" t="s">
         <v>198</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C60" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>584</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E60" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F60" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G59" s="12" t="s">
+      <c r="G60" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="I60" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J60" t="s">
         <v>199</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K60" t="s">
         <v>200</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L60" t="s">
         <v>201</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M60" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30">
-      <c r="A60" t="s">
-        <v>203</v>
-      </c>
-      <c r="B60" t="s">
-        <v>207</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>586</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="F60" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="30">
+    <row r="61" spans="1:13" ht="29">
       <c r="A61" t="s">
         <v>203</v>
       </c>
       <c r="B61" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>412</v>
+        <v>588</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>411</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="J61" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="30">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="29">
       <c r="A62" t="s">
         <v>203</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="G62" s="12"/>
+        <v>412</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
       <c r="J62" s="5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="30">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="29">
       <c r="A63" t="s">
         <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>368</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="29">
       <c r="A64" t="s">
         <v>203</v>
       </c>
       <c r="B64" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>600</v>
+        <v>596</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>597</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="J64" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>203</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>603</v>
+        <v>599</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>600</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1"/>
       <c r="J65" s="5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="30">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="29">
       <c r="A66" t="s">
         <v>203</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="1"/>
       <c r="J66" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="30">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="29">
       <c r="A67" t="s">
         <v>203</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="J67" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="30">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29">
       <c r="A68" t="s">
         <v>203</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>373</v>
+        <v>609</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>372</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="1"/>
       <c r="J68" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="29">
       <c r="A69" t="s">
         <v>203</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>374</v>
+        <v>612</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>373</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="1"/>
       <c r="J69" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>203</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="1"/>
       <c r="J70" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="H71" s="4"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="5" t="s">
         <v>324</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M70" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M70">
-      <sortCondition ref="A1:A70"/>
+  <autoFilter ref="A1:M71" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M71">
+      <sortCondition ref="A1:A71"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated stat labels to be capitalized
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B6283-E8C8-40FA-BE5E-8F47F16F2646}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE14435C-2768-49D3-89C0-8822CC581068}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="619">
   <si>
     <t>context</t>
   </si>
@@ -332,54 +332,24 @@
     <t>Estatisticas apresentadas</t>
   </si>
   <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>media</t>
-  </si>
-  <si>
     <t>Mittelwert</t>
   </si>
   <si>
-    <t>moyenne</t>
-  </si>
-  <si>
     <t>Média</t>
   </si>
   <si>
-    <t>median</t>
-  </si>
-  <si>
-    <t>mediana</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
-    <t>médiane</t>
-  </si>
-  <si>
     <t>Mediana</t>
   </si>
   <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>mínimo</t>
-  </si>
-  <si>
     <t>Minimum</t>
   </si>
   <si>
     <t>Mínimo</t>
   </si>
   <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>máximo</t>
-  </si>
-  <si>
     <t>Maximum</t>
   </si>
   <si>
@@ -464,9 +434,6 @@
     <t>Número de dados faltantes</t>
   </si>
   <si>
-    <t>no. obs.</t>
-  </si>
-  <si>
     <t>Anz. Beob.</t>
   </si>
   <si>
@@ -788,16 +755,7 @@
     <t>Karakteristika</t>
   </si>
   <si>
-    <t>kvartilavstånd</t>
-  </si>
-  <si>
-    <t>medelvärde</t>
-  </si>
-  <si>
     <t>N bortfall</t>
-  </si>
-  <si>
-    <t>antal obs</t>
   </si>
   <si>
     <t>Statistikor presenterade</t>
@@ -2010,7 +1968,34 @@
     <t>提示された統計</t>
   </si>
   <si>
-    <t>range</t>
+    <t>No. obs.</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Kvartilavstånd</t>
+  </si>
+  <si>
+    <t>Medelvärde</t>
+  </si>
+  <si>
+    <t>Antal obs</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Médiane</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
   </si>
 </sst>
 </file>
@@ -2458,25 +2443,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="51.81640625" customWidth="1"/>
-    <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.26953125" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="49" style="22" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2487,25 +2475,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -2522,41 +2510,41 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="K2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="M2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2567,25 +2555,25 @@
         <v>17</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -2608,25 +2596,25 @@
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -2649,22 +2637,22 @@
         <v>42</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>42</v>
@@ -2690,25 +2678,25 @@
         <v>37</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="J6" t="s">
         <v>38</v>
@@ -2731,25 +2719,25 @@
         <v>32</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="J7" t="s">
         <v>33</v>
@@ -2772,25 +2760,25 @@
         <v>47</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="J8" t="s">
         <v>48</v>
@@ -2813,25 +2801,25 @@
         <v>27</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="J9" t="s">
         <v>28</v>
@@ -2854,25 +2842,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
@@ -2895,22 +2883,22 @@
         <v>52</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>52</v>
@@ -2936,25 +2924,25 @@
         <v>12</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
@@ -2971,398 +2959,398 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="L13" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="J14" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="K14" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="L14" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="M14" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="J15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L15" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="M15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="J16" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="K16" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="L16" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K17" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L17" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="M17" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="J18" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="K18" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="L18" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="M18" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
         <v>143</v>
       </c>
-      <c r="B19" t="s">
-        <v>154</v>
-      </c>
       <c r="C19" s="22" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="J19" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="L19" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="M19" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="K20" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="L20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="M20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="J21" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="K21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="L21" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="M21" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="4" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3373,25 +3361,25 @@
         <v>75</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="J23" t="s">
         <v>76</v>
@@ -3414,25 +3402,25 @@
         <v>58</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="J24" t="s">
         <v>59</v>
@@ -3452,23 +3440,23 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="4" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -3479,25 +3467,25 @@
         <v>71</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="J26" t="s">
         <v>72</v>
@@ -3517,23 +3505,23 @@
         <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="4" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3544,22 +3532,22 @@
         <v>67</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>67</v>
@@ -3582,21 +3570,21 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="4"/>
       <c r="I29" s="1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3604,21 +3592,21 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="4"/>
       <c r="I30" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -3626,21 +3614,21 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="4"/>
       <c r="I31" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -3648,21 +3636,21 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="4"/>
       <c r="I32" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -3670,23 +3658,23 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="4" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -3697,25 +3685,25 @@
         <v>63</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="J34" t="s">
         <v>64</v>
@@ -3735,40 +3723,40 @@
         <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="J35" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="K35" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L35" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="M35" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -3776,27 +3764,27 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="4" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="12" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -3804,40 +3792,40 @@
         <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="K37" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="L37" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="M37" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -3845,27 +3833,27 @@
         <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="4" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="11" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -3876,25 +3864,25 @@
         <v>81</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="J39" t="s">
         <v>82</v>
@@ -3914,40 +3902,40 @@
         <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>248</v>
+        <v>613</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="K40" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="L40" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="M40" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3955,40 +3943,40 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K41" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L41" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="M41" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -3996,40 +3984,40 @@
         <v>80</v>
       </c>
       <c r="B42" t="s">
+        <v>610</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="J42" t="s">
+        <v>616</v>
+      </c>
+      <c r="K42" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>537</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>539</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>404</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="L42" t="s">
+        <v>618</v>
+      </c>
+      <c r="M42" t="s">
         <v>97</v>
-      </c>
-      <c r="K42" t="s">
-        <v>98</v>
-      </c>
-      <c r="L42" t="s">
-        <v>99</v>
-      </c>
-      <c r="M42" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -4037,40 +4025,40 @@
         <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L43" t="s">
-        <v>104</v>
+        <v>617</v>
       </c>
       <c r="M43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -4078,40 +4066,40 @@
         <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J44" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K44" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -4119,22 +4107,22 @@
         <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1"/>
       <c r="J45" s="9" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -4142,35 +4130,35 @@
         <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J46" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="K46" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L46" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M46" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -4178,35 +4166,35 @@
         <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="J47" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="K47" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L47" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M47" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -4214,22 +4202,22 @@
         <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="4"/>
       <c r="I48" s="1"/>
       <c r="J48" s="8" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="2" customFormat="1">
@@ -4237,22 +4225,22 @@
         <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="12"/>
       <c r="H49" s="4"/>
       <c r="J49" s="7" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="2" customFormat="1">
@@ -4260,22 +4248,22 @@
         <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="12"/>
       <c r="H50" s="4"/>
       <c r="J50" s="7" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="2" customFormat="1">
@@ -4283,36 +4271,36 @@
         <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="12" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="2" t="s">
-        <v>251</v>
+        <v>615</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>140</v>
+        <v>609</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:13" s="12" customFormat="1">
@@ -4320,7 +4308,7 @@
         <v>80</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
@@ -4332,40 +4320,40 @@
         <v>80</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1">
@@ -4376,25 +4364,25 @@
         <v>91</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>92</v>
@@ -4414,22 +4402,22 @@
         <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="12"/>
       <c r="H55" s="4"/>
       <c r="J55" s="6" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="2" customFormat="1">
@@ -4437,22 +4425,22 @@
         <v>80</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="12"/>
       <c r="H56" s="4"/>
       <c r="J56" s="6" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="2" customFormat="1">
@@ -4463,25 +4451,25 @@
         <v>86</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>87</v>
@@ -4501,428 +4489,428 @@
         <v>80</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>118</v>
+        <v>612</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="J59" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K59" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="L59" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="M59" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="J60" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="K60" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="L60" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="M60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="29">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="30">
       <c r="A61" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="J61" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="30">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
       <c r="J62" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="29">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="30">
       <c r="A63" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="29">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="30">
       <c r="A64" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B64" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="J64" s="5" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" t="s">
         <v>203</v>
       </c>
-      <c r="B65" t="s">
-        <v>214</v>
-      </c>
       <c r="C65" s="22" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1"/>
       <c r="J65" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="29">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="45">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="1"/>
       <c r="J66" s="5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="29">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="J67" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="29">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="30">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B68" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="1"/>
       <c r="J68" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="29">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30">
       <c r="A69" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B69" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="1"/>
       <c r="J69" s="5" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="1"/>
       <c r="J70" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="30">
       <c r="A71" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="1"/>
       <c r="J71" s="5" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding range to translations
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE14435C-2768-49D3-89C0-8822CC581068}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656F1BB1-C5C5-49DC-A946-6246AB12657B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="626">
   <si>
     <t>context</t>
   </si>
@@ -1996,6 +1996,27 @@
   </si>
   <si>
     <t>Moyenne</t>
+  </si>
+  <si>
+    <t>值域</t>
+  </si>
+  <si>
+    <t>範圍</t>
+  </si>
+  <si>
+    <t>Spannweite</t>
+  </si>
+  <si>
+    <t>レンジ</t>
+  </si>
+  <si>
+    <t>Variationsbredd</t>
+  </si>
+  <si>
+    <t>Étendue</t>
+  </si>
+  <si>
+    <t>Rango</t>
   </si>
 </sst>
 </file>
@@ -2444,10 +2465,10 @@
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
+      <selection pane="bottomRight" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4313,7 +4334,27 @@
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
-      <c r="F52" s="14"/>
+      <c r="F52" s="14" t="s">
+        <v>620</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>625</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="53" spans="1:13" s="2" customFormat="1">
       <c r="A53" s="2" t="s">

</xml_diff>

<commit_message>
Adding continuous2 summary type (#631)
* Update utils-tbl_summary.R

* Update utils-tbl_summary.R

* in progress

* in progress

* Update utils-tbl_summary.R

* Update tbl_summary.R

* in progress

* updates

* in progress

* in progress

* added tests

* Update test-add_stat_label.R

* adding tests

* bug fix for stat column location

* added range to translation excel file

* in progress

* updating figures

* updated stat labels to be capitalized

* adding range to translations

* translation updates

* updated translation

* doc updates

* documentation update

* Update utils-tbl_summary.R

* Update utils-tbl_summary.R

* documentation updates

* update NEWS

* Increment version number

* codemeta

* Update NEWS.md

Co-authored-by: whitingk <whitingk@mskcc.org>
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52730DF3-65D6-47CC-9E48-9011099271DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F717CE-B56E-46E2-B0BA-620A6C071791}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="626">
   <si>
     <t>context</t>
   </si>
@@ -332,54 +332,24 @@
     <t>Estatisticas apresentadas</t>
   </si>
   <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>media</t>
-  </si>
-  <si>
     <t>Mittelwert</t>
   </si>
   <si>
-    <t>moyenne</t>
-  </si>
-  <si>
     <t>Média</t>
   </si>
   <si>
-    <t>median</t>
-  </si>
-  <si>
-    <t>mediana</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
-    <t>médiane</t>
-  </si>
-  <si>
     <t>Mediana</t>
   </si>
   <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>mínimo</t>
-  </si>
-  <si>
     <t>Minimum</t>
   </si>
   <si>
     <t>Mínimo</t>
   </si>
   <si>
-    <t>maximum</t>
-  </si>
-  <si>
-    <t>máximo</t>
-  </si>
-  <si>
     <t>Maximum</t>
   </si>
   <si>
@@ -413,9 +383,6 @@
     <t>IQR</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>EI</t>
   </si>
   <si>
@@ -464,9 +431,6 @@
     <t>Número de dados faltantes</t>
   </si>
   <si>
-    <t>no. obs.</t>
-  </si>
-  <si>
     <t>Anz. Beob.</t>
   </si>
   <si>
@@ -788,16 +752,7 @@
     <t>Karakteristika</t>
   </si>
   <si>
-    <t>kvartilavstånd</t>
-  </si>
-  <si>
-    <t>medelvärde</t>
-  </si>
-  <si>
     <t>N bortfall</t>
-  </si>
-  <si>
-    <t>antal obs</t>
   </si>
   <si>
     <t>Statistikor presenterade</t>
@@ -2008,6 +1963,60 @@
   </si>
   <si>
     <t>提示された統計</t>
+  </si>
+  <si>
+    <t>No. obs.</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Kvartilavstånd</t>
+  </si>
+  <si>
+    <t>Medelvärde</t>
+  </si>
+  <si>
+    <t>Antal obs</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Médiane</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>值域</t>
+  </si>
+  <si>
+    <t>範圍</t>
+  </si>
+  <si>
+    <t>Spannweite</t>
+  </si>
+  <si>
+    <t>レンジ</t>
+  </si>
+  <si>
+    <t>Variationsbredd</t>
+  </si>
+  <si>
+    <t>Étendue</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Intervalo</t>
   </si>
 </sst>
 </file>
@@ -2453,27 +2462,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L33" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="51.81640625" customWidth="1"/>
+    <col min="3" max="3" width="49" style="22" customWidth="1"/>
+    <col min="4" max="4" width="47.26953125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.453125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2484,25 +2496,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>620</v>
+        <v>605</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -2519,41 +2531,41 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="K2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="L2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="M2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2564,25 +2576,25 @@
         <v>17</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -2605,25 +2617,25 @@
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -2646,22 +2658,22 @@
         <v>42</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>42</v>
@@ -2687,25 +2699,25 @@
         <v>37</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="J6" t="s">
         <v>38</v>
@@ -2728,25 +2740,25 @@
         <v>32</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="J7" t="s">
         <v>33</v>
@@ -2769,25 +2781,25 @@
         <v>47</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="J8" t="s">
         <v>48</v>
@@ -2810,25 +2822,25 @@
         <v>27</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="J9" t="s">
         <v>28</v>
@@ -2851,25 +2863,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
@@ -2892,22 +2904,22 @@
         <v>52</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>52</v>
@@ -2933,25 +2945,25 @@
         <v>12</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
@@ -2968,398 +2980,398 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="L13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="M13" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="J14" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="K14" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="L14" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="M14" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="J15" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="L15" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="M15" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="J16" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="K16" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="L16" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="M16" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="K17" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="L17" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="M17" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="J18" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="K18" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="L18" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="M18" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J19" t="s">
         <v>143</v>
       </c>
-      <c r="B19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>473</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>474</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>475</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="J19" t="s">
-        <v>155</v>
-      </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="L19" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="M19" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="J20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K20" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="L20" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="M20" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="J21" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="K21" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="L21" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="M21" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.5">
       <c r="A22" t="s">
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3370,25 +3382,25 @@
         <v>75</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J23" t="s">
         <v>76</v>
@@ -3411,25 +3423,25 @@
         <v>58</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="J24" t="s">
         <v>59</v>
@@ -3449,23 +3461,23 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="4" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -3476,25 +3488,25 @@
         <v>71</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="J26" t="s">
         <v>72</v>
@@ -3514,23 +3526,23 @@
         <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="4" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3541,22 +3553,22 @@
         <v>67</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>67</v>
@@ -3579,21 +3591,21 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="4"/>
       <c r="I29" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3601,21 +3613,21 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="4"/>
       <c r="I30" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -3623,21 +3635,21 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="4"/>
       <c r="I31" s="1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -3645,21 +3657,21 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="4"/>
       <c r="I32" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -3667,23 +3679,23 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="4" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -3694,25 +3706,25 @@
         <v>63</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J34" t="s">
         <v>64</v>
@@ -3732,40 +3744,40 @@
         <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="J35" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="K35" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="L35" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="M35" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -3773,27 +3785,27 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="4" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="12" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -3801,40 +3813,40 @@
         <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="K37" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="L37" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="M37" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -3842,27 +3854,27 @@
         <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="4" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="11" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -3873,25 +3885,25 @@
         <v>81</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="J39" t="s">
         <v>82</v>
@@ -3911,40 +3923,40 @@
         <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>248</v>
+        <v>612</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="K40" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="L40" t="s">
-        <v>124</v>
-      </c>
-      <c r="M40" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="M40" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3952,40 +3964,40 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K41" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L41" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="M41" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -3993,40 +4005,40 @@
         <v>80</v>
       </c>
       <c r="B42" t="s">
+        <v>609</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="J42" t="s">
+        <v>615</v>
+      </c>
+      <c r="K42" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>537</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>539</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>404</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="L42" t="s">
+        <v>617</v>
+      </c>
+      <c r="M42" t="s">
         <v>97</v>
-      </c>
-      <c r="K42" t="s">
-        <v>98</v>
-      </c>
-      <c r="L42" t="s">
-        <v>99</v>
-      </c>
-      <c r="M42" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -4034,40 +4046,40 @@
         <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L43" t="s">
-        <v>104</v>
+        <v>616</v>
       </c>
       <c r="M43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -4075,40 +4087,40 @@
         <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J44" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K44" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -4116,22 +4128,22 @@
         <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1"/>
       <c r="J45" s="9" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -4139,35 +4151,35 @@
         <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="J46" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="K46" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="L46" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="M46" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -4175,35 +4187,35 @@
         <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="J47" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="K47" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="L47" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="M47" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -4211,22 +4223,22 @@
         <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="4"/>
       <c r="I48" s="1"/>
       <c r="J48" s="8" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="2" customFormat="1">
@@ -4234,22 +4246,22 @@
         <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="12"/>
       <c r="H49" s="4"/>
       <c r="J49" s="7" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="2" customFormat="1">
@@ -4257,22 +4269,22 @@
         <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="12"/>
       <c r="H50" s="4"/>
       <c r="J50" s="7" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="2" customFormat="1">
@@ -4280,77 +4292,71 @@
         <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>140</v>
+        <v>608</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>561</v>
+        <v>546</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="12" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="2" t="s">
-        <v>251</v>
+        <v>614</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>140</v>
+        <v>608</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>140</v>
+        <v>608</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="2" customFormat="1">
-      <c r="A52" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="12" customFormat="1">
+      <c r="A52" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>406</v>
+      <c r="B52" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="14" t="s">
+        <v>619</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>117</v>
+        <v>618</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>624</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="2" customFormat="1">
@@ -4358,40 +4364,40 @@
         <v>80</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>407</v>
+        <v>550</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>391</v>
       </c>
       <c r="G53" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="H53" s="22" t="s">
-        <v>622</v>
+      <c r="H53" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>252</v>
+        <v>104</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1">
@@ -4399,22 +4405,40 @@
         <v>80</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>274</v>
+        <v>91</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="4"/>
-      <c r="J54" s="6" t="s">
-        <v>312</v>
+        <v>553</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="2" customFormat="1">
@@ -4422,22 +4446,22 @@
         <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>574</v>
+        <v>554</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>556</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="12"/>
       <c r="H55" s="4"/>
       <c r="J55" s="6" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="2" customFormat="1">
@@ -4445,40 +4469,22 @@
         <v>80</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>86</v>
+        <v>263</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>90</v>
+        <v>557</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="F56" s="14"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="4"/>
+      <c r="J56" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="2" customFormat="1">
@@ -4486,434 +4492,475 @@
         <v>80</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>578</v>
+        <v>560</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>409</v>
+        <v>561</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>393</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" t="s">
-        <v>195</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="2" customFormat="1">
+      <c r="A58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>611</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>580</v>
+        <v>562</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>581</v>
+        <v>563</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>582</v>
+        <v>564</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="J58" t="s">
-        <v>196</v>
-      </c>
-      <c r="K58" t="s">
-        <v>197</v>
-      </c>
-      <c r="L58" t="s">
-        <v>195</v>
-      </c>
-      <c r="M58" t="s">
-        <v>196</v>
+        <v>257</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>584</v>
+        <v>566</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>303</v>
+        <v>567</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>395</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>255</v>
+        <v>184</v>
       </c>
       <c r="J59" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K59" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="L59" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="M59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="30">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="F60" s="21" t="s">
-        <v>411</v>
+        <v>570</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>288</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="30">
+        <v>350</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J60" t="s">
+        <v>187</v>
+      </c>
+      <c r="K60" t="s">
+        <v>188</v>
+      </c>
+      <c r="L60" t="s">
+        <v>189</v>
+      </c>
+      <c r="M60" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="29">
       <c r="A61" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>412</v>
+        <v>573</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>396</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1"/>
       <c r="J61" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="30">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="29">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="G62" s="12"/>
+        <v>397</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>352</v>
+      </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
       <c r="J62" s="5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="29">
       <c r="A63" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>368</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="29">
       <c r="A64" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>600</v>
+        <v>581</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>582</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="J64" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="45">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>603</v>
+        <v>584</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>585</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1"/>
       <c r="J65" s="5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="30">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="29">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="1"/>
       <c r="J66" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="30">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="29">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="J67" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>373</v>
+        <v>594</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="1"/>
       <c r="J68" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="29">
       <c r="A69" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>374</v>
+        <v>597</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>358</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="1"/>
       <c r="J69" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>618</v>
+        <v>600</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="1"/>
       <c r="J70" s="5" t="s">
-        <v>324</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="H71" s="4"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="5" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M70" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M70">
-      <sortCondition ref="A1:A70"/>
+  <autoFilter ref="A1:M71" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M71">
+      <sortCondition ref="A1:A71"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added SE to translation
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F717CE-B56E-46E2-B0BA-620A6C071791}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C52D559-5F2E-45B4-844E-C03D59F2E6B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="627">
   <si>
     <t>context</t>
   </si>
@@ -2017,6 +2017,9 @@
   </si>
   <si>
     <t>Intervalo</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
@@ -2462,30 +2465,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M55" sqref="M55"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="51.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="49" style="22" customWidth="1"/>
-    <col min="4" max="4" width="47.26953125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3347,7 +3350,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.5">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3739,73 +3742,57 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="J35" t="s">
-        <v>115</v>
-      </c>
-      <c r="K35" t="s">
-        <v>116</v>
-      </c>
-      <c r="L35" t="s">
-        <v>117</v>
-      </c>
-      <c r="M35" t="s">
-        <v>118</v>
-      </c>
+    <row r="35" spans="1:13" s="12" customFormat="1">
+      <c r="A35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>114</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>507</v>
+        <v>503</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>504</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="G36" s="12"/>
+        <v>384</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>336</v>
+      </c>
       <c r="H36" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="12" t="s">
-        <v>291</v>
+        <v>283</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J36" t="s">
+        <v>115</v>
+      </c>
+      <c r="K36" t="s">
+        <v>116</v>
+      </c>
+      <c r="L36" t="s">
+        <v>117</v>
+      </c>
+      <c r="M36" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -3813,40 +3800,27 @@
         <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>266</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>337</v>
-      </c>
+        <v>506</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J37" t="s">
-        <v>120</v>
-      </c>
-      <c r="K37" t="s">
-        <v>121</v>
-      </c>
-      <c r="L37" t="s">
-        <v>122</v>
-      </c>
-      <c r="M37" t="s">
-        <v>123</v>
+        <v>284</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -3854,27 +3828,40 @@
         <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>119</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>512</v>
+        <v>508</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>509</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="G38" s="12"/>
+        <v>386</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>337</v>
+      </c>
       <c r="H38" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="11" t="s">
-        <v>292</v>
+        <v>285</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J38" t="s">
+        <v>120</v>
+      </c>
+      <c r="K38" t="s">
+        <v>121</v>
+      </c>
+      <c r="L38" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -3882,40 +3869,27 @@
         <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>267</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>338</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="G39" s="12"/>
       <c r="H39" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J39" t="s">
-        <v>82</v>
-      </c>
-      <c r="K39" t="s">
-        <v>83</v>
-      </c>
-      <c r="L39" t="s">
-        <v>84</v>
-      </c>
-      <c r="M39" t="s">
-        <v>85</v>
+        <v>286</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="11" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -3923,40 +3897,40 @@
         <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>518</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>339</v>
+        <v>515</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>388</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>293</v>
+        <v>235</v>
+      </c>
+      <c r="J40" t="s">
+        <v>82</v>
       </c>
       <c r="K40" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="L40" t="s">
-        <v>113</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>112</v>
+        <v>84</v>
+      </c>
+      <c r="M40" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3964,40 +3938,40 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>252</v>
+        <v>518</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>339</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J41" t="s">
-        <v>103</v>
+        <v>612</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>293</v>
       </c>
       <c r="K41" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="L41" t="s">
-        <v>102</v>
-      </c>
-      <c r="M41" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -4005,40 +3979,40 @@
         <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>609</v>
+        <v>102</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>524</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>389</v>
+        <v>520</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>252</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>613</v>
+        <v>102</v>
       </c>
       <c r="J42" t="s">
-        <v>615</v>
+        <v>103</v>
       </c>
       <c r="K42" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="L42" t="s">
-        <v>617</v>
+        <v>102</v>
       </c>
       <c r="M42" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -4046,40 +4020,40 @@
         <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>609</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>98</v>
+        <v>613</v>
       </c>
       <c r="J43" t="s">
-        <v>99</v>
+        <v>615</v>
       </c>
       <c r="K43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L43" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="M43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -4087,40 +4061,40 @@
         <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>255</v>
+        <v>526</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>390</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L44" t="s">
-        <v>100</v>
+        <v>616</v>
       </c>
       <c r="M44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -4128,22 +4102,40 @@
         <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>100</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="9" t="s">
-        <v>262</v>
+        <v>530</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J45" t="s">
+        <v>101</v>
+      </c>
+      <c r="K45" t="s">
+        <v>100</v>
+      </c>
+      <c r="L45" t="s">
+        <v>100</v>
+      </c>
+      <c r="M45" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -4151,35 +4143,22 @@
         <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>262</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>535</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>344</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="G46" s="12"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J46" t="s">
-        <v>125</v>
-      </c>
-      <c r="K46" t="s">
-        <v>126</v>
-      </c>
-      <c r="L46" t="s">
-        <v>127</v>
-      </c>
-      <c r="M46" t="s">
-        <v>128</v>
+      <c r="I46" s="1"/>
+      <c r="J46" s="9" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -4187,7 +4166,7 @@
         <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>533</v>
@@ -4223,45 +4202,58 @@
         <v>80</v>
       </c>
       <c r="B48" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J48" t="s">
+        <v>125</v>
+      </c>
+      <c r="K48" t="s">
+        <v>126</v>
+      </c>
+      <c r="L48" t="s">
+        <v>127</v>
+      </c>
+      <c r="M48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s">
         <v>264</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C49" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D49" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E49" s="24" t="s">
         <v>538</v>
       </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="2" customFormat="1">
-      <c r="A49" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="F49" s="14"/>
       <c r="G49" s="12"/>
       <c r="H49" s="4"/>
-      <c r="J49" s="7" t="s">
-        <v>295</v>
+      <c r="I49" s="1"/>
+      <c r="J49" s="8" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="2" customFormat="1">
@@ -4269,22 +4261,22 @@
         <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>544</v>
+        <v>540</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>541</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="12"/>
       <c r="H50" s="4"/>
       <c r="J50" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="2" customFormat="1">
@@ -4292,112 +4284,94 @@
         <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="4"/>
+      <c r="J51" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="2" customFormat="1">
+      <c r="A52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C52" s="22" t="s">
         <v>545</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D52" s="22" t="s">
         <v>546</v>
       </c>
-      <c r="E51" s="22" t="s">
+      <c r="E52" s="22" t="s">
         <v>547</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="12" t="s">
+      <c r="F52" s="14"/>
+      <c r="G52" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="2" t="s">
+      <c r="H52" s="4"/>
+      <c r="I52" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="M52" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="12" customFormat="1">
-      <c r="A52" s="12" t="s">
+    <row r="53" spans="1:13" s="12" customFormat="1">
+      <c r="A53" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="14" t="s">
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="14" t="s">
         <v>619</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H53" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="I52" s="12" t="s">
+      <c r="I53" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="J52" s="12" t="s">
+      <c r="J53" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="K52" s="12" t="s">
+      <c r="K53" s="12" t="s">
         <v>620</v>
       </c>
-      <c r="L52" s="12" t="s">
+      <c r="L53" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="M52" s="12" t="s">
+      <c r="M53" s="12" t="s">
         <v>625</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="2" customFormat="1">
-      <c r="A53" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>391</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1">
@@ -4405,40 +4379,40 @@
         <v>80</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>392</v>
+        <v>550</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>391</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>607</v>
+        <v>361</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>237</v>
+        <v>104</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="2" customFormat="1">
@@ -4446,22 +4420,40 @@
         <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>259</v>
+        <v>91</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="4"/>
-      <c r="J55" s="6" t="s">
-        <v>297</v>
+        <v>553</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="2" customFormat="1">
@@ -4469,22 +4461,22 @@
         <v>80</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>559</v>
+        <v>554</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>556</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="12"/>
       <c r="H56" s="4"/>
       <c r="J56" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="2" customFormat="1">
@@ -4492,40 +4484,22 @@
         <v>80</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>86</v>
+        <v>263</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>90</v>
+        <v>557</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="4"/>
+      <c r="J57" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="1:13" s="2" customFormat="1">
@@ -4533,81 +4507,81 @@
         <v>80</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="2" customFormat="1">
+      <c r="A59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C59" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D59" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="E58" s="22" t="s">
+      <c r="E59" s="22" t="s">
         <v>564</v>
       </c>
-      <c r="F58" s="20" t="s">
+      <c r="F59" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="G58" s="12" t="s">
+      <c r="G59" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="J59" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="K59" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L58" s="2" t="s">
+      <c r="L59" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="M59" s="2" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59" t="s">
-        <v>182</v>
-      </c>
-      <c r="B59" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>395</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J59" t="s">
-        <v>184</v>
-      </c>
-      <c r="K59" t="s">
-        <v>185</v>
-      </c>
-      <c r="L59" t="s">
-        <v>183</v>
-      </c>
-      <c r="M59" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -4615,318 +4589,331 @@
         <v>182</v>
       </c>
       <c r="B60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>567</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J60" t="s">
+        <v>184</v>
+      </c>
+      <c r="K60" t="s">
+        <v>185</v>
+      </c>
+      <c r="L60" t="s">
+        <v>183</v>
+      </c>
+      <c r="M60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C61" s="22" t="s">
         <v>568</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D61" s="22" t="s">
         <v>569</v>
       </c>
-      <c r="E60" s="22" t="s">
+      <c r="E61" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F61" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G61" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="I61" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J61" t="s">
         <v>187</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K61" t="s">
         <v>188</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L61" t="s">
         <v>189</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M61" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="29">
-      <c r="A61" t="s">
-        <v>191</v>
-      </c>
-      <c r="B61" t="s">
-        <v>195</v>
-      </c>
-      <c r="C61" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="29">
+    <row r="62" spans="1:13" ht="30">
       <c r="A62" t="s">
         <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>397</v>
+        <v>573</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>396</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
       <c r="J62" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="29">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="30">
       <c r="A63" t="s">
         <v>191</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="G63" s="12"/>
+        <v>397</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>352</v>
+      </c>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="30">
       <c r="A64" t="s">
         <v>191</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>353</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="G64" s="12"/>
       <c r="H64" s="4"/>
       <c r="I64" s="1"/>
       <c r="J64" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30">
       <c r="A65" t="s">
         <v>191</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>585</v>
+        <v>581</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>582</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1"/>
       <c r="J65" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="29">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>191</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>588</v>
+        <v>584</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>585</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="1"/>
       <c r="J66" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="29">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="45">
       <c r="A67" t="s">
         <v>191</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="1"/>
       <c r="J67" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="29">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="30">
       <c r="A68" t="s">
         <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="1"/>
       <c r="J68" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="29">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30">
       <c r="A69" t="s">
         <v>191</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>404</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>358</v>
+        <v>594</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="1"/>
       <c r="J69" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30">
       <c r="A70" t="s">
         <v>191</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>600</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>359</v>
+        <v>597</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>358</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="1"/>
       <c r="J70" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4934,33 +4921,61 @@
         <v>191</v>
       </c>
       <c r="B71" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="1"/>
       <c r="J71" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="30">
+      <c r="A72" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" t="s">
+        <v>199</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="H72" s="4"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="5" t="s">
         <v>309</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M71" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M71">
-      <sortCondition ref="A1:A71"/>
+  <autoFilter ref="A1:M72" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M72">
+      <sortCondition ref="A1:A72"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update gtsummary_translated file to incorporate add_glance labels
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laveryj\Desktop\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F717CE-B56E-46E2-B0BA-620A6C071791}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ACF4FA-70DC-4EBF-993C-F40130CDD68A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="636">
   <si>
     <t>context</t>
   </si>
@@ -2017,6 +2017,36 @@
   </si>
   <si>
     <t>Intervalo</t>
+  </si>
+  <si>
+    <t>add_glance_source_note</t>
+  </si>
+  <si>
+    <t>log-likelihood</t>
+  </si>
+  <si>
+    <t>Residual df</t>
+  </si>
+  <si>
+    <t>Null deviance</t>
+  </si>
+  <si>
+    <t>Null df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	N events</t>
+  </si>
+  <si>
+    <t>c-index</t>
+  </si>
+  <si>
+    <t>c-index SE</t>
+  </si>
+  <si>
+    <t>R\U00B2</t>
+  </si>
+  <si>
+    <t>Adjusted R\U00B2</t>
   </si>
 </sst>
 </file>
@@ -2462,30 +2492,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M55" sqref="M55"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="51.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="49" style="22" customWidth="1"/>
-    <col min="4" max="4" width="47.26953125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2531,1147 +2561,908 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>626</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>408</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K2" t="s">
-        <v>180</v>
-      </c>
-      <c r="L2" t="s">
-        <v>181</v>
-      </c>
-      <c r="M2" t="s">
-        <v>181</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>413</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="A4" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s">
-        <v>46</v>
+        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>421</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
-        <v>36</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>426</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>427</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>367</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" t="s">
-        <v>51</v>
+        <v>629</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>6</v>
+      <c r="A9" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>428</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>429</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>430</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" t="s">
-        <v>31</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>6</v>
+      <c r="A10" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>431</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" t="s">
-        <v>11</v>
+        <v>631</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>6</v>
+      <c r="A11" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>434</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>369</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" t="s">
-        <v>56</v>
+        <v>632</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>6</v>
+      <c r="A12" s="12" t="s">
+        <v>626</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" t="s">
-        <v>16</v>
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>440</v>
+        <v>408</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>441</v>
+        <v>409</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>442</v>
+        <v>410</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>371</v>
+        <v>311</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>220</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="K13" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="L13" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="M13" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>443</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>444</v>
+        <v>411</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>412</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>372</v>
+        <v>413</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>362</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J14" t="s">
-        <v>158</v>
+        <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>159</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="M14" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>446</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>447</v>
+        <v>414</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>415</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>448</v>
+        <v>416</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="J15" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="L15" t="s">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="M15" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>450</v>
+        <v>417</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>418</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>451</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>374</v>
+        <v>419</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>364</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>164</v>
+        <v>44</v>
       </c>
       <c r="L16" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="M16" t="s">
-        <v>166</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>453</v>
+        <v>420</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>420</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>375</v>
+        <v>421</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>365</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J17" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="K17" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="M17" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>455</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>456</v>
+        <v>422</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>423</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>376</v>
+        <v>424</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>366</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="J18" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
       <c r="M18" t="s">
-        <v>136</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>459</v>
+        <v>425</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>426</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>377</v>
+        <v>427</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>367</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J19" t="s">
-        <v>143</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s">
-        <v>144</v>
+        <v>49</v>
       </c>
       <c r="L19" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="M19" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>27</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>462</v>
+        <v>428</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>429</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>463</v>
+        <v>430</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>378</v>
+        <v>272</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="J20" t="s">
-        <v>168</v>
+        <v>28</v>
       </c>
       <c r="K20" t="s">
-        <v>169</v>
+        <v>29</v>
       </c>
       <c r="L20" t="s">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="M20" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>464</v>
+        <v>431</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>465</v>
+        <v>432</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>282</v>
+        <v>433</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>368</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="J21" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="L21" t="s">
-        <v>175</v>
+        <v>10</v>
       </c>
       <c r="M21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>52</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>467</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>467</v>
+        <v>434</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>435</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="G22" s="12"/>
+        <v>369</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>320</v>
+      </c>
       <c r="H22" s="4" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>209</v>
+        <v>52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>469</v>
+        <v>437</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>470</v>
+        <v>438</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>379</v>
+        <v>439</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>247</v>
+        <v>290</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="J23" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="M23" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>472</v>
+        <v>440</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>473</v>
+        <v>441</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>474</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>380</v>
+        <v>442</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>371</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="J24" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
       <c r="K24" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="L24" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="M24" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>475</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>475</v>
+        <v>443</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>476</v>
-      </c>
-      <c r="G25" s="12"/>
+        <v>445</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>323</v>
+      </c>
       <c r="H25" s="4" t="s">
-        <v>205</v>
+        <v>275</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>205</v>
+        <v>221</v>
+      </c>
+      <c r="J25" t="s">
+        <v>158</v>
+      </c>
+      <c r="K25" t="s">
+        <v>159</v>
+      </c>
+      <c r="L25" t="s">
+        <v>160</v>
+      </c>
+      <c r="M25" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>477</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>478</v>
+        <v>446</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>447</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>381</v>
+        <v>448</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>373</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="J26" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="K26" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="L26" t="s">
-        <v>73</v>
+        <v>150</v>
       </c>
       <c r="M26" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>481</v>
+        <v>449</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>450</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>482</v>
-      </c>
-      <c r="G27" s="12"/>
+        <v>451</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>325</v>
+      </c>
       <c r="H27" s="4" t="s">
-        <v>207</v>
+        <v>277</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
+      </c>
+      <c r="J27" t="s">
+        <v>163</v>
+      </c>
+      <c r="K27" t="s">
+        <v>164</v>
+      </c>
+      <c r="L27" t="s">
+        <v>165</v>
+      </c>
+      <c r="M27" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>483</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>484</v>
+        <v>452</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>453</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>382</v>
+        <v>454</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>249</v>
+        <v>278</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="K28" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="L28" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="M28" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>132</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>487</v>
+        <v>455</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>488</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="4"/>
+        <v>457</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="I29" s="1" t="s">
-        <v>210</v>
+        <v>225</v>
+      </c>
+      <c r="J29" t="s">
+        <v>133</v>
+      </c>
+      <c r="K29" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>489</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>490</v>
+        <v>458</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="4"/>
+        <v>460</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>280</v>
+      </c>
       <c r="I30" s="1" t="s">
-        <v>206</v>
+        <v>226</v>
+      </c>
+      <c r="J30" t="s">
+        <v>143</v>
+      </c>
+      <c r="K30" t="s">
+        <v>144</v>
+      </c>
+      <c r="L30" t="s">
+        <v>145</v>
+      </c>
+      <c r="M30" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>493</v>
+        <v>461</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="4"/>
+        <v>463</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>281</v>
+      </c>
       <c r="I31" s="1" t="s">
-        <v>208</v>
+        <v>227</v>
+      </c>
+      <c r="J31" t="s">
+        <v>168</v>
+      </c>
+      <c r="K31" t="s">
+        <v>169</v>
+      </c>
+      <c r="L31" t="s">
+        <v>170</v>
+      </c>
+      <c r="M31" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>495</v>
+        <v>464</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>497</v>
-      </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="4"/>
+        <v>466</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>282</v>
+      </c>
       <c r="I32" s="1" t="s">
-        <v>204</v>
+        <v>228</v>
+      </c>
+      <c r="J32" t="s">
+        <v>173</v>
+      </c>
+      <c r="K32" t="s">
+        <v>174</v>
+      </c>
+      <c r="L32" t="s">
+        <v>175</v>
+      </c>
+      <c r="M32" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -3679,23 +3470,26 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>498</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>498</v>
+        <v>467</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>467</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>499</v>
+        <v>468</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>209</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="4" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -3703,447 +3497,364 @@
         <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>501</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>502</v>
+        <v>469</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>471</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J34" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="K34" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="L34" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="M34" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>503</v>
+        <v>472</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>384</v>
+        <v>474</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>380</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J35" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="K35" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="L35" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="M35" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>205</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>507</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>385</v>
+        <v>475</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>476</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="12" t="s">
-        <v>291</v>
+        <v>205</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>508</v>
+        <v>477</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>386</v>
+        <v>479</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>381</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>285</v>
+        <v>248</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J37" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="K37" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="L37" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="M37" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>512</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>387</v>
+        <v>481</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>482</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="11" t="s">
-        <v>292</v>
+        <v>207</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>388</v>
+        <v>485</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>382</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>235</v>
+        <v>67</v>
       </c>
       <c r="J39" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="K39" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="L39" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="M39" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>516</v>
+        <v>486</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>517</v>
+        <v>487</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>518</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>251</v>
-      </c>
+        <v>488</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="K40" t="s">
-        <v>112</v>
-      </c>
-      <c r="L40" t="s">
-        <v>113</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>519</v>
+        <v>489</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>252</v>
-      </c>
+        <v>491</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J41" t="s">
-        <v>103</v>
-      </c>
-      <c r="K41" t="s">
-        <v>102</v>
-      </c>
-      <c r="L41" t="s">
-        <v>102</v>
-      </c>
-      <c r="M41" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>609</v>
+        <v>208</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>522</v>
+        <v>492</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>524</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>253</v>
-      </c>
+        <v>493</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="G42" s="12"/>
+      <c r="H42" s="4"/>
       <c r="I42" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="J42" t="s">
-        <v>615</v>
-      </c>
-      <c r="K42" t="s">
-        <v>96</v>
-      </c>
-      <c r="L42" t="s">
-        <v>617</v>
-      </c>
-      <c r="M42" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>525</v>
+        <v>495</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>527</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>254</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="4"/>
       <c r="I43" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J43" t="s">
-        <v>99</v>
-      </c>
-      <c r="K43" t="s">
-        <v>98</v>
-      </c>
-      <c r="L43" t="s">
-        <v>616</v>
-      </c>
-      <c r="M43" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>203</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>528</v>
+        <v>498</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>529</v>
+        <v>498</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>343</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="G44" s="12"/>
       <c r="H44" s="4" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J44" t="s">
-        <v>101</v>
-      </c>
-      <c r="K44" t="s">
-        <v>100</v>
-      </c>
-      <c r="L44" t="s">
-        <v>100</v>
-      </c>
-      <c r="M44" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>63</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="9" t="s">
-        <v>262</v>
+        <v>500</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>501</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" t="s">
+        <v>63</v>
+      </c>
+      <c r="L45" t="s">
+        <v>65</v>
+      </c>
+      <c r="M45" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -4151,35 +3862,40 @@
         <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>533</v>
+        <v>503</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>534</v>
+        <v>503</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>535</v>
+        <v>504</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>384</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H46" s="4"/>
+        <v>336</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>283</v>
+      </c>
       <c r="I46" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J46" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="K46" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L46" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M46" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -4187,35 +3903,27 @@
         <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>533</v>
+        <v>505</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>534</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>535</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J47" t="s">
-        <v>125</v>
-      </c>
-      <c r="K47" t="s">
-        <v>126</v>
-      </c>
-      <c r="L47" t="s">
-        <v>127</v>
-      </c>
-      <c r="M47" t="s">
-        <v>128</v>
+        <v>506</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -4223,747 +3931,1158 @@
         <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>264</v>
+        <v>119</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>537</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>538</v>
-      </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="2" customFormat="1">
-      <c r="A49" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J48" t="s">
+        <v>120</v>
+      </c>
+      <c r="K48" t="s">
+        <v>121</v>
+      </c>
+      <c r="L48" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>260</v>
+      <c r="B49" t="s">
+        <v>267</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="F49" s="14"/>
+        <v>511</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>387</v>
+      </c>
       <c r="G49" s="12"/>
-      <c r="H49" s="4"/>
-      <c r="J49" s="7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="2" customFormat="1">
-      <c r="A50" s="2" t="s">
+      <c r="H49" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>265</v>
+      <c r="B50" t="s">
+        <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>542</v>
+        <v>513</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>544</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="4"/>
-      <c r="J50" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="2" customFormat="1">
-      <c r="A51" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J50" t="s">
+        <v>82</v>
+      </c>
+      <c r="K50" t="s">
+        <v>83</v>
+      </c>
+      <c r="L50" t="s">
+        <v>84</v>
+      </c>
+      <c r="M50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>608</v>
+      <c r="B51" t="s">
+        <v>112</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>545</v>
+        <v>516</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>546</v>
+        <v>517</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="F51" s="14"/>
+        <v>518</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>339</v>
+      </c>
       <c r="G51" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="12" customFormat="1">
-      <c r="A52" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="K51" t="s">
+        <v>112</v>
+      </c>
+      <c r="L51" t="s">
+        <v>113</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>610</v>
-      </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>521</v>
+      </c>
       <c r="F52" s="14" t="s">
-        <v>619</v>
+        <v>252</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>621</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>622</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>624</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>623</v>
-      </c>
-      <c r="M52" s="12" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="2" customFormat="1">
-      <c r="A53" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J52" t="s">
+        <v>103</v>
+      </c>
+      <c r="K52" t="s">
+        <v>102</v>
+      </c>
+      <c r="L52" t="s">
+        <v>102</v>
+      </c>
+      <c r="M52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>104</v>
+      <c r="B53" t="s">
+        <v>609</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>548</v>
+        <v>522</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>391</v>
+        <v>523</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>389</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="2" customFormat="1">
-      <c r="A54" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="J53" t="s">
+        <v>615</v>
+      </c>
+      <c r="K53" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53" t="s">
+        <v>617</v>
+      </c>
+      <c r="M53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>91</v>
+      <c r="B54" t="s">
+        <v>98</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>551</v>
+        <v>525</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>392</v>
+        <v>526</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>390</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" s="2" customFormat="1">
-      <c r="A55" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J54" t="s">
+        <v>99</v>
+      </c>
+      <c r="K54" t="s">
+        <v>98</v>
+      </c>
+      <c r="L54" t="s">
+        <v>616</v>
+      </c>
+      <c r="M54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>259</v>
+      <c r="B55" t="s">
+        <v>100</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>554</v>
+        <v>528</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="4"/>
-      <c r="J55" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" s="2" customFormat="1">
-      <c r="A56" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J55" t="s">
+        <v>101</v>
+      </c>
+      <c r="K55" t="s">
+        <v>100</v>
+      </c>
+      <c r="L55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>263</v>
+      <c r="B56" t="s">
+        <v>262</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="F56" s="14"/>
+        <v>531</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>532</v>
+      </c>
       <c r="G56" s="12"/>
       <c r="H56" s="4"/>
-      <c r="J56" s="6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="2" customFormat="1">
-      <c r="A57" s="2" t="s">
+      <c r="I56" s="1"/>
+      <c r="J56" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>86</v>
+      <c r="B57" t="s">
+        <v>124</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>560</v>
+        <v>533</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>393</v>
+        <v>535</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" s="2" customFormat="1">
-      <c r="A58" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K57" t="s">
+        <v>126</v>
+      </c>
+      <c r="L57" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>611</v>
+      <c r="B58" t="s">
+        <v>261</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>562</v>
+        <v>533</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>563</v>
+        <v>534</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>394</v>
+        <v>535</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>111</v>
+        <v>344</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J58" t="s">
+        <v>125</v>
+      </c>
+      <c r="K58" t="s">
+        <v>126</v>
+      </c>
+      <c r="L58" t="s">
+        <v>127</v>
+      </c>
+      <c r="M58" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>537</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="G59" s="12"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="2" customFormat="1">
+      <c r="A60" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>541</v>
+      </c>
+      <c r="F60" s="14"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="4"/>
+      <c r="J60" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="2" customFormat="1">
+      <c r="A61" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="F61" s="14"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="4"/>
+      <c r="J61" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="2" customFormat="1">
+      <c r="A62" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="F62" s="14"/>
+      <c r="G62" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="I62" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="12" customFormat="1">
+      <c r="A63" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="J63" s="12" t="s">
+        <v>624</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="L63" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="M63" s="12" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="2" customFormat="1">
+      <c r="A64" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="2" customFormat="1">
+      <c r="A65" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="2" customFormat="1">
+      <c r="A66" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="F66" s="14"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="4"/>
+      <c r="J66" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="2" customFormat="1">
+      <c r="A67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="E67" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="4"/>
+      <c r="J67" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1">
+      <c r="A68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="2" customFormat="1">
+      <c r="A69" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" t="s">
         <v>182</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B70" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C70" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D70" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E70" s="22" t="s">
         <v>567</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F70" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="G59" s="12" t="s">
+      <c r="G70" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H70" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J70" t="s">
         <v>184</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K70" t="s">
         <v>185</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L70" t="s">
         <v>183</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M70" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
-      <c r="A60" t="s">
+    <row r="71" spans="1:13">
+      <c r="A71" t="s">
         <v>182</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B71" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C71" s="22" t="s">
         <v>568</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D71" s="22" t="s">
         <v>569</v>
       </c>
-      <c r="E60" s="22" t="s">
+      <c r="E71" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F71" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G71" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H71" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="I71" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J71" t="s">
         <v>187</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K71" t="s">
         <v>188</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L71" t="s">
         <v>189</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M71" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="29">
-      <c r="A61" t="s">
+    <row r="72" spans="1:13" ht="30">
+      <c r="A72" t="s">
         <v>191</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B72" t="s">
         <v>195</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C72" s="22" t="s">
         <v>571</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D72" s="22" t="s">
         <v>572</v>
       </c>
-      <c r="E61" s="22" t="s">
+      <c r="E72" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="F61" s="21" t="s">
+      <c r="F72" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="G61" s="12" t="s">
+      <c r="G72" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="5" t="s">
+      <c r="H72" s="4"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="5" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="29">
-      <c r="A62" t="s">
+    <row r="73" spans="1:13" ht="30">
+      <c r="A73" t="s">
         <v>191</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B73" t="s">
         <v>193</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C73" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D73" s="22" t="s">
         <v>575</v>
       </c>
-      <c r="E62" s="22" t="s">
+      <c r="E73" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F73" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="G62" s="12" t="s">
+      <c r="G73" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="5" t="s">
+      <c r="H73" s="4"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="5" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="29">
-      <c r="A63" t="s">
+    <row r="74" spans="1:13" ht="30">
+      <c r="A74" t="s">
         <v>191</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B74" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>577</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="E63" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>579</v>
       </c>
-      <c r="F63" s="14" t="s">
+      <c r="F74" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="G63" s="12"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="5" t="s">
+      <c r="G74" s="12"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="29">
-      <c r="A64" t="s">
+    <row r="75" spans="1:13" ht="30">
+      <c r="A75" t="s">
         <v>191</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B75" t="s">
         <v>200</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C75" s="22" t="s">
         <v>580</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D75" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="E64" s="22" t="s">
+      <c r="E75" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F75" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="G64" s="12" t="s">
+      <c r="G75" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="H64" s="4"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="5" t="s">
+      <c r="H75" s="4"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="5" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
-      <c r="A65" t="s">
+    <row r="76" spans="1:13">
+      <c r="A76" t="s">
         <v>191</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B76" t="s">
         <v>202</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D76" s="22" t="s">
         <v>584</v>
       </c>
-      <c r="E65" s="24" t="s">
+      <c r="E76" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F76" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="G65" s="12" t="s">
+      <c r="G76" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="5" t="s">
+      <c r="H76" s="4"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="29">
-      <c r="A66" t="s">
+    <row r="77" spans="1:13" ht="45">
+      <c r="A77" t="s">
         <v>191</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B77" t="s">
         <v>197</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C77" s="22" t="s">
         <v>586</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="D77" s="22" t="s">
         <v>587</v>
       </c>
-      <c r="E66" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="F66" s="14" t="s">
+      <c r="F77" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="G66" s="12" t="s">
+      <c r="G77" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="H66" s="4"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="5" t="s">
+      <c r="H77" s="4"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="5" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="29">
-      <c r="A67" t="s">
+    <row r="78" spans="1:13" ht="30">
+      <c r="A78" t="s">
         <v>191</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B78" t="s">
         <v>196</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C78" s="22" t="s">
         <v>589</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D78" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="E67" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>591</v>
       </c>
-      <c r="F67" s="14" t="s">
+      <c r="F78" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="G67" s="12" t="s">
+      <c r="G78" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="H67" s="4"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="5" t="s">
+      <c r="H78" s="4"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="5" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="29">
-      <c r="A68" t="s">
+    <row r="79" spans="1:13" ht="30">
+      <c r="A79" t="s">
         <v>191</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B79" t="s">
         <v>198</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C79" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="D68" s="22" t="s">
+      <c r="D79" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="E79" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F79" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="G68" s="12" t="s">
+      <c r="G79" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="H68" s="4"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="5" t="s">
+      <c r="H79" s="4"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="5" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="29">
-      <c r="A69" t="s">
+    <row r="80" spans="1:13" ht="30">
+      <c r="A80" t="s">
         <v>191</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B80" t="s">
         <v>201</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C80" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D80" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="E69" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="F80" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="G69" s="13" t="s">
+      <c r="G80" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="H69" s="4"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="5" t="s">
+      <c r="H80" s="4"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="5" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
-      <c r="A70" t="s">
+    <row r="81" spans="1:10">
+      <c r="A81" t="s">
         <v>191</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B81" t="s">
         <v>194</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C81" s="22" t="s">
         <v>598</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D81" s="22" t="s">
         <v>599</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F81" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="G70" s="12" t="s">
+      <c r="G81" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="H70" s="4"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="5" t="s">
+      <c r="H81" s="4"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="5" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
+    <row r="82" spans="1:10" ht="30">
+      <c r="A82" t="s">
         <v>191</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B82" t="s">
         <v>199</v>
       </c>
-      <c r="C71" s="22" t="s">
+      <c r="C82" s="22" t="s">
         <v>601</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="D82" s="22" t="s">
         <v>602</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>603</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F82" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="G71" s="12" t="s">
+      <c r="G82" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="H71" s="4"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="5" t="s">
+      <c r="H82" s="4"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="5" t="s">
         <v>309</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M71" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M71">
-      <sortCondition ref="A1:A71"/>
+  <autoFilter ref="A1:M82" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M82">
+      <sortCondition ref="A1:A82"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Unifying the code base behind add_p() (#697)
* in progress

* udpated `assert_package()`

* Update utils-misc.R

* in progress

* Update sysdata.rda

* in progress

* in progress

* in progress

* doc updates

* doc updates

* in progress

* in progress

* in progress

* in progress

* Update WORDLIST

* added `all_summary_cols()` function

* Update select_helpers.R

* Update utils-add_p_tests.R

* in progress

* updating add_p example

* updated help file images

* Update gallery.Rmd

* empty arg messaging

* Update utils-add_p_tests.R

* Update utils-add_p_tests.R

* Increment version number

* Update _pkgdown.yml

* Update _pkgdown.yml

* Update pull_request_template.md

* Update NEWS.md

* Update pull_request_template.md

* Update WORDLIST
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE9469E-FD70-4E3C-9437-04025112AB07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371AFA9-3CF6-4AC0-8F12-35084D8E6697}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-20" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="643">
   <si>
     <t>context</t>
   </si>
@@ -62,9 +62,6 @@
     <t>pt</t>
   </si>
   <si>
-    <t>add_p</t>
-  </si>
-  <si>
     <t>Statistical tests performed</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Testes estatísticos realizados</t>
   </si>
   <si>
-    <t>Wilcoxon rank-sum test</t>
-  </si>
-  <si>
     <t>prueba de los rangos con signo de Wilcoxon</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Teste de soma de postos de Wilcoxon</t>
   </si>
   <si>
-    <t>chi-square test of independence</t>
-  </si>
-  <si>
     <t>prueba chi cuadrado de independencia</t>
   </si>
   <si>
@@ -615,9 +606,6 @@
   </si>
   <si>
     <t>Tempo</t>
-  </si>
-  <si>
-    <t>tbl_svysummary</t>
   </si>
   <si>
     <t>chi-squared test with Rao &amp; Scott's second-order correction</t>
@@ -2056,6 +2044,30 @@
   </si>
   <si>
     <t>CI</t>
+  </si>
+  <si>
+    <t>Welch Two Sample t-test</t>
+  </si>
+  <si>
+    <t>Two Sample t-test</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallis rank sum test</t>
+  </si>
+  <si>
+    <t>Wilcoxon rank sum test with continuity correction</t>
+  </si>
+  <si>
+    <t>Wilcoxon rank sum test</t>
+  </si>
+  <si>
+    <t>Pearson's Chi-squared test</t>
+  </si>
+  <si>
+    <t>add_p.tbl_summary</t>
+  </si>
+  <si>
+    <t>add_p.tbl_svysummary</t>
   </si>
 </sst>
 </file>
@@ -2501,19 +2513,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M85"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
-    <col min="2" max="2" width="51.81640625" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" width="85.54296875" customWidth="1"/>
     <col min="3" max="3" width="49" style="22" customWidth="1"/>
     <col min="4" max="4" width="47.26953125" style="12" customWidth="1"/>
     <col min="5" max="5" width="53.54296875" style="22" customWidth="1"/>
@@ -2535,25 +2548,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -2568,2560 +2581,2648 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" hidden="1">
       <c r="A2" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" hidden="1">
+      <c r="A3" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B3" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" hidden="1">
+      <c r="A4" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" hidden="1">
+      <c r="A5" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" hidden="1">
+      <c r="A6" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" hidden="1">
+      <c r="A7" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B7" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" hidden="1">
+      <c r="A8" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B8" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" hidden="1">
+      <c r="A9" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B9" t="s">
         <v>626</v>
       </c>
-      <c r="B2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="10" spans="1:13" hidden="1">
+      <c r="A10" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B10" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:13" hidden="1">
+      <c r="A11" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B11" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="12" spans="1:13" hidden="1">
+      <c r="A12" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B12" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B9" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B10" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B11" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B12" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" hidden="1">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
+        <v>641</v>
+      </c>
+      <c r="B14" t="s">
+        <v>640</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B16" t="s">
+        <v>637</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>426</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>413</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="J15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="F16" s="16" t="s">
+      <c r="C21" s="22" t="s">
+        <v>427</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>429</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="G21" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" t="s">
-        <v>45</v>
-      </c>
-      <c r="M16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>421</v>
-      </c>
-      <c r="F17" s="17" t="s">
+      <c r="I21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B22" t="s">
+        <v>635</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="G22" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B23" t="s">
+        <v>638</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>433</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="F23" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="G23" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>426</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>427</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>367</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="I24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J24" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" t="s">
+        <v>151</v>
+      </c>
+      <c r="L24" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" hidden="1">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J19" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" t="s">
-        <v>49</v>
-      </c>
-      <c r="L19" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>428</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>429</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>430</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="I25" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" t="s">
+        <v>156</v>
+      </c>
+      <c r="L25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" hidden="1">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>431</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="I26" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J26" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" t="s">
+        <v>146</v>
+      </c>
+      <c r="L26" t="s">
+        <v>147</v>
+      </c>
+      <c r="M26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" hidden="1">
+      <c r="A27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J21" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>434</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>369</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="I27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J27" t="s">
+        <v>160</v>
+      </c>
+      <c r="K27" t="s">
+        <v>161</v>
+      </c>
+      <c r="L27" t="s">
+        <v>162</v>
+      </c>
+      <c r="M27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" hidden="1">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J28" t="s">
+        <v>135</v>
+      </c>
+      <c r="K28" t="s">
+        <v>136</v>
+      </c>
+      <c r="L28" t="s">
+        <v>137</v>
+      </c>
+      <c r="M28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" hidden="1">
+      <c r="A29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>453</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" hidden="1">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>456</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J30" t="s">
+        <v>140</v>
+      </c>
+      <c r="K30" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" t="s">
+        <v>142</v>
+      </c>
+      <c r="M30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" hidden="1">
+      <c r="A31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J31" t="s">
+        <v>165</v>
+      </c>
+      <c r="K31" t="s">
+        <v>166</v>
+      </c>
+      <c r="L31" t="s">
+        <v>167</v>
+      </c>
+      <c r="M31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" hidden="1">
+      <c r="A32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J32" t="s">
+        <v>170</v>
+      </c>
+      <c r="K32" t="s">
+        <v>171</v>
+      </c>
+      <c r="L32" t="s">
+        <v>172</v>
+      </c>
+      <c r="M32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.5" hidden="1">
+      <c r="A33" t="s">
         <v>54</v>
       </c>
-      <c r="L22" t="s">
-        <v>55</v>
-      </c>
-      <c r="M22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" t="s">
-        <v>15</v>
-      </c>
-      <c r="M23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>442</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J24" t="s">
-        <v>153</v>
-      </c>
-      <c r="K24" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" t="s">
-        <v>155</v>
-      </c>
-      <c r="M24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>443</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J25" t="s">
-        <v>158</v>
-      </c>
-      <c r="K25" t="s">
-        <v>159</v>
-      </c>
-      <c r="L25" t="s">
-        <v>160</v>
-      </c>
-      <c r="M25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>446</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>448</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J26" t="s">
-        <v>148</v>
-      </c>
-      <c r="K26" t="s">
-        <v>149</v>
-      </c>
-      <c r="L26" t="s">
-        <v>150</v>
-      </c>
-      <c r="M26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>451</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J27" t="s">
-        <v>163</v>
-      </c>
-      <c r="K27" t="s">
-        <v>164</v>
-      </c>
-      <c r="L27" t="s">
-        <v>165</v>
-      </c>
-      <c r="M27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>453</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J28" t="s">
-        <v>138</v>
-      </c>
-      <c r="K28" t="s">
-        <v>139</v>
-      </c>
-      <c r="L28" t="s">
-        <v>140</v>
-      </c>
-      <c r="M28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>455</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>456</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J29" t="s">
-        <v>133</v>
-      </c>
-      <c r="K29" t="s">
-        <v>134</v>
-      </c>
-      <c r="L29" t="s">
-        <v>135</v>
-      </c>
-      <c r="M29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>459</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" t="s">
-        <v>143</v>
-      </c>
-      <c r="K30" t="s">
-        <v>144</v>
-      </c>
-      <c r="L30" t="s">
-        <v>145</v>
-      </c>
-      <c r="M30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>462</v>
-      </c>
-      <c r="E31" s="22" t="s">
+      <c r="B33" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J31" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" t="s">
-        <v>169</v>
-      </c>
-      <c r="L31" t="s">
-        <v>170</v>
-      </c>
-      <c r="M31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="22" t="s">
+      <c r="D33" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J32" t="s">
-        <v>173</v>
-      </c>
-      <c r="K32" t="s">
-        <v>174</v>
-      </c>
-      <c r="L32" t="s">
-        <v>175</v>
-      </c>
-      <c r="M32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.5">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>209</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>467</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>467</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>468</v>
-      </c>
       <c r="F33" s="16" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5" hidden="1">
       <c r="A34" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="23"/>
       <c r="E34" s="22"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J35" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L35" t="s">
+        <v>75</v>
+      </c>
+      <c r="M35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" hidden="1">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J36" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>469</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="E35" s="22" t="s">
+      <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" hidden="1">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>471</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J35" t="s">
-        <v>76</v>
-      </c>
-      <c r="K35" t="s">
-        <v>77</v>
-      </c>
-      <c r="L35" t="s">
-        <v>78</v>
-      </c>
-      <c r="M35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="22" t="s">
+      <c r="D37" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>472</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>473</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>474</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J36" t="s">
-        <v>59</v>
-      </c>
-      <c r="K36" t="s">
-        <v>60</v>
-      </c>
-      <c r="L36" t="s">
-        <v>61</v>
-      </c>
-      <c r="M36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>475</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>475</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>476</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" t="s">
+        <v>68</v>
+      </c>
+      <c r="L38" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="22" t="s">
+    </row>
+    <row r="39" spans="1:13" hidden="1">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>476</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>477</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="E39" s="22" t="s">
         <v>478</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J38" t="s">
-        <v>72</v>
-      </c>
-      <c r="K38" t="s">
-        <v>71</v>
-      </c>
-      <c r="L38" t="s">
-        <v>73</v>
-      </c>
-      <c r="M38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>481</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>482</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" t="s">
+        <v>65</v>
+      </c>
+      <c r="K40" t="s">
+        <v>64</v>
+      </c>
+      <c r="L40" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="22" t="s">
+    </row>
+    <row r="41" spans="1:13" hidden="1">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>482</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>483</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="E41" s="22" t="s">
         <v>484</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J40" t="s">
-        <v>68</v>
-      </c>
-      <c r="K40" t="s">
-        <v>67</v>
-      </c>
-      <c r="L40" t="s">
-        <v>69</v>
-      </c>
-      <c r="M40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" t="s">
-        <v>210</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>487</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>488</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="4"/>
       <c r="I42" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" hidden="1">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="4"/>
       <c r="I43" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="4"/>
       <c r="I44" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>496</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J46" t="s">
+        <v>61</v>
+      </c>
+      <c r="K46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" t="s">
+        <v>62</v>
+      </c>
+      <c r="M46" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>501</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>502</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J46" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" t="s">
-        <v>63</v>
-      </c>
-      <c r="L46" t="s">
-        <v>65</v>
-      </c>
-      <c r="M46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="12" customFormat="1">
+    </row>
+    <row r="47" spans="1:13" s="12" customFormat="1" hidden="1">
       <c r="A47" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C47" s="22"/>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
       <c r="F47" s="14"/>
     </row>
-    <row r="48" spans="1:13" s="12" customFormat="1">
+    <row r="48" spans="1:13" s="12" customFormat="1" hidden="1">
       <c r="A48" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="14"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J49" t="s">
+        <v>112</v>
+      </c>
+      <c r="K49" t="s">
+        <v>113</v>
+      </c>
+      <c r="L49" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="M49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" hidden="1">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="E50" s="24" t="s">
         <v>503</v>
       </c>
-      <c r="D49" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="J49" t="s">
-        <v>115</v>
-      </c>
-      <c r="K49" t="s">
-        <v>116</v>
-      </c>
-      <c r="L49" t="s">
-        <v>117</v>
-      </c>
-      <c r="M49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" t="s">
-        <v>266</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>507</v>
-      </c>
       <c r="F50" s="15" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="12" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J51" t="s">
+        <v>117</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+      <c r="L51" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="M51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" hidden="1">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" t="s">
+        <v>263</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>506</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="E52" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J51" t="s">
-        <v>120</v>
-      </c>
-      <c r="K51" t="s">
-        <v>121</v>
-      </c>
-      <c r="L51" t="s">
-        <v>122</v>
-      </c>
-      <c r="M51" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>512</v>
-      </c>
       <c r="F52" s="14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" hidden="1">
       <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="J53" t="s">
+        <v>79</v>
+      </c>
+      <c r="K53" t="s">
         <v>80</v>
       </c>
-      <c r="B53" t="s">
+      <c r="L53" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="M53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" hidden="1">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="D54" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E54" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="E53" s="22" t="s">
+      <c r="F54" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="K54" t="s">
+        <v>109</v>
+      </c>
+      <c r="L54" t="s">
+        <v>110</v>
+      </c>
+      <c r="M54" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" hidden="1">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>515</v>
       </c>
-      <c r="F53" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="G53" s="12" t="s">
+      <c r="D55" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J55" t="s">
+        <v>100</v>
+      </c>
+      <c r="K55" t="s">
+        <v>99</v>
+      </c>
+      <c r="L55" t="s">
+        <v>99</v>
+      </c>
+      <c r="M55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" hidden="1">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" t="s">
+        <v>605</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="J56" t="s">
+        <v>611</v>
+      </c>
+      <c r="K56" t="s">
+        <v>93</v>
+      </c>
+      <c r="L56" t="s">
+        <v>613</v>
+      </c>
+      <c r="M56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" hidden="1">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="G57" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J53" t="s">
-        <v>82</v>
-      </c>
-      <c r="K53" t="s">
-        <v>83</v>
-      </c>
-      <c r="L53" t="s">
-        <v>84</v>
-      </c>
-      <c r="M53" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>518</v>
-      </c>
-      <c r="F54" s="20" t="s">
+      <c r="H57" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J57" t="s">
+        <v>96</v>
+      </c>
+      <c r="K57" t="s">
+        <v>95</v>
+      </c>
+      <c r="L57" t="s">
+        <v>612</v>
+      </c>
+      <c r="M57" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" hidden="1">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="G58" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="G54" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H54" s="4" t="s">
+      <c r="H58" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="K54" t="s">
-        <v>112</v>
-      </c>
-      <c r="L54" t="s">
-        <v>113</v>
-      </c>
-      <c r="M54" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>520</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J55" t="s">
-        <v>103</v>
-      </c>
-      <c r="K55" t="s">
-        <v>102</v>
-      </c>
-      <c r="L55" t="s">
-        <v>102</v>
-      </c>
-      <c r="M55" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" t="s">
-        <v>609</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>524</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="J56" t="s">
-        <v>615</v>
-      </c>
-      <c r="K56" t="s">
-        <v>96</v>
-      </c>
-      <c r="L56" t="s">
-        <v>617</v>
-      </c>
-      <c r="M56" t="s">
+      <c r="I58" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="J58" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E57" s="24" t="s">
+      <c r="K58" t="s">
+        <v>97</v>
+      </c>
+      <c r="L58" t="s">
+        <v>97</v>
+      </c>
+      <c r="M58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" hidden="1">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="22" t="s">
         <v>527</v>
       </c>
-      <c r="F57" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J57" t="s">
-        <v>99</v>
-      </c>
-      <c r="K57" t="s">
-        <v>98</v>
-      </c>
-      <c r="L57" t="s">
-        <v>616</v>
-      </c>
-      <c r="M57" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="22" t="s">
+      <c r="D59" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="E59" s="22" t="s">
         <v>528</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J58" t="s">
-        <v>101</v>
-      </c>
-      <c r="K58" t="s">
-        <v>100</v>
-      </c>
-      <c r="L58" t="s">
-        <v>100</v>
-      </c>
-      <c r="M58" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" t="s">
-        <v>262</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>532</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="4"/>
       <c r="I59" s="1"/>
       <c r="J59" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J60" t="s">
+        <v>122</v>
+      </c>
+      <c r="K60" t="s">
+        <v>123</v>
+      </c>
+      <c r="L60" t="s">
+        <v>124</v>
+      </c>
+      <c r="M60" t="s">
         <v>125</v>
       </c>
-      <c r="K60" t="s">
-        <v>126</v>
-      </c>
-      <c r="L60" t="s">
-        <v>127</v>
-      </c>
-      <c r="M60" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+    </row>
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J61" t="s">
+        <v>122</v>
+      </c>
+      <c r="K61" t="s">
+        <v>123</v>
+      </c>
+      <c r="L61" t="s">
+        <v>124</v>
+      </c>
+      <c r="M61" t="s">
         <v>125</v>
       </c>
-      <c r="K61" t="s">
-        <v>126</v>
-      </c>
-      <c r="L61" t="s">
-        <v>127</v>
-      </c>
-      <c r="M61" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+    </row>
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
       <c r="J62" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" s="2" customFormat="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A63" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="J63" s="7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" s="2" customFormat="1">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A64" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="12"/>
       <c r="H64" s="4"/>
       <c r="J64" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="2" customFormat="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A65" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="2" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" s="12" customFormat="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="12" customFormat="1" hidden="1">
       <c r="A66" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
       <c r="F66" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="J66" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="K66" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="L66" s="12" t="s">
         <v>619</v>
       </c>
-      <c r="G66" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="H66" s="12" t="s">
+      <c r="M66" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="I66" s="12" t="s">
-        <v>622</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>624</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="L66" s="12" t="s">
-        <v>623</v>
-      </c>
-      <c r="M66" s="12" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" s="2" customFormat="1">
+    </row>
+    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A67" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M67" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="22" t="s">
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1" hidden="1">
+      <c r="A68" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="E68" s="22" t="s">
         <v>549</v>
       </c>
-      <c r="E67" s="22" t="s">
+      <c r="F68" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H68" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1">
+      <c r="A69" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="F67" s="16" t="s">
-        <v>391</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" s="2" customFormat="1">
-      <c r="A68" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="22" t="s">
+      <c r="D69" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="D68" s="22" t="s">
+      <c r="E69" s="22" t="s">
         <v>552</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="H68" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M68" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" s="2" customFormat="1">
-      <c r="A69" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>554</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>556</v>
       </c>
       <c r="F69" s="14"/>
       <c r="G69" s="12"/>
       <c r="H69" s="4"/>
       <c r="J69" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" s="2" customFormat="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A70" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E70" s="24" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="12"/>
       <c r="H70" s="4"/>
       <c r="J70" s="6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" s="2" customFormat="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="2" customFormat="1" hidden="1">
       <c r="A71" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L71" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="22" t="s">
+      <c r="M71" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="2" customFormat="1" hidden="1">
+      <c r="A72" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="E72" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="D71" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="E71" s="22" t="s">
+      <c r="F72" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" hidden="1">
+      <c r="A73" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" t="s">
+        <v>180</v>
+      </c>
+      <c r="C73" s="22" t="s">
         <v>561</v>
       </c>
-      <c r="F71" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="G71" s="12" t="s">
+      <c r="D73" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J73" t="s">
+        <v>181</v>
+      </c>
+      <c r="K73" t="s">
+        <v>182</v>
+      </c>
+      <c r="L73" t="s">
+        <v>180</v>
+      </c>
+      <c r="M73" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" hidden="1">
+      <c r="A74" t="s">
+        <v>179</v>
+      </c>
+      <c r="B74" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J74" t="s">
+        <v>184</v>
+      </c>
+      <c r="K74" t="s">
+        <v>185</v>
+      </c>
+      <c r="L74" t="s">
+        <v>186</v>
+      </c>
+      <c r="M74" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="29">
+      <c r="A75" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B75" t="s">
+        <v>191</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>567</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="F75" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="G75" s="12" t="s">
         <v>347</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" s="2" customFormat="1">
-      <c r="A72" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="F72" s="20" t="s">
-        <v>394</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="A73" t="s">
-        <v>182</v>
-      </c>
-      <c r="B73" t="s">
-        <v>183</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="F73" s="20" t="s">
-        <v>395</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J73" t="s">
-        <v>184</v>
-      </c>
-      <c r="K73" t="s">
-        <v>185</v>
-      </c>
-      <c r="L73" t="s">
-        <v>183</v>
-      </c>
-      <c r="M73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" t="s">
-        <v>182</v>
-      </c>
-      <c r="B74" t="s">
-        <v>186</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="E74" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="F74" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="J74" t="s">
-        <v>187</v>
-      </c>
-      <c r="K74" t="s">
-        <v>188</v>
-      </c>
-      <c r="L74" t="s">
-        <v>189</v>
-      </c>
-      <c r="M74" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="29">
-      <c r="A75" t="s">
-        <v>191</v>
-      </c>
-      <c r="B75" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="F75" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>351</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="1"/>
       <c r="J75" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="29">
-      <c r="A76" t="s">
-        <v>191</v>
+      <c r="A76" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B76" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="1"/>
       <c r="J76" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="29">
-      <c r="A77" t="s">
-        <v>191</v>
+      <c r="A77" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B77" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77" s="4"/>
       <c r="I77" s="1"/>
       <c r="J77" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="29">
-      <c r="A78" t="s">
-        <v>191</v>
+      <c r="A78" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B78" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="79" spans="1:13">
-      <c r="A79" t="s">
-        <v>191</v>
+      <c r="A79" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B79" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="29">
-      <c r="A80" t="s">
-        <v>191</v>
+      <c r="A80" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29">
-      <c r="A81" t="s">
-        <v>191</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="29">
+      <c r="A81" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B81" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29">
-      <c r="A82" t="s">
-        <v>191</v>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="29">
+      <c r="A82" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B82" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="29">
-      <c r="A83" t="s">
-        <v>191</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="29">
+      <c r="A83" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B83" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" t="s">
-        <v>191</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B84" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" t="s">
-        <v>191</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="12" t="s">
+        <v>642</v>
       </c>
       <c r="B85" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" s="12" customFormat="1">
+      <c r="A86" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="F86" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H86" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="I86" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J86" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K86" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L86" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M86" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="12" customFormat="1">
+      <c r="A87" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>433</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="F87" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H87" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="J87" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K87" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L87" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M87" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M85" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+  <autoFilter ref="A1:M87" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="add_p"/>
+        <filter val="tbl_svysummary"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M85">
       <sortCondition ref="A1:A85"/>
     </sortState>

</xml_diff>

<commit_message>
added RR to translation xls file
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371AFA9-3CF6-4AC0-8F12-35084D8E6697}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA93947E-574F-430B-A0C1-89F14BC4DBA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$90</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="646">
   <si>
     <t>context</t>
   </si>
@@ -2068,6 +2068,15 @@
   </si>
   <si>
     <t>add_p.tbl_svysummary</t>
+  </si>
+  <si>
+    <t>log(RR)</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>RR = Relative Risk</t>
   </si>
 </sst>
 </file>
@@ -2513,14 +2522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2581,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>622</v>
       </c>
@@ -2589,7 +2597,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="12" t="s">
         <v>622</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="12" t="s">
         <v>622</v>
       </c>
@@ -2605,7 +2613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="12" t="s">
         <v>622</v>
       </c>
@@ -2613,7 +2621,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="12" t="s">
         <v>622</v>
       </c>
@@ -2621,7 +2629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="12" t="s">
         <v>622</v>
       </c>
@@ -2629,7 +2637,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="12" t="s">
         <v>622</v>
       </c>
@@ -2637,7 +2645,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="12" t="s">
         <v>622</v>
       </c>
@@ -2645,7 +2653,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="12" t="s">
         <v>622</v>
       </c>
@@ -2653,7 +2661,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>622</v>
       </c>
@@ -2661,7 +2669,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="12" t="s">
         <v>622</v>
       </c>
@@ -2669,7 +2677,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -3118,7 +3126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -3159,7 +3167,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -3241,7 +3249,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -3282,7 +3290,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -3323,7 +3331,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -3364,7 +3372,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -3446,7 +3454,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -3487,7 +3495,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.5" hidden="1">
+    <row r="33" spans="1:13" ht="15.5">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3514,7 +3522,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5" hidden="1">
+    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5">
       <c r="A34" s="12" t="s">
         <v>54</v>
       </c>
@@ -3526,7 +3534,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3567,7 +3575,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -3608,7 +3616,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -3632,7 +3640,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -3673,7 +3681,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -3697,7 +3705,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3738,7 +3746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3760,7 +3768,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3782,7 +3790,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3804,1109 +3812,1063 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1">
-      <c r="A44" t="s">
+    <row r="44" spans="1:13" s="12" customFormat="1">
+      <c r="A44" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" s="12" customFormat="1">
+      <c r="A45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>644</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" s="12" customFormat="1">
+      <c r="A46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
         <v>200</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D47" s="22" t="s">
         <v>492</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E47" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="1" t="s">
+      <c r="G47" s="12"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1">
-      <c r="A45" t="s">
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>199</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C48" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D48" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>495</v>
       </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="4" t="s">
+      <c r="G48" s="12"/>
+      <c r="H48" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1">
-      <c r="A46" t="s">
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C49" s="22" t="s">
         <v>496</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D49" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E49" s="24" t="s">
         <v>498</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G49" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J49" t="s">
         <v>61</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K49" t="s">
         <v>60</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L49" t="s">
         <v>62</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M49" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A47" s="12" t="s">
+    <row r="50" spans="1:13" s="12" customFormat="1">
+      <c r="A50" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>632</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A48" s="12" t="s">
+      <c r="C50" s="22"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" s="12" customFormat="1">
+      <c r="A51" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B51" s="12" t="s">
         <v>633</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:13" hidden="1">
-      <c r="A49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" t="s">
-        <v>111</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J49" t="s">
-        <v>112</v>
-      </c>
-      <c r="K49" t="s">
-        <v>113</v>
-      </c>
-      <c r="L49" t="s">
-        <v>114</v>
-      </c>
-      <c r="M49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" hidden="1">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>262</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>501</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>502</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>503</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" hidden="1">
-      <c r="A51" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J51" t="s">
-        <v>117</v>
-      </c>
-      <c r="K51" t="s">
-        <v>118</v>
-      </c>
-      <c r="L51" t="s">
-        <v>119</v>
-      </c>
-      <c r="M51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" hidden="1">
+      <c r="C51" s="22"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>507</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G52" s="12"/>
+        <v>499</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>332</v>
+      </c>
       <c r="H52" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I52" s="1"/>
-      <c r="J52" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" hidden="1">
+        <v>279</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" t="s">
+        <v>112</v>
+      </c>
+      <c r="K52" t="s">
+        <v>113</v>
+      </c>
+      <c r="L52" t="s">
+        <v>114</v>
+      </c>
+      <c r="M52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>262</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>334</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J53" t="s">
-        <v>79</v>
-      </c>
-      <c r="K53" t="s">
-        <v>80</v>
-      </c>
-      <c r="L53" t="s">
-        <v>81</v>
-      </c>
-      <c r="M53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1">
+        <v>280</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>335</v>
+        <v>505</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>382</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>289</v>
+        <v>230</v>
+      </c>
+      <c r="J54" t="s">
+        <v>117</v>
       </c>
       <c r="K54" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L54" t="s">
-        <v>110</v>
-      </c>
-      <c r="M54" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" hidden="1">
+        <v>119</v>
+      </c>
+      <c r="M54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>517</v>
+        <v>507</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>508</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>336</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="G55" s="12"/>
       <c r="H55" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J55" t="s">
-        <v>100</v>
-      </c>
-      <c r="K55" t="s">
-        <v>99</v>
-      </c>
-      <c r="L55" t="s">
-        <v>99</v>
-      </c>
-      <c r="M55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" hidden="1">
+        <v>282</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>605</v>
+        <v>78</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>520</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>385</v>
+        <v>510</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>384</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>609</v>
+        <v>231</v>
       </c>
       <c r="J56" t="s">
-        <v>611</v>
+        <v>79</v>
       </c>
       <c r="K56" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="L56" t="s">
-        <v>613</v>
+        <v>81</v>
       </c>
       <c r="M56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" hidden="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>523</v>
+        <v>513</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>514</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>386</v>
+        <v>335</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J57" t="s">
-        <v>96</v>
+        <v>608</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>289</v>
       </c>
       <c r="K57" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="L57" t="s">
-        <v>612</v>
-      </c>
-      <c r="M57" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" hidden="1">
+        <v>110</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J58" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>605</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>527</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" hidden="1">
+        <v>519</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="J59" t="s">
+        <v>611</v>
+      </c>
+      <c r="K59" t="s">
+        <v>93</v>
+      </c>
+      <c r="L59" t="s">
+        <v>613</v>
+      </c>
+      <c r="M59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>531</v>
+        <v>522</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>386</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H60" s="4"/>
+        <v>338</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="I60" s="1" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
       <c r="J60" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="K60" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="L60" t="s">
-        <v>124</v>
+        <v>612</v>
       </c>
       <c r="M60" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" hidden="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>531</v>
+        <v>526</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>251</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H61" s="4"/>
+        <v>339</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>251</v>
+      </c>
       <c r="I61" s="1" t="s">
-        <v>232</v>
+        <v>97</v>
       </c>
       <c r="J61" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="K61" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="L61" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="M61" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" hidden="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>534</v>
+        <v>527</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>528</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="8" t="s">
+      <c r="J62" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J63" t="s">
+        <v>122</v>
+      </c>
+      <c r="K63" t="s">
+        <v>123</v>
+      </c>
+      <c r="L63" t="s">
+        <v>124</v>
+      </c>
+      <c r="M63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J64" t="s">
+        <v>122</v>
+      </c>
+      <c r="K64" t="s">
+        <v>123</v>
+      </c>
+      <c r="L64" t="s">
+        <v>124</v>
+      </c>
+      <c r="M64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>260</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A63" s="2" t="s">
+    <row r="66" spans="1:13" s="2" customFormat="1">
+      <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C66" s="22" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D66" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="E63" s="22" t="s">
+      <c r="E66" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="4"/>
-      <c r="J63" s="7" t="s">
+      <c r="F66" s="14"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="4"/>
+      <c r="J66" s="7" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A64" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="D64" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>540</v>
-      </c>
-      <c r="F64" s="14"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="4"/>
-      <c r="J64" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A65" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>542</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="F65" s="14"/>
-      <c r="G65" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A66" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="H66" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="L66" s="12" t="s">
-        <v>619</v>
-      </c>
-      <c r="M66" s="12" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1">
+    <row r="67" spans="1:13" s="2" customFormat="1">
       <c r="A67" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>101</v>
+        <v>261</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>539</v>
+      </c>
+      <c r="E67" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="4"/>
+      <c r="J67" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>604</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>388</v>
-      </c>
+        <v>543</v>
+      </c>
+      <c r="F68" s="14"/>
       <c r="G68" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H68" s="22" t="s">
-        <v>603</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="H68" s="4"/>
       <c r="I68" s="2" t="s">
-        <v>233</v>
+        <v>610</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>89</v>
+        <v>604</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>91</v>
+        <v>604</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A69" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="12" customFormat="1">
+      <c r="A69" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="F69" s="14"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="4"/>
-      <c r="J69" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" s="2" customFormat="1" hidden="1">
+      <c r="B69" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="J69" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="K69" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="L69" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="M69" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>259</v>
+        <v>101</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>554</v>
-      </c>
-      <c r="E70" s="24" t="s">
-        <v>555</v>
-      </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="4"/>
-      <c r="J70" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>544</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>389</v>
+        <v>549</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>388</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>283</v>
+        <v>342</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>603</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="4"/>
+      <c r="J72" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="2" customFormat="1">
+      <c r="A73" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="E73" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="F73" s="14"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="4"/>
+      <c r="J73" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="2" customFormat="1">
+      <c r="A75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C75" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D75" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E75" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F75" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G75" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="H72" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J75" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K75" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="M75" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1">
-      <c r="A73" t="s">
+    <row r="76" spans="1:13">
+      <c r="A76" t="s">
         <v>179</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>180</v>
       </c>
-      <c r="C73" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>561</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D76" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E76" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F76" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="G73" s="12" t="s">
+      <c r="G76" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H76" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J73" t="s">
+      <c r="J76" t="s">
         <v>181</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K76" t="s">
         <v>182</v>
       </c>
-      <c r="L73" t="s">
+      <c r="L76" t="s">
         <v>180</v>
       </c>
-      <c r="M73" t="s">
+      <c r="M76" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1">
-      <c r="A74" t="s">
+    <row r="77" spans="1:13">
+      <c r="A77" t="s">
         <v>179</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>183</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C77" s="22" t="s">
         <v>564</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D77" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="F74" s="16" t="s">
+      <c r="F77" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="G74" s="12" t="s">
+      <c r="G77" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H77" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="I77" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J77" t="s">
         <v>184</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K77" t="s">
         <v>185</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L77" t="s">
         <v>186</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M77" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="29">
-      <c r="A75" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B75" t="s">
-        <v>191</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="F75" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="H75" s="4"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="29">
-      <c r="A76" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B76" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="H76" s="4"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="29">
-      <c r="A77" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B77" t="s">
-        <v>188</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>574</v>
-      </c>
-      <c r="E77" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G77" s="12"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="5" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="29">
@@ -4914,55 +4876,55 @@
         <v>642</v>
       </c>
       <c r="B78" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>395</v>
+        <v>569</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>392</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="29">
       <c r="A79" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B79" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>581</v>
+        <v>571</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>572</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="29">
@@ -4970,27 +4932,25 @@
         <v>642</v>
       </c>
       <c r="B80" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>351</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="G80" s="12"/>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="29">
@@ -4998,55 +4958,55 @@
         <v>642</v>
       </c>
       <c r="B81" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="29">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B82" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>589</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>590</v>
+        <v>580</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>581</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="29">
@@ -5054,177 +5014,255 @@
         <v>642</v>
       </c>
       <c r="B83" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="F83" s="15" t="s">
-        <v>400</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>354</v>
+        <v>584</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>351</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="29">
       <c r="A84" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="29">
       <c r="A85" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" s="12" customFormat="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="29">
       <c r="A86" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>636</v>
+      <c r="B86" t="s">
+        <v>197</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>430</v>
+        <v>591</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>431</v>
+        <v>592</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H86" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="I86" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J86" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K86" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L86" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="M86" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" s="12" customFormat="1">
+        <v>593</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="H86" s="4"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B88" t="s">
+        <v>195</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="H88" s="4"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" s="12" customFormat="1">
+      <c r="A89" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J89" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K89" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L89" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M89" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="12" customFormat="1">
+      <c r="A90" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B90" s="12" t="s">
         <v>639</v>
       </c>
-      <c r="C87" s="22" t="s">
+      <c r="C90" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="D90" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="E87" s="22" t="s">
+      <c r="E90" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="F87" s="19" t="s">
+      <c r="F90" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="G87" s="12" t="s">
+      <c r="G90" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="H87" s="12" t="s">
+      <c r="H90" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="I87" s="12" t="s">
+      <c r="I90" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="J87" s="12" t="s">
+      <c r="J90" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K87" s="12" t="s">
+      <c r="K90" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L87" s="12" t="s">
+      <c r="L90" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M87" s="12" t="s">
+      <c r="M90" s="12" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M87" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="add_p"/>
-        <filter val="tbl_svysummary"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M85">
-      <sortCondition ref="A1:A85"/>
+  <autoFilter ref="A1:M90" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M88">
+      <sortCondition ref="A1:A88"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
`tbl_regression()` adding Relative Risk footnote with RR definition (#791)
* Add footnote for RR

* added RR to translation xls file
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371AFA9-3CF6-4AC0-8F12-35084D8E6697}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA93947E-574F-430B-A0C1-89F14BC4DBA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$90</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="646">
   <si>
     <t>context</t>
   </si>
@@ -2068,6 +2068,15 @@
   </si>
   <si>
     <t>add_p.tbl_svysummary</t>
+  </si>
+  <si>
+    <t>log(RR)</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>RR = Relative Risk</t>
   </si>
 </sst>
 </file>
@@ -2513,14 +2522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2581,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>622</v>
       </c>
@@ -2589,7 +2597,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="12" t="s">
         <v>622</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="12" t="s">
         <v>622</v>
       </c>
@@ -2605,7 +2613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="12" t="s">
         <v>622</v>
       </c>
@@ -2613,7 +2621,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="12" t="s">
         <v>622</v>
       </c>
@@ -2621,7 +2629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="12" t="s">
         <v>622</v>
       </c>
@@ -2629,7 +2637,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="12" t="s">
         <v>622</v>
       </c>
@@ -2637,7 +2645,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="12" t="s">
         <v>622</v>
       </c>
@@ -2645,7 +2653,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="12" t="s">
         <v>622</v>
       </c>
@@ -2653,7 +2661,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" s="12" t="s">
         <v>622</v>
       </c>
@@ -2661,7 +2669,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="12" t="s">
         <v>622</v>
       </c>
@@ -2669,7 +2677,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -3118,7 +3126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -3159,7 +3167,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -3241,7 +3249,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -3282,7 +3290,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -3323,7 +3331,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -3364,7 +3372,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -3446,7 +3454,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -3487,7 +3495,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.5" hidden="1">
+    <row r="33" spans="1:13" ht="15.5">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3514,7 +3522,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5" hidden="1">
+    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5">
       <c r="A34" s="12" t="s">
         <v>54</v>
       </c>
@@ -3526,7 +3534,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3567,7 +3575,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -3608,7 +3616,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -3632,7 +3640,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -3673,7 +3681,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -3697,7 +3705,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3738,7 +3746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3760,7 +3768,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3782,7 +3790,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3804,1109 +3812,1063 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1">
-      <c r="A44" t="s">
+    <row r="44" spans="1:13" s="12" customFormat="1">
+      <c r="A44" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" s="12" customFormat="1">
+      <c r="A45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>644</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" s="12" customFormat="1">
+      <c r="A46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
         <v>200</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D47" s="22" t="s">
         <v>492</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E47" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="1" t="s">
+      <c r="G47" s="12"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1">
-      <c r="A45" t="s">
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>199</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C48" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D48" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>495</v>
       </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="4" t="s">
+      <c r="G48" s="12"/>
+      <c r="H48" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1">
-      <c r="A46" t="s">
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C49" s="22" t="s">
         <v>496</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D49" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E49" s="24" t="s">
         <v>498</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G49" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J49" t="s">
         <v>61</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K49" t="s">
         <v>60</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L49" t="s">
         <v>62</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M49" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A47" s="12" t="s">
+    <row r="50" spans="1:13" s="12" customFormat="1">
+      <c r="A50" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>632</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A48" s="12" t="s">
+      <c r="C50" s="22"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" s="12" customFormat="1">
+      <c r="A51" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B51" s="12" t="s">
         <v>633</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:13" hidden="1">
-      <c r="A49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" t="s">
-        <v>111</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J49" t="s">
-        <v>112</v>
-      </c>
-      <c r="K49" t="s">
-        <v>113</v>
-      </c>
-      <c r="L49" t="s">
-        <v>114</v>
-      </c>
-      <c r="M49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" hidden="1">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>262</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>501</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>502</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>503</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" hidden="1">
-      <c r="A51" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J51" t="s">
-        <v>117</v>
-      </c>
-      <c r="K51" t="s">
-        <v>118</v>
-      </c>
-      <c r="L51" t="s">
-        <v>119</v>
-      </c>
-      <c r="M51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" hidden="1">
+      <c r="C51" s="22"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>507</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G52" s="12"/>
+        <v>499</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>332</v>
+      </c>
       <c r="H52" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I52" s="1"/>
-      <c r="J52" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" hidden="1">
+        <v>279</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" t="s">
+        <v>112</v>
+      </c>
+      <c r="K52" t="s">
+        <v>113</v>
+      </c>
+      <c r="L52" t="s">
+        <v>114</v>
+      </c>
+      <c r="M52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>262</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>334</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J53" t="s">
-        <v>79</v>
-      </c>
-      <c r="K53" t="s">
-        <v>80</v>
-      </c>
-      <c r="L53" t="s">
-        <v>81</v>
-      </c>
-      <c r="M53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1">
+        <v>280</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>335</v>
+        <v>505</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>382</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>289</v>
+        <v>230</v>
+      </c>
+      <c r="J54" t="s">
+        <v>117</v>
       </c>
       <c r="K54" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L54" t="s">
-        <v>110</v>
-      </c>
-      <c r="M54" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" hidden="1">
+        <v>119</v>
+      </c>
+      <c r="M54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>517</v>
+        <v>507</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>508</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>336</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="G55" s="12"/>
       <c r="H55" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J55" t="s">
-        <v>100</v>
-      </c>
-      <c r="K55" t="s">
-        <v>99</v>
-      </c>
-      <c r="L55" t="s">
-        <v>99</v>
-      </c>
-      <c r="M55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" hidden="1">
+        <v>282</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>605</v>
+        <v>78</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>520</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>385</v>
+        <v>510</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>384</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>609</v>
+        <v>231</v>
       </c>
       <c r="J56" t="s">
-        <v>611</v>
+        <v>79</v>
       </c>
       <c r="K56" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="L56" t="s">
-        <v>613</v>
+        <v>81</v>
       </c>
       <c r="M56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" hidden="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>523</v>
+        <v>513</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>514</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>386</v>
+        <v>335</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J57" t="s">
-        <v>96</v>
+        <v>608</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>289</v>
       </c>
       <c r="K57" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="L57" t="s">
-        <v>612</v>
-      </c>
-      <c r="M57" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" hidden="1">
+        <v>110</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J58" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L58" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>605</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>527</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" hidden="1">
+        <v>519</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="J59" t="s">
+        <v>611</v>
+      </c>
+      <c r="K59" t="s">
+        <v>93</v>
+      </c>
+      <c r="L59" t="s">
+        <v>613</v>
+      </c>
+      <c r="M59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>531</v>
+        <v>522</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>386</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H60" s="4"/>
+        <v>338</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="I60" s="1" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
       <c r="J60" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="K60" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="L60" t="s">
-        <v>124</v>
+        <v>612</v>
       </c>
       <c r="M60" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" hidden="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>531</v>
+        <v>526</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>251</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H61" s="4"/>
+        <v>339</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>251</v>
+      </c>
       <c r="I61" s="1" t="s">
-        <v>232</v>
+        <v>97</v>
       </c>
       <c r="J61" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="K61" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="L61" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="M61" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" hidden="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>534</v>
+        <v>527</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>528</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="4"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="8" t="s">
+      <c r="J62" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J63" t="s">
+        <v>122</v>
+      </c>
+      <c r="K63" t="s">
+        <v>123</v>
+      </c>
+      <c r="L63" t="s">
+        <v>124</v>
+      </c>
+      <c r="M63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J64" t="s">
+        <v>122</v>
+      </c>
+      <c r="K64" t="s">
+        <v>123</v>
+      </c>
+      <c r="L64" t="s">
+        <v>124</v>
+      </c>
+      <c r="M64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>260</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A63" s="2" t="s">
+    <row r="66" spans="1:13" s="2" customFormat="1">
+      <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C66" s="22" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D66" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="E63" s="22" t="s">
+      <c r="E66" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="4"/>
-      <c r="J63" s="7" t="s">
+      <c r="F66" s="14"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="4"/>
+      <c r="J66" s="7" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A64" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="D64" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>540</v>
-      </c>
-      <c r="F64" s="14"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="4"/>
-      <c r="J64" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A65" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>542</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="F65" s="14"/>
-      <c r="G65" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L65" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" s="12" customFormat="1" hidden="1">
-      <c r="A66" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="H66" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="L66" s="12" t="s">
-        <v>619</v>
-      </c>
-      <c r="M66" s="12" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1">
+    <row r="67" spans="1:13" s="2" customFormat="1">
       <c r="A67" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>101</v>
+        <v>261</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>539</v>
+      </c>
+      <c r="E67" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="4"/>
+      <c r="J67" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>604</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>388</v>
-      </c>
+        <v>543</v>
+      </c>
+      <c r="F68" s="14"/>
       <c r="G68" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H68" s="22" t="s">
-        <v>603</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="H68" s="4"/>
       <c r="I68" s="2" t="s">
-        <v>233</v>
+        <v>610</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>89</v>
+        <v>604</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>91</v>
+        <v>604</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1">
-      <c r="A69" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="12" customFormat="1">
+      <c r="A69" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="F69" s="14"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="4"/>
-      <c r="J69" s="6" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" s="2" customFormat="1" hidden="1">
+      <c r="B69" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="J69" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="K69" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="L69" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="M69" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>259</v>
+        <v>101</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>554</v>
-      </c>
-      <c r="E70" s="24" t="s">
-        <v>555</v>
-      </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="4"/>
-      <c r="J70" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>544</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>389</v>
+        <v>549</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>388</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>283</v>
+        <v>342</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>603</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" s="2" customFormat="1" hidden="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="4"/>
+      <c r="J72" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="2" customFormat="1">
+      <c r="A73" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="E73" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="F73" s="14"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="4"/>
+      <c r="J73" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="2" customFormat="1">
+      <c r="A75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C75" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D75" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E75" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F75" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G75" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="H72" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J75" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K75" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="M75" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1">
-      <c r="A73" t="s">
+    <row r="76" spans="1:13">
+      <c r="A76" t="s">
         <v>179</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>180</v>
       </c>
-      <c r="C73" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>561</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D76" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E76" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F76" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="G73" s="12" t="s">
+      <c r="G76" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H76" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J73" t="s">
+      <c r="J76" t="s">
         <v>181</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K76" t="s">
         <v>182</v>
       </c>
-      <c r="L73" t="s">
+      <c r="L76" t="s">
         <v>180</v>
       </c>
-      <c r="M73" t="s">
+      <c r="M76" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1">
-      <c r="A74" t="s">
+    <row r="77" spans="1:13">
+      <c r="A77" t="s">
         <v>179</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>183</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C77" s="22" t="s">
         <v>564</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D77" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="F74" s="16" t="s">
+      <c r="F77" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="G74" s="12" t="s">
+      <c r="G77" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H77" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="I77" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J77" t="s">
         <v>184</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K77" t="s">
         <v>185</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L77" t="s">
         <v>186</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M77" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="29">
-      <c r="A75" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B75" t="s">
-        <v>191</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="F75" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="H75" s="4"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="29">
-      <c r="A76" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B76" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="H76" s="4"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="29">
-      <c r="A77" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B77" t="s">
-        <v>188</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>574</v>
-      </c>
-      <c r="E77" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G77" s="12"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="5" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="29">
@@ -4914,55 +4876,55 @@
         <v>642</v>
       </c>
       <c r="B78" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>395</v>
+        <v>569</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>392</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="29">
       <c r="A79" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B79" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>581</v>
+        <v>571</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>572</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="29">
@@ -4970,27 +4932,25 @@
         <v>642</v>
       </c>
       <c r="B80" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>351</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="G80" s="12"/>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="29">
@@ -4998,55 +4958,55 @@
         <v>642</v>
       </c>
       <c r="B81" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="29">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B82" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>589</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>590</v>
+        <v>580</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>581</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="29">
@@ -5054,177 +5014,255 @@
         <v>642</v>
       </c>
       <c r="B83" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="F83" s="15" t="s">
-        <v>400</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>354</v>
+        <v>584</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>351</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="29">
       <c r="A84" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="29">
       <c r="A85" s="12" t="s">
         <v>642</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" s="12" customFormat="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="29">
       <c r="A86" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>636</v>
+      <c r="B86" t="s">
+        <v>197</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>430</v>
+        <v>591</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>431</v>
+        <v>592</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H86" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="I86" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J86" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K86" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L86" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="M86" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" s="12" customFormat="1">
+        <v>593</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="H86" s="4"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B88" t="s">
+        <v>195</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="H88" s="4"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" s="12" customFormat="1">
+      <c r="A89" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J89" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K89" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L89" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M89" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="12" customFormat="1">
+      <c r="A90" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="B90" s="12" t="s">
         <v>639</v>
       </c>
-      <c r="C87" s="22" t="s">
+      <c r="C90" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="D90" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="E87" s="22" t="s">
+      <c r="E90" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="F87" s="19" t="s">
+      <c r="F90" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="G87" s="12" t="s">
+      <c r="G90" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="H87" s="12" t="s">
+      <c r="H90" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="I87" s="12" t="s">
+      <c r="I90" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="J87" s="12" t="s">
+      <c r="J90" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K87" s="12" t="s">
+      <c r="K90" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L87" s="12" t="s">
+      <c r="L90" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M87" s="12" t="s">
+      <c r="M90" s="12" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M87" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="add_p"/>
-        <filter val="tbl_svysummary"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M85">
-      <sortCondition ref="A1:A85"/>
+  <autoFilter ref="A1:M90" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M88">
+      <sortCondition ref="A1:A88"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Icelandic language support (#793)
* Icelandic language support

* Changes to the man for the icelandic language

* checking translations

* updates

* Update DESCRIPTION

* Update add_p.R

* Update utils-tbl_summary.R

Co-authored-by: ddsjoberg <danield.sjoberg@gmail.com>
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA93947E-574F-430B-A0C1-89F14BC4DBA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828AFEC-6018-4DE0-9D25-2F9325FE801A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="684">
   <si>
     <t>context</t>
   </si>
@@ -2077,6 +2077,120 @@
   </si>
   <si>
     <t>RR = Relative Risk</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Samtals</t>
+  </si>
+  <si>
+    <t>Kí kvaðrat próf</t>
+  </si>
+  <si>
+    <t>Einhliða fervikagreining</t>
+  </si>
+  <si>
+    <t>p-gildi</t>
+  </si>
+  <si>
+    <t>Tölfræði</t>
+  </si>
+  <si>
+    <t>Tölfræðipróf framkvæmd</t>
+  </si>
+  <si>
+    <t>t-próf</t>
+  </si>
+  <si>
+    <t>q-gildi</t>
+  </si>
+  <si>
+    <t>CI = Öryggisbil</t>
+  </si>
+  <si>
+    <t>Öryggisbil</t>
+  </si>
+  <si>
+    <t>HR - Hættuhlutfall</t>
+  </si>
+  <si>
+    <t>IRR - Nýgengihlutfall</t>
+  </si>
+  <si>
+    <t>OR - Gagnlíkindahlutfall</t>
+  </si>
+  <si>
+    <t>SE = Staðalskekkja</t>
+  </si>
+  <si>
+    <t>% ekki til staðar</t>
+  </si>
+  <si>
+    <t>% ekki til staðar (óvigtað)</t>
+  </si>
+  <si>
+    <t>%  til staðar</t>
+  </si>
+  <si>
+    <t>%  til staðar (óvigtað)</t>
+  </si>
+  <si>
+    <t>Einkenni</t>
+  </si>
+  <si>
+    <t>Hámark</t>
+  </si>
+  <si>
+    <t>Meðaltal</t>
+  </si>
+  <si>
+    <t>Miðgildi</t>
+  </si>
+  <si>
+    <t>Lágmark</t>
+  </si>
+  <si>
+    <t>N ekki til staðar</t>
+  </si>
+  <si>
+    <t>N ekki til staðar (án vigtar)</t>
+  </si>
+  <si>
+    <t>N til staðar</t>
+  </si>
+  <si>
+    <t>N til staðar (án vigtar)</t>
+  </si>
+  <si>
+    <t>Engar athuganir</t>
+  </si>
+  <si>
+    <t>Spönn</t>
+  </si>
+  <si>
+    <t>Staðalfrávik</t>
+  </si>
+  <si>
+    <t>Tölfræði sýnd</t>
+  </si>
+  <si>
+    <t>Heildarfjöldi N</t>
+  </si>
+  <si>
+    <t>Heildarfjöldi N (án vigtar)</t>
+  </si>
+  <si>
+    <t>Óþekkt</t>
+  </si>
+  <si>
+    <t>Dreifni</t>
+  </si>
+  <si>
+    <t>Prósentumörk</t>
+  </si>
+  <si>
+    <t>Tími</t>
   </si>
 </sst>
 </file>
@@ -2522,33 +2636,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.54296875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="51.6328125" customWidth="1"/>
     <col min="3" max="3" width="49" style="22" customWidth="1"/>
-    <col min="4" max="4" width="47.26953125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="49" customWidth="1"/>
-    <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.26953125" style="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" style="22" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="38.453125" style="14" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" style="13" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="39.54296875" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="49" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="67" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="51" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="52" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="52.7265625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="57.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2588,8 +2703,11 @@
       <c r="M1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>622</v>
       </c>
@@ -2597,7 +2715,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="12" t="s">
         <v>622</v>
       </c>
@@ -2605,7 +2723,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="12" t="s">
         <v>622</v>
       </c>
@@ -2613,7 +2731,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="12" t="s">
         <v>622</v>
       </c>
@@ -2621,7 +2739,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="12" t="s">
         <v>622</v>
       </c>
@@ -2629,7 +2747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="12" t="s">
         <v>622</v>
       </c>
@@ -2637,7 +2755,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="12" t="s">
         <v>622</v>
       </c>
@@ -2645,7 +2763,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="12" t="s">
         <v>622</v>
       </c>
@@ -2653,7 +2771,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="12" t="s">
         <v>622</v>
       </c>
@@ -2661,7 +2779,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="12" t="s">
         <v>622</v>
       </c>
@@ -2669,7 +2787,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="12" t="s">
         <v>622</v>
       </c>
@@ -2677,7 +2795,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -2715,8 +2833,11 @@
       <c r="M13" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>641</v>
       </c>
@@ -2756,8 +2877,11 @@
       <c r="M14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="12" t="s">
         <v>641</v>
       </c>
@@ -2798,7 +2922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="12" t="s">
         <v>641</v>
       </c>
@@ -2839,7 +2963,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" s="12" t="s">
         <v>641</v>
       </c>
@@ -2879,8 +3003,11 @@
       <c r="M17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="12" t="s">
         <v>641</v>
       </c>
@@ -2920,8 +3047,11 @@
       <c r="M18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="12" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="12" t="s">
         <v>641</v>
       </c>
@@ -2961,8 +3091,9 @@
       <c r="M19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="12" t="s">
         <v>641</v>
       </c>
@@ -3002,8 +3133,11 @@
       <c r="M20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="12" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="12" t="s">
         <v>641</v>
       </c>
@@ -3043,8 +3177,11 @@
       <c r="M21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="12" t="s">
         <v>641</v>
       </c>
@@ -3084,8 +3221,11 @@
       <c r="M22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="12" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="12" t="s">
         <v>641</v>
       </c>
@@ -3126,7 +3266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -3167,7 +3307,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -3208,7 +3348,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -3249,7 +3389,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -3290,7 +3430,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -3331,7 +3471,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -3372,7 +3512,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -3413,7 +3553,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -3454,7 +3594,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -3494,8 +3634,11 @@
       <c r="M32" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.5">
+      <c r="N32" s="12" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.5">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3521,8 +3664,11 @@
       <c r="I33" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" s="12" customFormat="1" ht="15.5">
+      <c r="N33" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="12" customFormat="1" ht="15.5">
       <c r="A34" s="12" t="s">
         <v>54</v>
       </c>
@@ -3533,8 +3679,11 @@
       <c r="D34" s="23"/>
       <c r="E34" s="22"/>
       <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3574,8 +3723,11 @@
       <c r="M35" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="12" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -3615,8 +3767,11 @@
       <c r="M36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="12" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -3639,8 +3794,11 @@
       <c r="I37" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -3680,8 +3838,11 @@
       <c r="M38" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="12" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -3704,8 +3865,11 @@
       <c r="I39" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3745,8 +3909,11 @@
       <c r="M40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" s="12" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3768,7 +3935,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3790,7 +3957,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3812,7 +3979,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="12" customFormat="1">
+    <row r="44" spans="1:14" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
         <v>54</v>
       </c>
@@ -3824,7 +3991,7 @@
       <c r="E44" s="22"/>
       <c r="F44" s="14"/>
     </row>
-    <row r="45" spans="1:13" s="12" customFormat="1">
+    <row r="45" spans="1:14" s="12" customFormat="1">
       <c r="A45" s="12" t="s">
         <v>54</v>
       </c>
@@ -3836,7 +4003,7 @@
       <c r="E45" s="22"/>
       <c r="F45" s="14"/>
     </row>
-    <row r="46" spans="1:13" s="12" customFormat="1">
+    <row r="46" spans="1:14" s="12" customFormat="1">
       <c r="A46" s="12" t="s">
         <v>54</v>
       </c>
@@ -3848,7 +4015,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="14"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -3869,8 +4036,11 @@
       <c r="I47" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -3893,8 +4063,11 @@
       <c r="I48" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -3934,8 +4107,11 @@
       <c r="M49" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" s="12" customFormat="1">
+      <c r="N49" s="12" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" s="12" customFormat="1">
       <c r="A50" s="12" t="s">
         <v>54</v>
       </c>
@@ -3946,8 +4122,11 @@
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
       <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="1:13" s="12" customFormat="1">
+      <c r="N50" s="12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="12" customFormat="1">
       <c r="A51" s="12" t="s">
         <v>54</v>
       </c>
@@ -3958,8 +4137,11 @@
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51" s="12" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -3999,8 +4181,11 @@
       <c r="M52" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52" s="12" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -4027,8 +4212,11 @@
       <c r="J53" s="12" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53" s="12" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -4068,8 +4256,11 @@
       <c r="M54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54" s="12" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -4096,8 +4287,11 @@
       <c r="J55" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55" s="12" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4137,8 +4331,11 @@
       <c r="M56" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56" s="12" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -4178,8 +4375,11 @@
       <c r="M57" s="12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -4219,8 +4419,11 @@
       <c r="M58" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58" s="12" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -4260,8 +4463,11 @@
       <c r="M59" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59" s="12" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -4301,8 +4507,11 @@
       <c r="M60" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60" s="12" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -4342,8 +4551,11 @@
       <c r="M61" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61" s="12" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -4365,8 +4577,11 @@
       <c r="J62" s="9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -4401,8 +4616,11 @@
       <c r="M63" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63" s="12" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -4437,8 +4655,11 @@
       <c r="M64" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64" s="12" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -4460,8 +4681,11 @@
       <c r="J65" s="8" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" s="2" customFormat="1">
+      <c r="N65" s="12" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" s="2" customFormat="1">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
@@ -4483,8 +4707,11 @@
       <c r="J66" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" s="2" customFormat="1">
+      <c r="N66" s="12" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" s="2" customFormat="1">
       <c r="A67" s="2" t="s">
         <v>77</v>
       </c>
@@ -4506,8 +4733,11 @@
       <c r="J67" s="7" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" s="2" customFormat="1">
+      <c r="N67" s="12" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
@@ -4543,8 +4773,11 @@
       <c r="M68" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" s="12" customFormat="1">
+      <c r="N68" s="12" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" s="12" customFormat="1">
       <c r="A69" s="12" t="s">
         <v>77</v>
       </c>
@@ -4578,8 +4811,11 @@
       <c r="M69" s="12" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" s="2" customFormat="1">
+      <c r="N69" s="12" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
@@ -4619,8 +4855,11 @@
       <c r="M70" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" s="2" customFormat="1">
+      <c r="N70" s="12" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
@@ -4660,8 +4899,11 @@
       <c r="M71" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" s="2" customFormat="1">
+      <c r="N71" s="12" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -4683,8 +4925,11 @@
       <c r="J72" s="6" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" s="2" customFormat="1">
+      <c r="N72" s="12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
         <v>77</v>
       </c>
@@ -4706,8 +4951,11 @@
       <c r="J73" s="6" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" s="2" customFormat="1">
+      <c r="N73" s="12" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" s="2" customFormat="1">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
@@ -4747,8 +4995,11 @@
       <c r="M74" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" s="2" customFormat="1">
+      <c r="N74" s="12" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" s="2" customFormat="1">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
@@ -4788,8 +5039,11 @@
       <c r="M75" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75" s="12" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
         <v>179</v>
       </c>
@@ -4829,8 +5083,11 @@
       <c r="M76" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76" s="12" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" t="s">
         <v>179</v>
       </c>
@@ -4870,8 +5127,11 @@
       <c r="M77" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" ht="29">
+      <c r="N77" s="12" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="29">
       <c r="A78" s="12" t="s">
         <v>642</v>
       </c>
@@ -4899,7 +5159,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="29">
+    <row r="79" spans="1:14" ht="29">
       <c r="A79" s="12" t="s">
         <v>642</v>
       </c>
@@ -4927,7 +5187,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="29">
+    <row r="80" spans="1:14" ht="29">
       <c r="A80" s="12" t="s">
         <v>642</v>
       </c>

</xml_diff>

<commit_message>
Adding Korean language translations (#847)
* added korean

* translation update

* Increment version number
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjobergd\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828AFEC-6018-4DE0-9D25-2F9325FE801A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37F73A1-A0E1-4A59-ADB4-9C3AB6BB7BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="745">
   <si>
     <t>context</t>
   </si>
@@ -2049,15 +2049,9 @@
     <t>Welch Two Sample t-test</t>
   </si>
   <si>
-    <t>Two Sample t-test</t>
-  </si>
-  <si>
     <t>Kruskal-Wallis rank sum test</t>
   </si>
   <si>
-    <t>Wilcoxon rank sum test with continuity correction</t>
-  </si>
-  <si>
     <t>Wilcoxon rank sum test</t>
   </si>
   <si>
@@ -2191,13 +2185,202 @@
   </si>
   <si>
     <t>Tími</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>결정계수</t>
+  </si>
+  <si>
+    <t>조정 결정 계수</t>
+  </si>
+  <si>
+    <t>p 값</t>
+  </si>
+  <si>
+    <t>로그 가능도 함수</t>
+  </si>
+  <si>
+    <t>통계량</t>
+  </si>
+  <si>
+    <t>잔차 자유도</t>
+  </si>
+  <si>
+    <t>카이제곱 독립성 검정</t>
+  </si>
+  <si>
+    <t>피셔의 정확검정</t>
+  </si>
+  <si>
+    <t>크루스칼-왈리스 검정</t>
+  </si>
+  <si>
+    <t>일원분산분석</t>
+  </si>
+  <si>
+    <t>가설검정</t>
+  </si>
+  <si>
+    <t>t 검정</t>
+  </si>
+  <si>
+    <t>윌콕슨 순위합검정</t>
+  </si>
+  <si>
+    <t>Benjamini &amp; Hochberg 다중비교교정</t>
+  </si>
+  <si>
+    <t>Benjamini &amp; Yekutieli 다중비교교정</t>
+  </si>
+  <si>
+    <t>Bonferroni 다중비교교정</t>
+  </si>
+  <si>
+    <t>False discovery rate 다중비교교정</t>
+  </si>
+  <si>
+    <t>Hochberg 다중비교교정</t>
+  </si>
+  <si>
+    <t>Holm 다중비교교정</t>
+  </si>
+  <si>
+    <t>Hommel 다중비교교정</t>
+  </si>
+  <si>
+    <t>다중비교교정 생략</t>
+  </si>
+  <si>
+    <t>q 값</t>
+  </si>
+  <si>
+    <t>CI = 신뢰구간</t>
+  </si>
+  <si>
+    <t>신뢰구간</t>
+  </si>
+  <si>
+    <t>HR = 위험비</t>
+  </si>
+  <si>
+    <t>IRR = 발생률비</t>
+  </si>
+  <si>
+    <t>OR = 오즈비</t>
+  </si>
+  <si>
+    <t>표준오차</t>
+  </si>
+  <si>
+    <t>% 결측치</t>
+  </si>
+  <si>
+    <t>% 결측치 (비가중)</t>
+  </si>
+  <si>
+    <t>% 비결측치</t>
+  </si>
+  <si>
+    <t>% 비결측치 (비가중)</t>
+  </si>
+  <si>
+    <t>특성</t>
+  </si>
+  <si>
+    <t>사분위 범위</t>
+  </si>
+  <si>
+    <t>최대값</t>
+  </si>
+  <si>
+    <t>평균</t>
+  </si>
+  <si>
+    <t>중앙값</t>
+  </si>
+  <si>
+    <t>최소값</t>
+  </si>
+  <si>
+    <t>N 결측치</t>
+  </si>
+  <si>
+    <t>N 결측치 (비가중)</t>
+  </si>
+  <si>
+    <t>N 비결측치</t>
+  </si>
+  <si>
+    <t>N 비결측치 (비가중)</t>
+  </si>
+  <si>
+    <t>관측 수</t>
+  </si>
+  <si>
+    <t>범위</t>
+  </si>
+  <si>
+    <t>표준편차</t>
+  </si>
+  <si>
+    <t>제시된 통계량</t>
+  </si>
+  <si>
+    <t>총 N</t>
+  </si>
+  <si>
+    <t>총 N (비가중)</t>
+  </si>
+  <si>
+    <t>미지수</t>
+  </si>
+  <si>
+    <t>분산</t>
+  </si>
+  <si>
+    <t>백분위수</t>
+  </si>
+  <si>
+    <t>시간</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 조정된 Wald 독립성 검정</t>
+  </si>
+  <si>
+    <t>설계효과 추정치로 조정한 카이제곱 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 크루스칼-왈리스 순위합 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 중앙값 Mood's 검정</t>
+  </si>
+  <si>
+    <t>안장점 근사를 이용한 복합조사 표본 독립성 검정</t>
+  </si>
+  <si>
+    <t>정확 점근분포를 이용한 복합조사 표본 독립성 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본에 적합한 t 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 van der Waerden's 정규점수 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 Wald 독립성 검정</t>
+  </si>
+  <si>
+    <t>복합조사 표본을 위한 윌콕슨 순위합 검정</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2257,6 +2440,18 @@
       <color rgb="FF222222"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2284,7 +2479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2322,6 +2517,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2636,34 +2833,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
-    <col min="2" max="2" width="51.6328125" customWidth="1"/>
-    <col min="3" max="3" width="49" style="22" customWidth="1"/>
-    <col min="4" max="4" width="47.26953125" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.54296875" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" style="22" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="14" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="49" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="67" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="51" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="52" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57.453125" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="57.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2704,1282 +2902,1374 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>644</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>622</v>
       </c>
       <c r="B2" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="25" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B3" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="12" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>623</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B5" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>624</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B7" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B8" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B9" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
         <v>622</v>
       </c>
       <c r="B10" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="12" t="s">
-        <v>622</v>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="12" t="s">
-        <v>622</v>
+        <v>175</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11" t="s">
+        <v>177</v>
+      </c>
+      <c r="L11" t="s">
+        <v>178</v>
+      </c>
+      <c r="M11" t="s">
+        <v>178</v>
+      </c>
+      <c r="N11" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>639</v>
       </c>
       <c r="B12" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>174</v>
+        <v>638</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" t="s">
+        <v>646</v>
+      </c>
+      <c r="O12" s="26" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="12" t="s">
+        <v>639</v>
       </c>
       <c r="B13" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>307</v>
+        <v>359</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>239</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="L13" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="M13" t="s">
-        <v>178</v>
-      </c>
-      <c r="N13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="25" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B14" t="s">
+        <v>636</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>641</v>
-      </c>
-      <c r="B14" t="s">
-        <v>640</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>407</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>408</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="J14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="O15" s="26" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="12" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="12" t="s">
-        <v>641</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="12" t="s">
-        <v>641</v>
-      </c>
-      <c r="B16" t="s">
-        <v>637</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>413</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="26" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K17" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="M17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>426</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="12" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="12" t="s">
-        <v>641</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="12" t="s">
+      <c r="O18" s="26" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>427</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>429</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="12" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="12" t="s">
-        <v>641</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>421</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J19" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" t="s">
-        <v>46</v>
-      </c>
-      <c r="L19" t="s">
-        <v>47</v>
-      </c>
-      <c r="M19" t="s">
-        <v>48</v>
-      </c>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="26" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>635</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>426</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>268</v>
+        <v>432</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>365</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>213</v>
+        <v>49</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K20" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="M20" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" s="25" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>637</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>429</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>364</v>
+        <v>435</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>366</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L21" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="M21" t="s">
-        <v>10</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="12" t="s">
-        <v>641</v>
+        <v>14</v>
+      </c>
+      <c r="O21" s="25" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>635</v>
+        <v>149</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>365</v>
+        <v>438</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>367</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>49</v>
+        <v>216</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="K22" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="L22" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="M22" t="s">
-        <v>53</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="12" t="s">
-        <v>641</v>
+        <v>153</v>
+      </c>
+      <c r="O22" s="26" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>128</v>
       </c>
       <c r="B23" t="s">
-        <v>638</v>
+        <v>154</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>434</v>
+        <v>439</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>440</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>366</v>
+        <v>441</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>368</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="K23" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="L23" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="M23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>158</v>
+      </c>
+      <c r="O23" s="26" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>437</v>
+        <v>442</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K24" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>148</v>
+      </c>
+      <c r="O24" s="26" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J25" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="L25" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="M25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>163</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J26" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="L26" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="M26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>138</v>
+      </c>
+      <c r="O26" s="26" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="J27" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="K27" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="L27" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="M27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>133</v>
+      </c>
+      <c r="O27" s="26" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="J28" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="K28" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="L28" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="M28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>143</v>
+      </c>
+      <c r="O28" s="25" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J29" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="K29" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="L29" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="M29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>168</v>
+      </c>
+      <c r="O29" s="26" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>455</v>
+        <v>460</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>461</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>373</v>
+        <v>278</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J30" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="K30" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="L30" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="M30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>173</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="O30" s="26" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>458</v>
+        <v>463</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>463</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>325</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G31" s="12"/>
       <c r="H31" s="4" t="s">
-        <v>277</v>
+        <v>205</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J31" t="s">
-        <v>165</v>
-      </c>
-      <c r="K31" t="s">
-        <v>166</v>
-      </c>
-      <c r="L31" t="s">
-        <v>167</v>
-      </c>
-      <c r="M31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J32" t="s">
-        <v>170</v>
-      </c>
-      <c r="K32" t="s">
-        <v>171</v>
-      </c>
-      <c r="L32" t="s">
-        <v>172</v>
-      </c>
-      <c r="M32" t="s">
-        <v>173</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="12" customFormat="1">
+      <c r="A32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="16"/>
       <c r="N32" s="12" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15.5">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>72</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>463</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>463</v>
+        <v>465</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>466</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="G33" s="12"/>
+        <v>467</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="H33" s="4" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>205</v>
+        <v>225</v>
+      </c>
+      <c r="J33" t="s">
+        <v>73</v>
+      </c>
+      <c r="K33" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33" t="s">
+        <v>76</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="12" customFormat="1" ht="15.5">
-      <c r="A34" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="O33" s="26" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>634</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="16"/>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J34" t="s">
+        <v>56</v>
+      </c>
+      <c r="K34" t="s">
+        <v>57</v>
+      </c>
+      <c r="L34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" t="s">
+        <v>59</v>
+      </c>
       <c r="N34" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>654</v>
+      </c>
+      <c r="O34" s="25" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>467</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>327</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="G35" s="12"/>
       <c r="H35" s="4" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J35" t="s">
-        <v>73</v>
-      </c>
-      <c r="K35" t="s">
-        <v>74</v>
-      </c>
-      <c r="L35" t="s">
-        <v>75</v>
-      </c>
-      <c r="M35" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J36" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="K36" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="L36" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="M36" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>655</v>
+      </c>
+      <c r="O36" s="26" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>227</v>
+        <v>64</v>
       </c>
       <c r="J38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L38" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>656</v>
+      </c>
+      <c r="O38" s="26" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="G39" s="12"/>
-      <c r="H39" s="4" t="s">
-        <v>203</v>
-      </c>
+      <c r="H39" s="4"/>
       <c r="I39" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="N39" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>481</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>245</v>
-      </c>
+        <v>487</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J40" t="s">
-        <v>65</v>
-      </c>
-      <c r="K40" t="s">
-        <v>64</v>
-      </c>
-      <c r="L40" t="s">
-        <v>66</v>
-      </c>
-      <c r="M40" t="s">
-        <v>67</v>
-      </c>
-      <c r="N40" s="12" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="12" customFormat="1">
+      <c r="A42" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B42" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>487</v>
-      </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
-      <c r="A43" t="s">
+      <c r="B42" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:15" s="12" customFormat="1">
+      <c r="A43" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B43" t="s">
-        <v>204</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>488</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>489</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>490</v>
-      </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" s="12" customFormat="1">
+      <c r="B43" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" spans="1:15" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
         <v>54</v>
       </c>
@@ -3991,1538 +4281,1543 @@
       <c r="E44" s="22"/>
       <c r="F44" s="14"/>
     </row>
-    <row r="45" spans="1:14" s="12" customFormat="1">
-      <c r="A45" s="12" t="s">
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>644</v>
-      </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="1:14" s="12" customFormat="1">
-      <c r="A46" s="12" t="s">
+      <c r="B45" t="s">
+        <v>200</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="G45" s="12"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>645</v>
-      </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="B46" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="G46" s="12"/>
+      <c r="H46" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="G47" s="12"/>
-      <c r="H47" s="4"/>
+        <v>496</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>200</v>
+        <v>228</v>
+      </c>
+      <c r="J47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" t="s">
+        <v>62</v>
+      </c>
+      <c r="M47" t="s">
+        <v>63</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" t="s">
+        <v>657</v>
+      </c>
+      <c r="O47" s="26" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="12" customFormat="1">
+      <c r="A48" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B48" t="s">
-        <v>199</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="B48" s="12" t="s">
+        <v>632</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="14"/>
       <c r="N48" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="A49" t="s">
+        <v>632</v>
+      </c>
+      <c r="O48" s="25" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="12" customFormat="1">
+      <c r="A49" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>496</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J49" t="s">
-        <v>61</v>
-      </c>
-      <c r="K49" t="s">
-        <v>60</v>
-      </c>
-      <c r="L49" t="s">
-        <v>62</v>
-      </c>
-      <c r="M49" t="s">
-        <v>63</v>
-      </c>
+      <c r="B49" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="14"/>
       <c r="N49" s="12" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J50" t="s">
+        <v>112</v>
+      </c>
+      <c r="K50" t="s">
+        <v>113</v>
+      </c>
+      <c r="L50" t="s">
+        <v>114</v>
+      </c>
+      <c r="M50" t="s">
+        <v>115</v>
+      </c>
+      <c r="N50" s="12" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" s="12" customFormat="1">
-      <c r="A50" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>632</v>
-      </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="14"/>
-      <c r="N50" s="12" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" s="12" customFormat="1">
-      <c r="A51" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>633</v>
-      </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="14"/>
+      <c r="O50" s="26" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="12" t="s">
+        <v>287</v>
+      </c>
       <c r="N51" s="12" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="O51" s="26" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>380</v>
+        <v>505</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>382</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J52" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="K52" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L52" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M52" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="N52" s="12" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="O52" s="26" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>503</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>381</v>
+        <v>508</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="I53" s="1"/>
-      <c r="J53" s="12" t="s">
-        <v>287</v>
+      <c r="J53" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="N53" s="12" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="O53" s="26" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>382</v>
+        <v>511</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>384</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J54" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="K54" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="L54" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="M54" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="N54" s="12" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="O54" s="25" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>507</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G55" s="12"/>
+        <v>513</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>335</v>
+      </c>
       <c r="H55" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I55" s="1"/>
-      <c r="J55" s="11" t="s">
-        <v>288</v>
+        <v>247</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="K55" t="s">
+        <v>109</v>
+      </c>
+      <c r="L55" t="s">
+        <v>110</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>109</v>
+      </c>
+      <c r="O55" s="26" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>384</v>
+        <v>517</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>248</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>285</v>
+        <v>248</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>231</v>
+        <v>99</v>
       </c>
       <c r="J56" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="K56" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="L56" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="M56" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>664</v>
+      </c>
+      <c r="O56" s="25" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>605</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>514</v>
+        <v>519</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>520</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>335</v>
+        <v>385</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>289</v>
+        <v>609</v>
+      </c>
+      <c r="J57" t="s">
+        <v>611</v>
       </c>
       <c r="K57" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="L57" t="s">
-        <v>110</v>
-      </c>
-      <c r="M57" s="12" t="s">
-        <v>109</v>
+        <v>613</v>
+      </c>
+      <c r="M57" t="s">
+        <v>94</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>665</v>
+      </c>
+      <c r="O57" s="25" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>248</v>
+        <v>522</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>386</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J58" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K58" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L58" t="s">
-        <v>99</v>
+        <v>612</v>
       </c>
       <c r="M58" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="N58" s="12" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="O58" s="25" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>605</v>
+        <v>97</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>520</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>385</v>
+        <v>525</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>251</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>609</v>
+        <v>97</v>
       </c>
       <c r="J59" t="s">
-        <v>611</v>
+        <v>98</v>
       </c>
       <c r="K59" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L59" t="s">
-        <v>613</v>
+        <v>97</v>
       </c>
       <c r="M59" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="N59" s="12" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="O59" s="25" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>258</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>523</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J60" t="s">
-        <v>96</v>
-      </c>
-      <c r="K60" t="s">
-        <v>95</v>
-      </c>
-      <c r="L60" t="s">
-        <v>612</v>
-      </c>
-      <c r="M60" t="s">
-        <v>96</v>
+        <v>527</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="G60" s="12"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>251</v>
+        <v>531</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>251</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="H61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="J61" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="K61" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="L61" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="M61" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>668</v>
+      </c>
+      <c r="O61" s="25" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="G62" s="12"/>
+        <v>531</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>340</v>
+      </c>
       <c r="H62" s="4"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="9" t="s">
-        <v>258</v>
+      <c r="I62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J62" t="s">
+        <v>122</v>
+      </c>
+      <c r="K62" t="s">
+        <v>123</v>
+      </c>
+      <c r="L62" t="s">
+        <v>124</v>
+      </c>
+      <c r="M62" t="s">
+        <v>125</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>668</v>
+      </c>
+      <c r="O62" s="25" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>260</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>340</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="G63" s="12"/>
       <c r="H63" s="4"/>
-      <c r="I63" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J63" t="s">
-        <v>122</v>
-      </c>
-      <c r="K63" t="s">
-        <v>123</v>
-      </c>
-      <c r="L63" t="s">
-        <v>124</v>
-      </c>
-      <c r="M63" t="s">
-        <v>125</v>
+      <c r="I63" s="1"/>
+      <c r="J63" s="8" t="s">
+        <v>290</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
-      <c r="A64" t="s">
+        <v>669</v>
+      </c>
+      <c r="O63" s="25" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" s="2" customFormat="1">
+      <c r="A64" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B64" t="s">
-        <v>257</v>
+      <c r="B64" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>340</v>
-      </c>
+        <v>537</v>
+      </c>
+      <c r="F64" s="14"/>
+      <c r="G64" s="12"/>
       <c r="H64" s="4"/>
-      <c r="I64" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J64" t="s">
-        <v>122</v>
-      </c>
-      <c r="K64" t="s">
-        <v>123</v>
-      </c>
-      <c r="L64" t="s">
-        <v>124</v>
-      </c>
-      <c r="M64" t="s">
-        <v>125</v>
+      <c r="J64" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="N64" s="12" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" t="s">
+      <c r="O64" s="26" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="2" customFormat="1">
+      <c r="A65" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B65" t="s">
-        <v>260</v>
+      <c r="B65" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>534</v>
-      </c>
+        <v>540</v>
+      </c>
+      <c r="F65" s="14"/>
       <c r="G65" s="12"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="8" t="s">
-        <v>290</v>
+      <c r="J65" s="7" t="s">
+        <v>292</v>
       </c>
       <c r="N65" s="12" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" s="2" customFormat="1">
+      <c r="O65" s="26" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" s="2" customFormat="1">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>256</v>
+        <v>604</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="F66" s="14"/>
-      <c r="G66" s="12"/>
+      <c r="G66" s="12" t="s">
+        <v>341</v>
+      </c>
       <c r="H66" s="4"/>
-      <c r="J66" s="7" t="s">
-        <v>291</v>
+      <c r="I66" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="N66" s="12" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" s="2" customFormat="1">
-      <c r="A67" s="2" t="s">
+      <c r="O66" s="26" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" s="12" customFormat="1">
+      <c r="A67" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="E67" s="24" t="s">
-        <v>540</v>
-      </c>
-      <c r="F67" s="14"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="4"/>
-      <c r="J67" s="7" t="s">
-        <v>292</v>
+      <c r="B67" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="L67" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="M67" s="12" t="s">
+        <v>621</v>
       </c>
       <c r="N67" s="12" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" s="2" customFormat="1">
+      <c r="O67" s="25" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>604</v>
+        <v>101</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="F68" s="14"/>
+        <v>546</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>387</v>
+      </c>
       <c r="G68" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H68" s="4"/>
+        <v>357</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="I68" s="2" t="s">
-        <v>610</v>
+        <v>101</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>604</v>
+        <v>102</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>604</v>
+        <v>103</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="N68" s="12" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" s="12" customFormat="1">
-      <c r="A69" s="12" t="s">
+      <c r="O68" s="25" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="2" customFormat="1">
+      <c r="A69" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
+      <c r="B69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>549</v>
+      </c>
       <c r="F69" s="14" t="s">
-        <v>615</v>
+        <v>388</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="H69" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="J69" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="K69" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="L69" s="12" t="s">
-        <v>619</v>
-      </c>
-      <c r="M69" s="12" t="s">
-        <v>621</v>
+        <v>342</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="N69" s="12" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" s="2" customFormat="1">
+      <c r="O69" s="26" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>101</v>
+        <v>255</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>104</v>
+        <v>552</v>
+      </c>
+      <c r="F70" s="14"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="4"/>
+      <c r="J70" s="6" t="s">
+        <v>293</v>
       </c>
       <c r="N70" s="12" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" s="2" customFormat="1">
+      <c r="O70" s="25" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>88</v>
+        <v>259</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D71" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="E71" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H71" s="22" t="s">
-        <v>603</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>92</v>
+        <v>553</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="4"/>
+      <c r="J71" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="N71" s="12" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" s="2" customFormat="1">
+      <c r="O71" s="25" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>255</v>
+        <v>83</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="F72" s="14"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="4"/>
-      <c r="J72" s="6" t="s">
-        <v>293</v>
+        <v>557</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="N72" s="12" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" s="2" customFormat="1">
+      <c r="O72" s="26" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>259</v>
+        <v>607</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>554</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>555</v>
-      </c>
-      <c r="F73" s="14"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="4"/>
-      <c r="J73" s="6" t="s">
-        <v>294</v>
+        <v>558</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="N73" s="12" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" s="2" customFormat="1">
-      <c r="A74" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>83</v>
+      <c r="O73" s="25" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="A74" t="s">
+        <v>179</v>
+      </c>
+      <c r="B74" t="s">
+        <v>180</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="F74" s="17" t="s">
-        <v>389</v>
+        <v>563</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>391</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>87</v>
+        <v>254</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J74" t="s">
+        <v>181</v>
+      </c>
+      <c r="K74" t="s">
+        <v>182</v>
+      </c>
+      <c r="L74" t="s">
+        <v>180</v>
+      </c>
+      <c r="M74" t="s">
+        <v>181</v>
       </c>
       <c r="N74" s="12" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" s="2" customFormat="1">
-      <c r="A75" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>607</v>
+      <c r="O74" s="25" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" t="s">
+        <v>183</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>390</v>
+        <v>566</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>284</v>
       </c>
       <c r="G75" s="12" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>108</v>
+        <v>284</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J75" t="s">
+        <v>184</v>
+      </c>
+      <c r="K75" t="s">
+        <v>185</v>
+      </c>
+      <c r="L75" t="s">
+        <v>186</v>
+      </c>
+      <c r="M75" t="s">
+        <v>187</v>
       </c>
       <c r="N75" s="12" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
-      <c r="A76" t="s">
-        <v>179</v>
+      <c r="O75" s="26" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="30">
+      <c r="A76" s="12" t="s">
+        <v>640</v>
       </c>
       <c r="B76" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>391</v>
+        <v>569</v>
+      </c>
+      <c r="F76" s="21" t="s">
+        <v>392</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J76" t="s">
-        <v>181</v>
-      </c>
-      <c r="K76" t="s">
-        <v>182</v>
-      </c>
-      <c r="L76" t="s">
-        <v>180</v>
-      </c>
-      <c r="M76" t="s">
-        <v>181</v>
-      </c>
-      <c r="N76" s="12" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
-      <c r="A77" t="s">
-        <v>179</v>
+        <v>347</v>
+      </c>
+      <c r="H76" s="4"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="O76" s="25" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="30">
+      <c r="A77" s="12" t="s">
+        <v>640</v>
       </c>
       <c r="B77" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="F77" s="16" t="s">
-        <v>284</v>
+        <v>572</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>393</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J77" t="s">
-        <v>184</v>
-      </c>
-      <c r="K77" t="s">
-        <v>185</v>
-      </c>
-      <c r="L77" t="s">
-        <v>186</v>
-      </c>
-      <c r="M77" t="s">
-        <v>187</v>
-      </c>
-      <c r="N77" s="12" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="29">
+        <v>348</v>
+      </c>
+      <c r="H77" s="4"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="O77" s="25" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="30">
       <c r="A78" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="F78" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="G78" s="12" t="s">
-        <v>347</v>
-      </c>
+        <v>575</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G78" s="12"/>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="29">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="30">
       <c r="A79" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="29">
+        <v>298</v>
+      </c>
+      <c r="O79" s="26" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>574</v>
-      </c>
-      <c r="E80" s="22" t="s">
-        <v>575</v>
+        <v>580</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>581</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G80" s="12"/>
+        <v>396</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>350</v>
+      </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="29">
+        <v>299</v>
+      </c>
+      <c r="O80" s="26" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="45">
       <c r="A81" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B81" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
+        <v>300</v>
+      </c>
+      <c r="O81" s="26" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="30">
       <c r="A82" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B82" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>581</v>
+        <v>586</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>587</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="29">
+        <v>301</v>
+      </c>
+      <c r="O82" s="26" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="30">
       <c r="A83" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B83" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="29">
+        <v>302</v>
+      </c>
+      <c r="O83" s="26" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="30">
       <c r="A84" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B84" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>352</v>
+        <v>593</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>354</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="29">
+        <v>303</v>
+      </c>
+      <c r="O84" s="26" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B85" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="29">
+        <v>304</v>
+      </c>
+      <c r="O85" s="26" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="30">
       <c r="A86" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="F86" s="15" t="s">
-        <v>400</v>
-      </c>
-      <c r="G86" s="13" t="s">
-        <v>354</v>
+        <v>599</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>356</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B87" t="s">
-        <v>190</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>594</v>
-      </c>
-      <c r="D87" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="F87" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="H87" s="4"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B88" t="s">
-        <v>195</v>
-      </c>
-      <c r="C88" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="D88" s="22" t="s">
-        <v>598</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="F88" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="G88" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="H88" s="4"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="5" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" s="12" customFormat="1">
-      <c r="A89" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>636</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>430</v>
-      </c>
-      <c r="D89" s="22" t="s">
-        <v>431</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>432</v>
-      </c>
-      <c r="F89" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="G89" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="I89" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J89" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K89" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L89" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="M89" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" s="12" customFormat="1">
-      <c r="A90" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>639</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="D90" s="22" t="s">
-        <v>434</v>
-      </c>
-      <c r="E90" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="G90" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H90" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="I90" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="J90" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K90" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L90" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="M90" s="12" t="s">
-        <v>14</v>
+      <c r="O86" s="26" t="s">
+        <v>744</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M90" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M88">
-      <sortCondition ref="A1:A88"/>
+  <autoFilter ref="A1:M86" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M86">
+      <sortCondition ref="A1:A86"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
French translation update (#1038)
* French translation update

* increment version number

Co-authored-by: Sjoberg <SjobergD@mskcc.org>
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24718"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37F73A1-A0E1-4A59-ADB4-9C3AB6BB7BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A8BE5D-2390-473B-A0AF-BAB166FE6F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="774">
   <si>
     <t>context</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>CI = Konfidenzintervall</t>
-  </si>
-  <si>
-    <t>CI = intervalle de confiance</t>
   </si>
   <si>
     <t>CI = Intervalo de confiança</t>
@@ -2374,6 +2371,96 @@
   </si>
   <si>
     <t>복합조사 표본을 위한 윌콕슨 순위합 검정</t>
+  </si>
+  <si>
+    <t>R\U00B2 ajusté</t>
+  </si>
+  <si>
+    <t>log-vraisemblance</t>
+  </si>
+  <si>
+    <t>degrés de liberté des résidus</t>
+  </si>
+  <si>
+    <t>déviance nulle</t>
+  </si>
+  <si>
+    <t>Nombre d'événements</t>
+  </si>
+  <si>
+    <t>degrés de liberté du modèle nul</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>IC = intervalle de confiance</t>
+  </si>
+  <si>
+    <t>RR = risque relatif</t>
+  </si>
+  <si>
+    <t>ET = écart-type</t>
+  </si>
+  <si>
+    <t>% manquant (non pondéré)</t>
+  </si>
+  <si>
+    <t>% non manquant (non pondéré)</t>
+  </si>
+  <si>
+    <t>N manquant (non pondéré)</t>
+  </si>
+  <si>
+    <t>N non manquant</t>
+  </si>
+  <si>
+    <t>Nombre d'observations</t>
+  </si>
+  <si>
+    <t>N non manquant (non pondéré)</t>
+  </si>
+  <si>
+    <t>N total</t>
+  </si>
+  <si>
+    <t>N total (non pondéré)</t>
+  </si>
+  <si>
+    <t>test d'indépendance de Wald ajusté pour les plans d'échantillonnage complexes</t>
+  </si>
+  <si>
+    <t>test du Chi² ajusté selon une estimation de l'effet du plan d'échantillonnage</t>
+  </si>
+  <si>
+    <t>test du Chi² avec la correction du second ordre de Rao &amp; Scott</t>
+  </si>
+  <si>
+    <t>test de Kruskal-Wallis avec prise en compte du plan d'échantillonnage</t>
+  </si>
+  <si>
+    <t>test des médianes de Mood  avec prise en compte du plan d'échantillonnage</t>
+  </si>
+  <si>
+    <t>test d'indépendance selon la méthode du point de col (saddlepoint approximation) pour la prise en compte du plan d'échantillonnage</t>
+  </si>
+  <si>
+    <t>test d'indépendance utilisant la distribution asymptotique exacte pour la prise en compte du plan d'échantillonnage</t>
+  </si>
+  <si>
+    <t>test t adapté aux plans d'échantillonnage complexes</t>
+  </si>
+  <si>
+    <t>test d'indépendance de Wald adapté aux plans d'échantillonnage complexes</t>
+  </si>
+  <si>
+    <t>test de Wilcoxon sur la somme des rangs adapté aux plans d'échantillonnage complexes</t>
+  </si>
+  <si>
+    <t>test de van der Waerden adapté aux plans d'échantillonnage complexes</t>
+  </si>
+  <si>
+    <t>ET des c-index</t>
   </si>
 </sst>
 </file>
@@ -2537,7 +2624,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2836,29 +2923,29 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="49" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="67" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="51" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="52" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57.42578125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="58.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="51.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49" style="22" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.5546875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="49" customWidth="1"/>
+    <col min="10" max="10" width="67" customWidth="1"/>
+    <col min="11" max="11" width="51" customWidth="1"/>
+    <col min="12" max="12" width="52" customWidth="1"/>
+    <col min="13" max="13" width="52.6640625" customWidth="1"/>
+    <col min="14" max="14" width="57.44140625" customWidth="1"/>
+    <col min="15" max="15" width="58.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2869,25 +2956,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="22" t="s">
         <v>601</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>602</v>
-      </c>
       <c r="F1" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -2902,165 +2989,186 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B3" t="s">
-        <v>631</v>
+        <v>630</v>
+      </c>
+      <c r="L3" t="s">
+        <v>744</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="B4" t="s">
         <v>622</v>
       </c>
-      <c r="B4" t="s">
-        <v>623</v>
+      <c r="L4" t="s">
+        <v>745</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B5" t="s">
-        <v>624</v>
+        <v>623</v>
+      </c>
+      <c r="L5" t="s">
+        <v>746</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B6" t="s">
-        <v>625</v>
+        <v>624</v>
+      </c>
+      <c r="L6" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B7" t="s">
-        <v>626</v>
+        <v>625</v>
+      </c>
+      <c r="L7" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B8" t="s">
-        <v>627</v>
+        <v>626</v>
+      </c>
+      <c r="L8" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B10" t="s">
-        <v>629</v>
+        <v>628</v>
+      </c>
+      <c r="L10" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" t="s">
         <v>174</v>
       </c>
-      <c r="B11" t="s">
-        <v>175</v>
-      </c>
       <c r="C11" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>404</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>406</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" t="s">
         <v>176</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>177</v>
       </c>
-      <c r="L11" t="s">
-        <v>178</v>
-      </c>
       <c r="M11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="E12" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>409</v>
-      </c>
       <c r="F12" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
@@ -3075,39 +3183,39 @@
         <v>18</v>
       </c>
       <c r="N12" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>410</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>412</v>
-      </c>
       <c r="F13" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J13" t="s">
         <v>20</v>
@@ -3122,33 +3230,33 @@
         <v>23</v>
       </c>
       <c r="O13" s="25" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>414</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>415</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>39</v>
@@ -3166,36 +3274,36 @@
         <v>43</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>416</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>417</v>
-      </c>
       <c r="F15" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J15" t="s">
         <v>35</v>
@@ -3210,39 +3318,39 @@
         <v>38</v>
       </c>
       <c r="N15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="E16" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>420</v>
-      </c>
       <c r="F16" s="16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J16" t="s">
         <v>30</v>
@@ -3257,39 +3365,39 @@
         <v>33</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>421</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="E17" s="22" t="s">
         <v>422</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>423</v>
-      </c>
       <c r="F17" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J17" t="s">
         <v>45</v>
@@ -3307,31 +3415,31 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="E18" s="22" t="s">
         <v>425</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>426</v>
-      </c>
       <c r="F18" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J18" t="s">
         <v>25</v>
@@ -3346,39 +3454,39 @@
         <v>28</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="22" t="s">
+        <v>426</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>427</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="E19" s="22" t="s">
         <v>428</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>429</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
@@ -3393,36 +3501,36 @@
         <v>10</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B20" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C20" s="22" t="s">
+        <v>429</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>431</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>432</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>49</v>
@@ -3440,39 +3548,39 @@
         <v>53</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>435</v>
-      </c>
       <c r="F21" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -3487,454 +3595,457 @@
         <v>14</v>
       </c>
       <c r="O21" s="25" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J22" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>150</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>151</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>152</v>
       </c>
-      <c r="M22" t="s">
-        <v>153</v>
-      </c>
       <c r="O22" s="26" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J23" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>155</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>156</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>157</v>
       </c>
-      <c r="M23" t="s">
-        <v>158</v>
-      </c>
       <c r="O23" s="26" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>443</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J24" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>442</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>444</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>145</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>146</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>147</v>
       </c>
-      <c r="M24" t="s">
-        <v>148</v>
-      </c>
       <c r="O24" s="26" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J25" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>160</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>161</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>162</v>
       </c>
-      <c r="M25" t="s">
-        <v>163</v>
-      </c>
       <c r="O25" s="26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J26" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>448</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>450</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>135</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>136</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>137</v>
       </c>
-      <c r="M26" t="s">
-        <v>138</v>
-      </c>
       <c r="O26" s="26" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
         <v>128</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J27" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>451</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>452</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>453</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>130</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>131</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>132</v>
       </c>
-      <c r="M27" t="s">
-        <v>133</v>
-      </c>
       <c r="O27" s="26" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>453</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J28" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>456</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>140</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>141</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>142</v>
       </c>
-      <c r="M28" t="s">
-        <v>143</v>
-      </c>
       <c r="O28" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>456</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J29" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>165</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>166</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>167</v>
       </c>
-      <c r="M29" t="s">
-        <v>168</v>
-      </c>
       <c r="O29" s="26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J30" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>170</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>171</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>172</v>
       </c>
-      <c r="M30" t="s">
-        <v>173</v>
-      </c>
       <c r="N30" s="12" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15">
       <c r="A31" t="s">
         <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>463</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>464</v>
-      </c>
       <c r="F31" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="12" customFormat="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="12" customFormat="1" ht="15">
       <c r="A32" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
       <c r="F32" s="16"/>
+      <c r="L32" s="12" t="s">
+        <v>750</v>
+      </c>
       <c r="N32" s="12" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -3945,25 +4056,25 @@
         <v>72</v>
       </c>
       <c r="C33" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="D33" s="22" t="s">
         <v>465</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="E33" s="22" t="s">
         <v>466</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>467</v>
-      </c>
       <c r="F33" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J33" t="s">
         <v>73</v>
@@ -3972,16 +4083,16 @@
         <v>74</v>
       </c>
       <c r="L33" t="s">
+        <v>751</v>
+      </c>
+      <c r="M33" t="s">
         <v>75</v>
       </c>
-      <c r="M33" t="s">
-        <v>76</v>
-      </c>
       <c r="N33" s="12" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -3992,25 +4103,25 @@
         <v>55</v>
       </c>
       <c r="C34" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="D34" s="22" t="s">
         <v>468</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="E34" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>470</v>
-      </c>
       <c r="F34" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J34" t="s">
         <v>56</v>
@@ -4025,10 +4136,10 @@
         <v>59</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -4036,26 +4147,26 @@
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C35" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>471</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>472</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -4066,25 +4177,25 @@
         <v>68</v>
       </c>
       <c r="C36" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="D36" s="22" t="s">
         <v>473</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="E36" s="22" t="s">
         <v>474</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>475</v>
-      </c>
       <c r="F36" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J36" t="s">
         <v>69</v>
@@ -4099,10 +4210,10 @@
         <v>71</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O36" s="26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -4110,26 +4221,26 @@
         <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>476</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="E37" s="22" t="s">
         <v>477</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>478</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -4140,22 +4251,22 @@
         <v>64</v>
       </c>
       <c r="C38" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>479</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="E38" s="22" t="s">
         <v>480</v>
       </c>
-      <c r="E38" s="22" t="s">
-        <v>481</v>
-      </c>
       <c r="F38" s="16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>64</v>
@@ -4173,10 +4284,10 @@
         <v>67</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="O38" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -4184,21 +4295,21 @@
         <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C39" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>482</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="22" t="s">
         <v>483</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>484</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="4"/>
       <c r="I39" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -4206,21 +4317,21 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C40" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>485</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="E40" s="22" t="s">
         <v>486</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>487</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="4"/>
       <c r="I40" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -4228,21 +4339,21 @@
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C41" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="E41" s="22" t="s">
         <v>489</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>490</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="12" customFormat="1">
@@ -4250,7 +4361,7 @@
         <v>54</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -4262,7 +4373,7 @@
         <v>54</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -4274,36 +4385,39 @@
         <v>54</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="14"/>
+      <c r="L44" s="12" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C45" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>492</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>493</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -4311,26 +4425,26 @@
         <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C46" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>494</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>495</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -4341,25 +4455,25 @@
         <v>60</v>
       </c>
       <c r="C47" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="D47" s="24" t="s">
         <v>496</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="E47" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="E47" s="24" t="s">
-        <v>498</v>
-      </c>
       <c r="F47" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J47" t="s">
         <v>61</v>
@@ -4374,10 +4488,10 @@
         <v>63</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O47" s="26" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="48" spans="1:15" s="12" customFormat="1">
@@ -4385,17 +4499,20 @@
         <v>54</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="14"/>
+      <c r="L48" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="N48" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="12" customFormat="1">
@@ -4403,1415 +4520,1472 @@
         <v>54</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
       <c r="F49" s="14"/>
+      <c r="L49" s="12" t="s">
+        <v>753</v>
+      </c>
       <c r="N49" s="12" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J50" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>112</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>113</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>114</v>
       </c>
-      <c r="M50" t="s">
-        <v>115</v>
-      </c>
       <c r="N50" s="12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O50" s="26" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C51" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="D51" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="E51" s="24" t="s">
         <v>502</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>503</v>
-      </c>
       <c r="F51" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="L51" t="s">
+        <v>754</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O51" s="26" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>117</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>118</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>119</v>
       </c>
-      <c r="M52" t="s">
-        <v>120</v>
-      </c>
       <c r="N52" s="12" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O52" s="26" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>506</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="24" t="s">
         <v>507</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>508</v>
-      </c>
       <c r="F53" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
+      </c>
+      <c r="L53" t="s">
+        <v>755</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="O53" s="26" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" t="s">
         <v>77</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J54" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>79</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>80</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>81</v>
       </c>
-      <c r="M54" t="s">
-        <v>82</v>
-      </c>
       <c r="N54" s="12" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O54" s="25" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="K55" t="s">
+        <v>108</v>
+      </c>
+      <c r="L55" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>512</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="K55" t="s">
-        <v>109</v>
-      </c>
-      <c r="L55" t="s">
-        <v>110</v>
-      </c>
       <c r="M55" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O55" s="26" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J56" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="I56" s="1" t="s">
+      <c r="K56" t="s">
+        <v>98</v>
+      </c>
+      <c r="L56" t="s">
+        <v>98</v>
+      </c>
+      <c r="M56" t="s">
         <v>99</v>
       </c>
-      <c r="J56" t="s">
-        <v>100</v>
-      </c>
-      <c r="K56" t="s">
-        <v>99</v>
-      </c>
-      <c r="L56" t="s">
-        <v>99</v>
-      </c>
-      <c r="M56" t="s">
-        <v>100</v>
-      </c>
       <c r="N56" s="12" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="O56" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C57" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="E57" s="24" t="s">
         <v>519</v>
       </c>
-      <c r="E57" s="24" t="s">
-        <v>520</v>
-      </c>
       <c r="F57" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J57" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K57" t="s">
+        <v>92</v>
+      </c>
+      <c r="L57" t="s">
+        <v>612</v>
+      </c>
+      <c r="M57" t="s">
         <v>93</v>
       </c>
-      <c r="L57" t="s">
-        <v>613</v>
-      </c>
-      <c r="M57" t="s">
-        <v>94</v>
-      </c>
       <c r="N57" s="12" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O57" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J58" t="s">
         <v>95</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>523</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I58" s="1" t="s">
+      <c r="K58" t="s">
+        <v>94</v>
+      </c>
+      <c r="L58" t="s">
+        <v>611</v>
+      </c>
+      <c r="M58" t="s">
         <v>95</v>
       </c>
-      <c r="J58" t="s">
-        <v>96</v>
-      </c>
-      <c r="K58" t="s">
-        <v>95</v>
-      </c>
-      <c r="L58" t="s">
-        <v>612</v>
-      </c>
-      <c r="M58" t="s">
-        <v>96</v>
-      </c>
       <c r="N58" s="12" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="O58" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J59" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>524</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I59" s="1" t="s">
+      <c r="K59" t="s">
+        <v>96</v>
+      </c>
+      <c r="L59" t="s">
+        <v>96</v>
+      </c>
+      <c r="M59" t="s">
         <v>97</v>
       </c>
-      <c r="J59" t="s">
-        <v>98</v>
-      </c>
-      <c r="K59" t="s">
-        <v>97</v>
-      </c>
-      <c r="L59" t="s">
-        <v>97</v>
-      </c>
-      <c r="M59" t="s">
-        <v>98</v>
-      </c>
       <c r="N59" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O59" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C60" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>527</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>527</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>528</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="4"/>
       <c r="I60" s="1"/>
       <c r="J60" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C61" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="E61" s="22" t="s">
         <v>530</v>
       </c>
-      <c r="E61" s="22" t="s">
-        <v>531</v>
-      </c>
       <c r="G61" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J61" t="s">
+        <v>121</v>
+      </c>
+      <c r="K61" t="s">
         <v>122</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>123</v>
       </c>
-      <c r="L61" t="s">
+      <c r="M61" t="s">
         <v>124</v>
       </c>
-      <c r="M61" t="s">
-        <v>125</v>
-      </c>
       <c r="N61" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O61" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C62" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="E62" s="22" t="s">
         <v>530</v>
       </c>
-      <c r="E62" s="22" t="s">
-        <v>531</v>
-      </c>
       <c r="G62" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J62" t="s">
+        <v>121</v>
+      </c>
+      <c r="K62" t="s">
         <v>122</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>123</v>
       </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>124</v>
       </c>
-      <c r="M62" t="s">
-        <v>125</v>
-      </c>
       <c r="N62" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O62" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C63" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="D63" s="22" t="s">
         <v>532</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="E63" s="24" t="s">
         <v>533</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>534</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
+      </c>
+      <c r="L63" t="s">
+        <v>756</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O63" s="25" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1">
       <c r="A64" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C64" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>535</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="E64" s="22" t="s">
         <v>536</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>537</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="12"/>
       <c r="H64" s="4"/>
       <c r="J64" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>757</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O64" s="26" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1">
       <c r="A65" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C65" s="22" t="s">
+        <v>537</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="E65" s="24" t="s">
         <v>539</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>540</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="12"/>
       <c r="H65" s="4"/>
       <c r="J65" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>759</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O65" s="26" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="66" spans="1:15" s="2" customFormat="1">
       <c r="A66" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="D66" s="22" t="s">
         <v>541</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="E66" s="22" t="s">
         <v>542</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>543</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="K66" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="M66" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L66" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="M66" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="N66" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O66" s="26" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="12" customFormat="1">
       <c r="A67" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
       <c r="F67" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>613</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="K67" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="I67" s="12" t="s">
+      <c r="L67" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="J67" s="12" t="s">
+      <c r="M67" s="12" t="s">
         <v>620</v>
       </c>
-      <c r="K67" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="L67" s="12" t="s">
-        <v>619</v>
-      </c>
-      <c r="M67" s="12" t="s">
-        <v>621</v>
-      </c>
       <c r="N67" s="12" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O67" s="25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="K68" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="M68" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="N68" s="12" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O68" s="25" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1">
       <c r="A69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>603</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J69" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="M69" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M69" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="N69" s="12" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="O69" s="26" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="70" spans="1:15" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C70" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="D70" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="E70" s="22" t="s">
         <v>551</v>
-      </c>
-      <c r="E70" s="22" t="s">
-        <v>552</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="12"/>
       <c r="H70" s="4"/>
       <c r="J70" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>760</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O70" s="25" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C71" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="E71" s="24" t="s">
         <v>554</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>555</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="12"/>
       <c r="H71" s="4"/>
       <c r="J71" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>761</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O71" s="25" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J72" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>389</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J72" s="2" t="s">
+      <c r="K72" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="M72" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M72" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="N72" s="12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O72" s="26" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C73" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="D73" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="E73" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="E73" s="22" t="s">
-        <v>560</v>
-      </c>
       <c r="F73" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K73" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M73" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="N73" s="12" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="O73" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="74" spans="1:15">
       <c r="A74" t="s">
+        <v>178</v>
+      </c>
+      <c r="B74" t="s">
         <v>179</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C74" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="E74" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="F74" s="20" t="s">
-        <v>391</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" t="s">
+        <v>180</v>
+      </c>
+      <c r="K74" t="s">
         <v>181</v>
       </c>
-      <c r="J74" t="s">
-        <v>181</v>
-      </c>
-      <c r="K74" t="s">
-        <v>182</v>
-      </c>
       <c r="L74" t="s">
+        <v>179</v>
+      </c>
+      <c r="M74" t="s">
         <v>180</v>
       </c>
-      <c r="M74" t="s">
-        <v>181</v>
-      </c>
       <c r="N74" s="12" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="O74" s="25" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="75" spans="1:15">
       <c r="A75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B75" t="s">
+        <v>182</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J75" t="s">
         <v>183</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="E75" s="22" t="s">
+      <c r="K75" t="s">
+        <v>184</v>
+      </c>
+      <c r="L75" t="s">
+        <v>185</v>
+      </c>
+      <c r="M75" t="s">
+        <v>186</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>680</v>
+      </c>
+      <c r="O75" s="26" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="28.8">
+      <c r="A76" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B76" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="F75" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="G75" s="12" t="s">
+      <c r="D76" s="22" t="s">
+        <v>567</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="F76" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="G76" s="12" t="s">
         <v>346</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J75" t="s">
-        <v>184</v>
-      </c>
-      <c r="K75" t="s">
-        <v>185</v>
-      </c>
-      <c r="L75" t="s">
-        <v>186</v>
-      </c>
-      <c r="M75" t="s">
-        <v>187</v>
-      </c>
-      <c r="N75" s="12" t="s">
-        <v>681</v>
-      </c>
-      <c r="O75" s="26" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="30">
-      <c r="A76" s="12" t="s">
-        <v>640</v>
-      </c>
-      <c r="B76" t="s">
-        <v>191</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="F76" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>347</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="1"/>
       <c r="J76" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="L76" t="s">
+        <v>762</v>
       </c>
       <c r="O76" s="25" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="30">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="28.8">
       <c r="A77" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C77" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>571</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>572</v>
-      </c>
       <c r="F77" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="1"/>
       <c r="J77" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="L77" t="s">
+        <v>763</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="30">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="28.8">
       <c r="A78" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C78" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="D78" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="E78" s="22" t="s">
-        <v>575</v>
-      </c>
       <c r="F78" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="30">
+        <v>296</v>
+      </c>
+      <c r="L78" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="28.8">
       <c r="A79" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C79" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="E79" s="22" t="s">
         <v>577</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>578</v>
-      </c>
       <c r="F79" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="L79" t="s">
+        <v>765</v>
       </c>
       <c r="O79" s="26" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="80" spans="1:15">
       <c r="A80" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C80" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>579</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="E80" s="24" t="s">
         <v>580</v>
       </c>
-      <c r="E80" s="24" t="s">
-        <v>581</v>
-      </c>
       <c r="F80" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
+      </c>
+      <c r="L80" t="s">
+        <v>766</v>
       </c>
       <c r="O80" s="26" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="45">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="28.8">
       <c r="A81" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C81" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="E81" s="22" t="s">
-        <v>584</v>
-      </c>
       <c r="F81" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
+      </c>
+      <c r="L81" t="s">
+        <v>767</v>
       </c>
       <c r="O81" s="26" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="30">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="28.8">
       <c r="A82" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="D82" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>586</v>
       </c>
-      <c r="E82" s="22" t="s">
-        <v>587</v>
-      </c>
       <c r="F82" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
+      </c>
+      <c r="L82" t="s">
+        <v>768</v>
       </c>
       <c r="O82" s="26" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="30">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="28.8">
       <c r="A83" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="D83" s="22" t="s">
+      <c r="E83" s="22" t="s">
         <v>589</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>590</v>
-      </c>
       <c r="F83" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="L83" t="s">
+        <v>769</v>
       </c>
       <c r="O83" s="26" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="30">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="28.8">
       <c r="A84" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C84" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="D84" s="22" t="s">
         <v>591</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="E84" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>593</v>
-      </c>
       <c r="F84" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
+      </c>
+      <c r="L84" t="s">
+        <v>772</v>
       </c>
       <c r="O84" s="26" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="85" spans="1:15">
       <c r="A85" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B85" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C85" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="D85" s="22" t="s">
+      <c r="E85" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>596</v>
-      </c>
       <c r="F85" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="L85" s="12" t="s">
+        <v>770</v>
       </c>
       <c r="O85" s="26" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="30">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C86" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="D86" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="D86" s="22" t="s">
+      <c r="E86" s="22" t="s">
         <v>598</v>
       </c>
-      <c r="E86" s="22" t="s">
-        <v>599</v>
-      </c>
       <c r="F86" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
+      </c>
+      <c r="L86" s="12" t="s">
+        <v>771</v>
       </c>
       <c r="O86" s="26" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding `digits=` argument to `tbl_cross()` (#1048)
* added digits arg to tbl_cross

* Update tbl_summary.R

* doc updates

* formalizing sum statistic
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24718"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A8BE5D-2390-473B-A0AF-BAB166FE6F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819FD20-9835-4ACC-9E96-56EA5506E64C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="782">
   <si>
     <t>context</t>
   </si>
@@ -2461,6 +2461,30 @@
   </si>
   <si>
     <t>ET des c-index</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Summa</t>
+  </si>
+  <si>
+    <t>합집합</t>
+  </si>
+  <si>
+    <t>和</t>
+  </si>
+  <si>
+    <t>Suma</t>
   </si>
 </sst>
 </file>
@@ -2624,7 +2648,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2920,16 +2944,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="51.5546875" customWidth="1"/>
@@ -5367,36 +5391,45 @@
         <v>727</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="2" customFormat="1">
-      <c r="A70" s="2" t="s">
+    <row r="70" spans="1:15" s="12" customFormat="1">
+      <c r="A70" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C70" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="D70" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="E70" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="4"/>
-      <c r="J70" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>760</v>
+      <c r="B70" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="14" t="s">
+        <v>780</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>780</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>780</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>778</v>
+      </c>
+      <c r="J70" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="K70" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="L70" s="12" t="s">
+        <v>776</v>
+      </c>
+      <c r="M70" s="12" t="s">
+        <v>777</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>675</v>
-      </c>
-      <c r="O70" s="25" t="s">
-        <v>728</v>
+        <v>778</v>
+      </c>
+      <c r="O70" s="14" t="s">
+        <v>779</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1">
@@ -5404,31 +5437,31 @@
         <v>76</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>553</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>554</v>
+        <v>549</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>551</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="12"/>
       <c r="H71" s="4"/>
       <c r="J71" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O71" s="25" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1">
@@ -5436,46 +5469,31 @@
         <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>82</v>
+        <v>258</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>84</v>
+        <v>552</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="4"/>
+      <c r="J72" s="6" t="s">
+        <v>293</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>86</v>
+        <v>761</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>677</v>
-      </c>
-      <c r="O72" s="26" t="s">
-        <v>730</v>
+        <v>676</v>
+      </c>
+      <c r="O72" s="25" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1">
@@ -5483,93 +5501,93 @@
         <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="O73" s="26" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="C73" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F74" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="G73" s="12" t="s">
+      <c r="G74" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H74" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="M74" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N73" s="12" t="s">
+      <c r="N74" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="O73" s="25" t="s">
+      <c r="O74" s="25" t="s">
         <v>731</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15">
-      <c r="A74" t="s">
-        <v>178</v>
-      </c>
-      <c r="B74" t="s">
-        <v>179</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="E74" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="F74" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J74" t="s">
-        <v>180</v>
-      </c>
-      <c r="K74" t="s">
-        <v>181</v>
-      </c>
-      <c r="L74" t="s">
-        <v>179</v>
-      </c>
-      <c r="M74" t="s">
-        <v>180</v>
-      </c>
-      <c r="N74" s="12" t="s">
-        <v>679</v>
-      </c>
-      <c r="O74" s="25" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -5577,80 +5595,93 @@
         <v>178</v>
       </c>
       <c r="B75" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J75" t="s">
+        <v>180</v>
+      </c>
+      <c r="K75" t="s">
+        <v>181</v>
+      </c>
+      <c r="L75" t="s">
+        <v>179</v>
+      </c>
+      <c r="M75" t="s">
+        <v>180</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>679</v>
+      </c>
+      <c r="O75" s="25" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="A76" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" t="s">
         <v>182</v>
       </c>
-      <c r="C75" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D76" s="22" t="s">
         <v>564</v>
       </c>
-      <c r="E75" s="22" t="s">
+      <c r="E76" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="F75" s="16" t="s">
+      <c r="F76" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="G75" s="12" t="s">
+      <c r="G76" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="H76" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J76" t="s">
         <v>183</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K76" t="s">
         <v>184</v>
       </c>
-      <c r="L75" t="s">
+      <c r="L76" t="s">
         <v>185</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M76" t="s">
         <v>186</v>
       </c>
-      <c r="N75" s="12" t="s">
+      <c r="N76" s="12" t="s">
         <v>680</v>
       </c>
-      <c r="O75" s="26" t="s">
+      <c r="O76" s="26" t="s">
         <v>733</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="28.8">
-      <c r="A76" s="12" t="s">
-        <v>639</v>
-      </c>
-      <c r="B76" t="s">
-        <v>190</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="F76" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="H76" s="4"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L76" t="s">
-        <v>762</v>
-      </c>
-      <c r="O76" s="25" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="28.8">
@@ -5658,33 +5689,33 @@
         <v>639</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>392</v>
+        <v>568</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>391</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="1"/>
       <c r="J77" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L77" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="28.8">
@@ -5692,28 +5723,33 @@
         <v>639</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="G78" s="12"/>
+        <v>392</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>347</v>
+      </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L78" t="s">
-        <v>764</v>
+        <v>763</v>
+      </c>
+      <c r="O78" s="25" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="28.8">
@@ -5721,101 +5757,96 @@
         <v>639</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G79" s="12" t="s">
-        <v>348</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="G79" s="12"/>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L79" t="s">
-        <v>765</v>
-      </c>
-      <c r="O79" s="26" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="28.8">
       <c r="A80" s="12" t="s">
         <v>639</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>580</v>
+        <v>576</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>577</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L80" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="O80" s="26" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="28.8">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="12" t="s">
         <v>639</v>
       </c>
       <c r="B81" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>583</v>
+        <v>579</v>
+      </c>
+      <c r="E81" s="24" t="s">
+        <v>580</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L81" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O81" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="28.8">
@@ -5823,33 +5854,33 @@
         <v>639</v>
       </c>
       <c r="B82" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L82" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="O82" s="26" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="28.8">
@@ -5857,33 +5888,33 @@
         <v>639</v>
       </c>
       <c r="B83" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L83" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="O83" s="26" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="28.8">
@@ -5891,67 +5922,67 @@
         <v>639</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>592</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>399</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>353</v>
+        <v>589</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>352</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L84" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="O84" s="26" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="28.8">
       <c r="A85" s="12" t="s">
         <v>639</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="F85" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>354</v>
+        <v>592</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>353</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="L85" s="12" t="s">
-        <v>770</v>
+        <v>302</v>
+      </c>
+      <c r="L85" t="s">
+        <v>772</v>
       </c>
       <c r="O85" s="26" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="86" spans="1:15">
@@ -5959,39 +5990,73 @@
         <v>639</v>
       </c>
       <c r="B86" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="L86" s="12" t="s">
+        <v>770</v>
+      </c>
+      <c r="O86" s="26" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="L86" s="12" t="s">
+      <c r="L87" s="12" t="s">
         <v>771</v>
       </c>
-      <c r="O86" s="26" t="s">
+      <c r="O87" s="26" t="s">
         <v>743</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M86" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M86">
-      <sortCondition ref="A1:A86"/>
+  <autoFilter ref="A1:M87" xr:uid="{B57C1AF0-F1B7-4296-BDC4-6CF4510928DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M87">
+      <sortCondition ref="A1:A87"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
translation update for ES Wilcoxon Rank sum test
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819FD20-9835-4ACC-9E96-56EA5506E64C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A692F8-DDF0-45D4-9930-EC1E2C7388B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Testes estatísticos realizados</t>
   </si>
   <si>
-    <t>prueba de los rangos con signo de Wilcoxon</t>
-  </si>
-  <si>
     <t>Wilcoxon-Mann-Whitney-Test</t>
   </si>
   <si>
@@ -2485,6 +2482,9 @@
   </si>
   <si>
     <t>Suma</t>
+  </si>
+  <si>
+    <t>Prueba de la suma de rangos de Wilcoxon</t>
   </si>
 </sst>
 </file>
@@ -2946,11 +2946,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2980,25 +2980,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>601</v>
-      </c>
       <c r="F1" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -3013,504 +3013,504 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B4" t="s">
         <v>621</v>
       </c>
-      <c r="B4" t="s">
-        <v>622</v>
-      </c>
       <c r="L4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B9" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L10" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" t="s">
         <v>173</v>
       </c>
-      <c r="B11" t="s">
-        <v>174</v>
-      </c>
       <c r="C11" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>403</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="22" t="s">
         <v>404</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>405</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
+        <v>174</v>
+      </c>
+      <c r="K11" t="s">
         <v>175</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>176</v>
       </c>
-      <c r="L11" t="s">
-        <v>177</v>
-      </c>
       <c r="M11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>406</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="E12" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>408</v>
-      </c>
       <c r="F12" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>16</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
-        <v>18</v>
-      </c>
       <c r="N12" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>21</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
       <c r="O13" s="25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>414</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
         <v>39</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>40</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>41</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>42</v>
       </c>
-      <c r="M14" t="s">
-        <v>43</v>
-      </c>
       <c r="O14" s="25" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>35</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>36</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>37</v>
       </c>
-      <c r="M15" t="s">
-        <v>38</v>
-      </c>
       <c r="N15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>30</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>31</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>32</v>
       </c>
-      <c r="M16" t="s">
-        <v>33</v>
-      </c>
       <c r="N16" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>421</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>45</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>46</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>47</v>
-      </c>
-      <c r="M17" t="s">
-        <v>48</v>
       </c>
       <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>25</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>26</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>27</v>
       </c>
-      <c r="M18" t="s">
-        <v>28</v>
-      </c>
       <c r="N18" s="12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="E19" s="22" t="s">
         <v>427</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>428</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
@@ -3525,867 +3525,867 @@
         <v>10</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C20" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>431</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
         <v>49</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>50</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>51</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>52</v>
       </c>
-      <c r="M20" t="s">
-        <v>53</v>
-      </c>
       <c r="N20" s="12" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>434</v>
-      </c>
       <c r="F21" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J21" t="s">
+        <v>781</v>
+      </c>
+      <c r="K21" t="s">
         <v>11</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>12</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>13</v>
       </c>
-      <c r="M21" t="s">
-        <v>14</v>
-      </c>
       <c r="O21" s="25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J22" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>149</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>150</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>151</v>
       </c>
-      <c r="M22" t="s">
-        <v>152</v>
-      </c>
       <c r="O22" s="26" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J23" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>154</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>155</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>156</v>
       </c>
-      <c r="M23" t="s">
-        <v>157</v>
-      </c>
       <c r="O23" s="26" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J24" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>443</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>144</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>145</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" t="s">
-        <v>147</v>
-      </c>
       <c r="O24" s="26" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>443</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>444</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>446</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>159</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>160</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>161</v>
       </c>
-      <c r="M25" t="s">
-        <v>162</v>
-      </c>
       <c r="O25" s="26" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J26" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>134</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>135</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>136</v>
       </c>
-      <c r="M26" t="s">
-        <v>137</v>
-      </c>
       <c r="O26" s="26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
         <v>127</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J27" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>450</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>129</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>130</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>131</v>
       </c>
-      <c r="M27" t="s">
-        <v>132</v>
-      </c>
       <c r="O27" s="26" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J28" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>453</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>455</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>139</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>140</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>141</v>
       </c>
-      <c r="M28" t="s">
-        <v>142</v>
-      </c>
       <c r="O28" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J29" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>456</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>457</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>164</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>165</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>166</v>
       </c>
-      <c r="M29" t="s">
-        <v>167</v>
-      </c>
       <c r="O29" s="26" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J30" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>169</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>170</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>171</v>
       </c>
-      <c r="M30" t="s">
-        <v>172</v>
-      </c>
       <c r="N30" s="12" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>462</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>463</v>
-      </c>
       <c r="F31" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="15">
       <c r="A32" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
       <c r="F32" s="16"/>
       <c r="L32" s="12" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J33" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>73</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
+        <v>750</v>
+      </c>
+      <c r="M33" t="s">
         <v>74</v>
       </c>
-      <c r="L33" t="s">
-        <v>751</v>
-      </c>
-      <c r="M33" t="s">
-        <v>75</v>
-      </c>
       <c r="N33" s="12" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J34" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>467</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>469</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>56</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>57</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>58</v>
       </c>
-      <c r="M34" t="s">
-        <v>59</v>
-      </c>
       <c r="N34" s="12" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C35" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>470</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>471</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>472</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>473</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>474</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>376</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
+        <v>67</v>
+      </c>
+      <c r="L36" t="s">
         <v>69</v>
       </c>
-      <c r="K36" t="s">
-        <v>68</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>70</v>
       </c>
-      <c r="M36" t="s">
-        <v>71</v>
-      </c>
       <c r="N36" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="O36" s="26" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>475</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="E37" s="22" t="s">
         <v>476</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>477</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>478</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38" t="s">
         <v>65</v>
       </c>
-      <c r="K38" t="s">
-        <v>64</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>66</v>
       </c>
-      <c r="M38" t="s">
-        <v>67</v>
-      </c>
       <c r="N38" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O38" s="26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="22" t="s">
         <v>482</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>483</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="4"/>
       <c r="I39" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C40" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>484</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="E40" s="22" t="s">
         <v>485</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>486</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="4"/>
       <c r="I40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C41" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>487</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="E41" s="22" t="s">
         <v>488</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>489</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="12" customFormat="1">
       <c r="A42" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -4394,10 +4394,10 @@
     </row>
     <row r="43" spans="1:15" s="12" customFormat="1">
       <c r="A43" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -4406,1651 +4406,1651 @@
     </row>
     <row r="44" spans="1:15" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="14"/>
       <c r="L44" s="12" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C45" s="22" t="s">
+        <v>489</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>490</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>491</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>492</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>493</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>494</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>495</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J47" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>496</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
+        <v>59</v>
+      </c>
+      <c r="L47" t="s">
         <v>61</v>
       </c>
-      <c r="K47" t="s">
-        <v>60</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>62</v>
       </c>
-      <c r="M47" t="s">
-        <v>63</v>
-      </c>
       <c r="N47" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="O47" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="48" spans="1:15" s="12" customFormat="1">
       <c r="A48" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="14"/>
       <c r="L48" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
       <c r="F49" s="14"/>
       <c r="L49" s="12" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J50" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>498</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>498</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>111</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>112</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>113</v>
       </c>
-      <c r="M50" t="s">
-        <v>114</v>
-      </c>
       <c r="N50" s="12" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="O50" s="26" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C51" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="D51" s="22" t="s">
         <v>500</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="E51" s="24" t="s">
         <v>501</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>502</v>
-      </c>
       <c r="F51" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L51" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O51" s="26" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J52" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>116</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>117</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>118</v>
       </c>
-      <c r="M52" t="s">
-        <v>119</v>
-      </c>
       <c r="N52" s="12" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O52" s="26" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="24" t="s">
         <v>506</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>507</v>
-      </c>
       <c r="F53" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L53" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O53" s="26" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
         <v>76</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J54" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>78</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>79</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>80</v>
       </c>
-      <c r="M54" t="s">
-        <v>81</v>
-      </c>
       <c r="N54" s="12" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="O54" s="25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K55" t="s">
+        <v>107</v>
+      </c>
+      <c r="L55" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>512</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="K55" t="s">
-        <v>108</v>
-      </c>
-      <c r="L55" t="s">
-        <v>109</v>
-      </c>
       <c r="M55" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O55" s="26" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J56" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I56" s="1" t="s">
+      <c r="K56" t="s">
+        <v>97</v>
+      </c>
+      <c r="L56" t="s">
+        <v>97</v>
+      </c>
+      <c r="M56" t="s">
         <v>98</v>
       </c>
-      <c r="J56" t="s">
-        <v>99</v>
-      </c>
-      <c r="K56" t="s">
-        <v>98</v>
-      </c>
-      <c r="L56" t="s">
-        <v>98</v>
-      </c>
-      <c r="M56" t="s">
-        <v>99</v>
-      </c>
       <c r="N56" s="12" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O56" s="25" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C57" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="E57" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="E57" s="24" t="s">
-        <v>519</v>
-      </c>
       <c r="F57" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K57" t="s">
+        <v>91</v>
+      </c>
+      <c r="L57" t="s">
+        <v>611</v>
+      </c>
+      <c r="M57" t="s">
         <v>92</v>
       </c>
-      <c r="L57" t="s">
-        <v>612</v>
-      </c>
-      <c r="M57" t="s">
-        <v>93</v>
-      </c>
       <c r="N57" s="12" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="O57" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>521</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J58" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>520</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>522</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="I58" s="1" t="s">
+      <c r="K58" t="s">
+        <v>93</v>
+      </c>
+      <c r="L58" t="s">
+        <v>610</v>
+      </c>
+      <c r="M58" t="s">
         <v>94</v>
       </c>
-      <c r="J58" t="s">
-        <v>95</v>
-      </c>
-      <c r="K58" t="s">
-        <v>94</v>
-      </c>
-      <c r="L58" t="s">
-        <v>611</v>
-      </c>
-      <c r="M58" t="s">
-        <v>95</v>
-      </c>
       <c r="N58" s="12" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O58" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J59" t="s">
         <v>96</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>524</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I59" s="1" t="s">
+      <c r="K59" t="s">
+        <v>95</v>
+      </c>
+      <c r="L59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M59" t="s">
         <v>96</v>
       </c>
-      <c r="J59" t="s">
-        <v>97</v>
-      </c>
-      <c r="K59" t="s">
-        <v>96</v>
-      </c>
-      <c r="L59" t="s">
-        <v>96</v>
-      </c>
-      <c r="M59" t="s">
-        <v>97</v>
-      </c>
       <c r="N59" s="12" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="O59" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C60" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>526</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>527</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="4"/>
       <c r="I60" s="1"/>
       <c r="J60" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="E61" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="E61" s="22" t="s">
-        <v>530</v>
-      </c>
       <c r="G61" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J61" t="s">
+        <v>120</v>
+      </c>
+      <c r="K61" t="s">
         <v>121</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>122</v>
       </c>
-      <c r="L61" t="s">
+      <c r="M61" t="s">
         <v>123</v>
       </c>
-      <c r="M61" t="s">
-        <v>124</v>
-      </c>
       <c r="N61" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O61" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C62" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="E62" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="E62" s="22" t="s">
-        <v>530</v>
-      </c>
       <c r="G62" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J62" t="s">
+        <v>120</v>
+      </c>
+      <c r="K62" t="s">
         <v>121</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>122</v>
       </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>123</v>
       </c>
-      <c r="M62" t="s">
-        <v>124</v>
-      </c>
       <c r="N62" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O62" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C63" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="D63" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="E63" s="24" t="s">
         <v>532</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>533</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L63" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O63" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1">
       <c r="A64" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C64" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>534</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="E64" s="22" t="s">
         <v>535</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>536</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="12"/>
       <c r="H64" s="4"/>
       <c r="J64" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O64" s="26" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1">
       <c r="A65" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C65" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="E65" s="24" t="s">
         <v>538</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>539</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="12"/>
       <c r="H65" s="4"/>
       <c r="J65" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O65" s="26" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="66" spans="1:15" s="2" customFormat="1">
       <c r="A66" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D66" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="E66" s="22" t="s">
         <v>541</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>542</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K66" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="M66" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="L66" s="2" t="s">
-        <v>758</v>
-      </c>
-      <c r="M66" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="N66" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O66" s="26" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="12" customFormat="1">
       <c r="A67" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
       <c r="F67" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>615</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="K67" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>613</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="I67" s="12" t="s">
+      <c r="L67" s="12" t="s">
         <v>617</v>
       </c>
-      <c r="J67" s="12" t="s">
+      <c r="M67" s="12" t="s">
         <v>619</v>
       </c>
-      <c r="K67" s="12" t="s">
-        <v>615</v>
-      </c>
-      <c r="L67" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="M67" s="12" t="s">
-        <v>620</v>
-      </c>
       <c r="N67" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O67" s="25" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M68" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="N68" s="12" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O68" s="25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1">
       <c r="A69" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J69" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J69" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="M69" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M69" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="N69" s="12" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O69" s="26" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="70" spans="1:15" s="12" customFormat="1">
       <c r="A70" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
       <c r="F70" s="14" t="s">
+        <v>779</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>779</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>779</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>777</v>
+      </c>
+      <c r="J70" s="22" t="s">
         <v>780</v>
       </c>
-      <c r="G70" s="12" t="s">
-        <v>780</v>
-      </c>
-      <c r="H70" s="22" t="s">
-        <v>780</v>
-      </c>
-      <c r="I70" s="22" t="s">
+      <c r="K70" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="L70" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="M70" s="12" t="s">
+        <v>776</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="O70" s="14" t="s">
         <v>778</v>
-      </c>
-      <c r="J70" s="22" t="s">
-        <v>781</v>
-      </c>
-      <c r="K70" s="12" t="s">
-        <v>775</v>
-      </c>
-      <c r="L70" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="M70" s="12" t="s">
-        <v>777</v>
-      </c>
-      <c r="N70" s="12" t="s">
-        <v>778</v>
-      </c>
-      <c r="O70" s="14" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C71" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D71" s="22" t="s">
         <v>549</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="E71" s="22" t="s">
         <v>550</v>
-      </c>
-      <c r="E71" s="22" t="s">
-        <v>551</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="12"/>
       <c r="H71" s="4"/>
       <c r="J71" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="O71" s="25" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C72" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="E72" s="24" t="s">
         <v>553</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>554</v>
       </c>
       <c r="F72" s="14"/>
       <c r="G72" s="12"/>
       <c r="H72" s="4"/>
       <c r="J72" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O72" s="25" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C73" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J73" s="2" t="s">
+      <c r="K73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="M73" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M73" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="N73" s="12" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O73" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="74" spans="1:15" s="2" customFormat="1">
       <c r="A74" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>559</v>
-      </c>
       <c r="F74" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J74" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="L74" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M74" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L74" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="N74" s="12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O74" s="25" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="75" spans="1:15">
       <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" t="s">
         <v>178</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" t="s">
+        <v>179</v>
+      </c>
+      <c r="K75" t="s">
         <v>180</v>
       </c>
-      <c r="J75" t="s">
-        <v>180</v>
-      </c>
-      <c r="K75" t="s">
-        <v>181</v>
-      </c>
       <c r="L75" t="s">
+        <v>178</v>
+      </c>
+      <c r="M75" t="s">
         <v>179</v>
       </c>
-      <c r="M75" t="s">
-        <v>180</v>
-      </c>
       <c r="N75" s="12" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="O75" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="76" spans="1:15">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J76" t="s">
         <v>182</v>
       </c>
-      <c r="C76" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>183</v>
       </c>
-      <c r="K76" t="s">
+      <c r="L76" t="s">
         <v>184</v>
       </c>
-      <c r="L76" t="s">
+      <c r="M76" t="s">
         <v>185</v>
       </c>
-      <c r="M76" t="s">
-        <v>186</v>
-      </c>
       <c r="N76" s="12" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="O76" s="26" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="28.8">
       <c r="A77" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C77" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>567</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>568</v>
-      </c>
       <c r="F77" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="1"/>
       <c r="J77" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L77" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="28.8">
       <c r="A78" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C78" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="D78" s="22" t="s">
         <v>569</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="E78" s="22" t="s">
-        <v>571</v>
-      </c>
       <c r="F78" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L78" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="O78" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="28.8">
       <c r="A79" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>572</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="E79" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>574</v>
-      </c>
       <c r="F79" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L79" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="28.8">
       <c r="A80" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C80" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>575</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E80" s="22" t="s">
-        <v>577</v>
-      </c>
       <c r="F80" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L80" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="O80" s="26" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="E81" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="E81" s="24" t="s">
-        <v>580</v>
-      </c>
       <c r="F81" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L81" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="O81" s="26" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="28.8">
       <c r="A82" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D82" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="E82" s="22" t="s">
-        <v>583</v>
-      </c>
       <c r="F82" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L82" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O82" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="28.8">
       <c r="A83" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C83" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>584</v>
       </c>
-      <c r="D83" s="22" t="s">
+      <c r="E83" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>586</v>
-      </c>
       <c r="F83" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L83" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="O83" s="26" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="28.8">
       <c r="A84" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C84" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="D84" s="22" t="s">
         <v>587</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="E84" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>589</v>
-      </c>
       <c r="F84" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L84" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="O84" s="26" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="28.8">
       <c r="A85" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C85" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="D85" s="22" t="s">
+      <c r="E85" s="22" t="s">
         <v>591</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>592</v>
-      </c>
       <c r="F85" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L85" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="O85" s="26" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="86" spans="1:15">
       <c r="A86" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C86" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="D86" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="D86" s="22" t="s">
+      <c r="E86" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="E86" s="22" t="s">
-        <v>595</v>
-      </c>
       <c r="F86" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="O86" s="26" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="87" spans="1:15">
       <c r="A87" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C87" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="E87" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="E87" s="22" t="s">
-        <v>598</v>
-      </c>
       <c r="F87" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="1"/>
       <c r="J87" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="O87" s="26" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
translation update for ES Wilcoxon Rank sum test (#1062)
* translation update for ES Wilcoxon Rank sum test

* increment version number
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819FD20-9835-4ACC-9E96-56EA5506E64C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A692F8-DDF0-45D4-9930-EC1E2C7388B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Testes estatísticos realizados</t>
   </si>
   <si>
-    <t>prueba de los rangos con signo de Wilcoxon</t>
-  </si>
-  <si>
     <t>Wilcoxon-Mann-Whitney-Test</t>
   </si>
   <si>
@@ -2485,6 +2482,9 @@
   </si>
   <si>
     <t>Suma</t>
+  </si>
+  <si>
+    <t>Prueba de la suma de rangos de Wilcoxon</t>
   </si>
 </sst>
 </file>
@@ -2946,11 +2946,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2980,25 +2980,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>601</v>
-      </c>
       <c r="F1" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -3013,504 +3013,504 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B4" t="s">
         <v>621</v>
       </c>
-      <c r="B4" t="s">
-        <v>622</v>
-      </c>
       <c r="L4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B9" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L10" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" t="s">
         <v>173</v>
       </c>
-      <c r="B11" t="s">
-        <v>174</v>
-      </c>
       <c r="C11" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>403</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="22" t="s">
         <v>404</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>405</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
+        <v>174</v>
+      </c>
+      <c r="K11" t="s">
         <v>175</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>176</v>
       </c>
-      <c r="L11" t="s">
-        <v>177</v>
-      </c>
       <c r="M11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>406</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="E12" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>408</v>
-      </c>
       <c r="F12" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>16</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
-        <v>18</v>
-      </c>
       <c r="N12" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>21</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
       <c r="O13" s="25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>414</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
         <v>39</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>40</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>41</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>42</v>
       </c>
-      <c r="M14" t="s">
-        <v>43</v>
-      </c>
       <c r="O14" s="25" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>35</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>36</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>37</v>
       </c>
-      <c r="M15" t="s">
-        <v>38</v>
-      </c>
       <c r="N15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>30</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>31</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>32</v>
       </c>
-      <c r="M16" t="s">
-        <v>33</v>
-      </c>
       <c r="N16" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>421</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>45</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>46</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>47</v>
-      </c>
-      <c r="M17" t="s">
-        <v>48</v>
       </c>
       <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>25</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>26</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>27</v>
       </c>
-      <c r="M18" t="s">
-        <v>28</v>
-      </c>
       <c r="N18" s="12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="E19" s="22" t="s">
         <v>427</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>428</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
@@ -3525,867 +3525,867 @@
         <v>10</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C20" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>431</v>
-      </c>
       <c r="F20" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
         <v>49</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>50</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>51</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>52</v>
       </c>
-      <c r="M20" t="s">
-        <v>53</v>
-      </c>
       <c r="N20" s="12" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>434</v>
-      </c>
       <c r="F21" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J21" t="s">
+        <v>781</v>
+      </c>
+      <c r="K21" t="s">
         <v>11</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>12</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>13</v>
       </c>
-      <c r="M21" t="s">
-        <v>14</v>
-      </c>
       <c r="O21" s="25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J22" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>435</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>149</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>150</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>151</v>
       </c>
-      <c r="M22" t="s">
-        <v>152</v>
-      </c>
       <c r="O22" s="26" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J23" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>154</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>155</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>156</v>
       </c>
-      <c r="M23" t="s">
-        <v>157</v>
-      </c>
       <c r="O23" s="26" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J24" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>443</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>144</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>145</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" t="s">
-        <v>147</v>
-      </c>
       <c r="O24" s="26" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>443</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>444</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>446</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>159</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>160</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>161</v>
       </c>
-      <c r="M25" t="s">
-        <v>162</v>
-      </c>
       <c r="O25" s="26" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J26" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>134</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>135</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>136</v>
       </c>
-      <c r="M26" t="s">
-        <v>137</v>
-      </c>
       <c r="O26" s="26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
         <v>127</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J27" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>450</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>129</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>130</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>131</v>
       </c>
-      <c r="M27" t="s">
-        <v>132</v>
-      </c>
       <c r="O27" s="26" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J28" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>453</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>455</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>139</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>140</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>141</v>
       </c>
-      <c r="M28" t="s">
-        <v>142</v>
-      </c>
       <c r="O28" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J29" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>456</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>457</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>164</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>165</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>166</v>
       </c>
-      <c r="M29" t="s">
-        <v>167</v>
-      </c>
       <c r="O29" s="26" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J30" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>169</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>170</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>171</v>
       </c>
-      <c r="M30" t="s">
-        <v>172</v>
-      </c>
       <c r="N30" s="12" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>462</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>463</v>
-      </c>
       <c r="F31" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="12" customFormat="1" ht="15">
       <c r="A32" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
       <c r="F32" s="16"/>
       <c r="L32" s="12" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J33" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>73</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
+        <v>750</v>
+      </c>
+      <c r="M33" t="s">
         <v>74</v>
       </c>
-      <c r="L33" t="s">
-        <v>751</v>
-      </c>
-      <c r="M33" t="s">
-        <v>75</v>
-      </c>
       <c r="N33" s="12" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J34" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>467</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>469</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>56</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>57</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>58</v>
       </c>
-      <c r="M34" t="s">
-        <v>59</v>
-      </c>
       <c r="N34" s="12" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C35" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>470</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>471</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>472</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>473</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>474</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>376</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
+        <v>67</v>
+      </c>
+      <c r="L36" t="s">
         <v>69</v>
       </c>
-      <c r="K36" t="s">
-        <v>68</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>70</v>
       </c>
-      <c r="M36" t="s">
-        <v>71</v>
-      </c>
       <c r="N36" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="O36" s="26" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>475</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="E37" s="22" t="s">
         <v>476</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>477</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>478</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38" t="s">
         <v>65</v>
       </c>
-      <c r="K38" t="s">
-        <v>64</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>66</v>
       </c>
-      <c r="M38" t="s">
-        <v>67</v>
-      </c>
       <c r="N38" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O38" s="26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="22" t="s">
         <v>482</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>483</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="4"/>
       <c r="I39" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C40" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>484</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="E40" s="22" t="s">
         <v>485</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>486</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="4"/>
       <c r="I40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C41" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>487</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="E41" s="22" t="s">
         <v>488</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>489</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4"/>
       <c r="I41" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="12" customFormat="1">
       <c r="A42" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -4394,10 +4394,10 @@
     </row>
     <row r="43" spans="1:15" s="12" customFormat="1">
       <c r="A43" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -4406,1651 +4406,1651 @@
     </row>
     <row r="44" spans="1:15" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="14"/>
       <c r="L44" s="12" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C45" s="22" t="s">
+        <v>489</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>490</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>491</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>492</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>493</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>494</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>495</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J47" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>496</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
+        <v>59</v>
+      </c>
+      <c r="L47" t="s">
         <v>61</v>
       </c>
-      <c r="K47" t="s">
-        <v>60</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>62</v>
       </c>
-      <c r="M47" t="s">
-        <v>63</v>
-      </c>
       <c r="N47" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="O47" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="48" spans="1:15" s="12" customFormat="1">
       <c r="A48" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="14"/>
       <c r="L48" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
       <c r="F49" s="14"/>
       <c r="L49" s="12" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J50" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>498</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>498</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>111</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>112</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>113</v>
       </c>
-      <c r="M50" t="s">
-        <v>114</v>
-      </c>
       <c r="N50" s="12" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="O50" s="26" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C51" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="D51" s="22" t="s">
         <v>500</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="E51" s="24" t="s">
         <v>501</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>502</v>
-      </c>
       <c r="F51" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L51" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O51" s="26" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J52" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>116</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>117</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>118</v>
       </c>
-      <c r="M52" t="s">
-        <v>119</v>
-      </c>
       <c r="N52" s="12" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O52" s="26" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="24" t="s">
         <v>506</v>
       </c>
-      <c r="E53" s="24" t="s">
-        <v>507</v>
-      </c>
       <c r="F53" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L53" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O53" s="26" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
         <v>76</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J54" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>510</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>78</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>79</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>80</v>
       </c>
-      <c r="M54" t="s">
-        <v>81</v>
-      </c>
       <c r="N54" s="12" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="O54" s="25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K55" t="s">
+        <v>107</v>
+      </c>
+      <c r="L55" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>512</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="K55" t="s">
-        <v>108</v>
-      </c>
-      <c r="L55" t="s">
-        <v>109</v>
-      </c>
       <c r="M55" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O55" s="26" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J56" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I56" s="1" t="s">
+      <c r="K56" t="s">
+        <v>97</v>
+      </c>
+      <c r="L56" t="s">
+        <v>97</v>
+      </c>
+      <c r="M56" t="s">
         <v>98</v>
       </c>
-      <c r="J56" t="s">
-        <v>99</v>
-      </c>
-      <c r="K56" t="s">
-        <v>98</v>
-      </c>
-      <c r="L56" t="s">
-        <v>98</v>
-      </c>
-      <c r="M56" t="s">
-        <v>99</v>
-      </c>
       <c r="N56" s="12" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O56" s="25" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C57" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="E57" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="E57" s="24" t="s">
-        <v>519</v>
-      </c>
       <c r="F57" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K57" t="s">
+        <v>91</v>
+      </c>
+      <c r="L57" t="s">
+        <v>611</v>
+      </c>
+      <c r="M57" t="s">
         <v>92</v>
       </c>
-      <c r="L57" t="s">
-        <v>612</v>
-      </c>
-      <c r="M57" t="s">
-        <v>93</v>
-      </c>
       <c r="N57" s="12" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="O57" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>521</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J58" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>520</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>522</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="I58" s="1" t="s">
+      <c r="K58" t="s">
+        <v>93</v>
+      </c>
+      <c r="L58" t="s">
+        <v>610</v>
+      </c>
+      <c r="M58" t="s">
         <v>94</v>
       </c>
-      <c r="J58" t="s">
-        <v>95</v>
-      </c>
-      <c r="K58" t="s">
-        <v>94</v>
-      </c>
-      <c r="L58" t="s">
-        <v>611</v>
-      </c>
-      <c r="M58" t="s">
-        <v>95</v>
-      </c>
       <c r="N58" s="12" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O58" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J59" t="s">
         <v>96</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>524</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="I59" s="1" t="s">
+      <c r="K59" t="s">
+        <v>95</v>
+      </c>
+      <c r="L59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M59" t="s">
         <v>96</v>
       </c>
-      <c r="J59" t="s">
-        <v>97</v>
-      </c>
-      <c r="K59" t="s">
-        <v>96</v>
-      </c>
-      <c r="L59" t="s">
-        <v>96</v>
-      </c>
-      <c r="M59" t="s">
-        <v>97</v>
-      </c>
       <c r="N59" s="12" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="O59" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C60" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>526</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>527</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="4"/>
       <c r="I60" s="1"/>
       <c r="J60" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="E61" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="E61" s="22" t="s">
-        <v>530</v>
-      </c>
       <c r="G61" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J61" t="s">
+        <v>120</v>
+      </c>
+      <c r="K61" t="s">
         <v>121</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>122</v>
       </c>
-      <c r="L61" t="s">
+      <c r="M61" t="s">
         <v>123</v>
       </c>
-      <c r="M61" t="s">
-        <v>124</v>
-      </c>
       <c r="N61" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O61" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C62" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="E62" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="E62" s="22" t="s">
-        <v>530</v>
-      </c>
       <c r="G62" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J62" t="s">
+        <v>120</v>
+      </c>
+      <c r="K62" t="s">
         <v>121</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>122</v>
       </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>123</v>
       </c>
-      <c r="M62" t="s">
-        <v>124</v>
-      </c>
       <c r="N62" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O62" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C63" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="D63" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="E63" s="24" t="s">
         <v>532</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>533</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="4"/>
       <c r="I63" s="1"/>
       <c r="J63" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L63" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O63" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1">
       <c r="A64" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C64" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>534</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="E64" s="22" t="s">
         <v>535</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>536</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="12"/>
       <c r="H64" s="4"/>
       <c r="J64" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O64" s="26" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1">
       <c r="A65" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C65" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="E65" s="24" t="s">
         <v>538</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>539</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="12"/>
       <c r="H65" s="4"/>
       <c r="J65" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O65" s="26" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="66" spans="1:15" s="2" customFormat="1">
       <c r="A66" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D66" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="E66" s="22" t="s">
         <v>541</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>542</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K66" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="M66" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="L66" s="2" t="s">
-        <v>758</v>
-      </c>
-      <c r="M66" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="N66" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O66" s="26" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="12" customFormat="1">
       <c r="A67" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
       <c r="F67" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>615</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="K67" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>613</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="I67" s="12" t="s">
+      <c r="L67" s="12" t="s">
         <v>617</v>
       </c>
-      <c r="J67" s="12" t="s">
+      <c r="M67" s="12" t="s">
         <v>619</v>
       </c>
-      <c r="K67" s="12" t="s">
-        <v>615</v>
-      </c>
-      <c r="L67" s="12" t="s">
-        <v>618</v>
-      </c>
-      <c r="M67" s="12" t="s">
-        <v>620</v>
-      </c>
       <c r="N67" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O67" s="25" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M68" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="N68" s="12" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O68" s="25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1">
       <c r="A69" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J69" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J69" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="M69" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M69" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="N69" s="12" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O69" s="26" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="70" spans="1:15" s="12" customFormat="1">
       <c r="A70" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
       <c r="F70" s="14" t="s">
+        <v>779</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>779</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>779</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>777</v>
+      </c>
+      <c r="J70" s="22" t="s">
         <v>780</v>
       </c>
-      <c r="G70" s="12" t="s">
-        <v>780</v>
-      </c>
-      <c r="H70" s="22" t="s">
-        <v>780</v>
-      </c>
-      <c r="I70" s="22" t="s">
+      <c r="K70" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="L70" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="M70" s="12" t="s">
+        <v>776</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="O70" s="14" t="s">
         <v>778</v>
-      </c>
-      <c r="J70" s="22" t="s">
-        <v>781</v>
-      </c>
-      <c r="K70" s="12" t="s">
-        <v>775</v>
-      </c>
-      <c r="L70" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="M70" s="12" t="s">
-        <v>777</v>
-      </c>
-      <c r="N70" s="12" t="s">
-        <v>778</v>
-      </c>
-      <c r="O70" s="14" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C71" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D71" s="22" t="s">
         <v>549</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="E71" s="22" t="s">
         <v>550</v>
-      </c>
-      <c r="E71" s="22" t="s">
-        <v>551</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="12"/>
       <c r="H71" s="4"/>
       <c r="J71" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="O71" s="25" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C72" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="E72" s="24" t="s">
         <v>553</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>554</v>
       </c>
       <c r="F72" s="14"/>
       <c r="G72" s="12"/>
       <c r="H72" s="4"/>
       <c r="J72" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O72" s="25" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C73" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J73" s="2" t="s">
+      <c r="K73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="M73" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M73" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="N73" s="12" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O73" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="74" spans="1:15" s="2" customFormat="1">
       <c r="A74" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C74" s="22" t="s">
+        <v>556</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>559</v>
-      </c>
       <c r="F74" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J74" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="L74" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M74" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L74" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="N74" s="12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O74" s="25" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="75" spans="1:15">
       <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" t="s">
         <v>178</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" t="s">
+        <v>179</v>
+      </c>
+      <c r="K75" t="s">
         <v>180</v>
       </c>
-      <c r="J75" t="s">
-        <v>180</v>
-      </c>
-      <c r="K75" t="s">
-        <v>181</v>
-      </c>
       <c r="L75" t="s">
+        <v>178</v>
+      </c>
+      <c r="M75" t="s">
         <v>179</v>
       </c>
-      <c r="M75" t="s">
-        <v>180</v>
-      </c>
       <c r="N75" s="12" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="O75" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="76" spans="1:15">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J76" t="s">
         <v>182</v>
       </c>
-      <c r="C76" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>183</v>
       </c>
-      <c r="K76" t="s">
+      <c r="L76" t="s">
         <v>184</v>
       </c>
-      <c r="L76" t="s">
+      <c r="M76" t="s">
         <v>185</v>
       </c>
-      <c r="M76" t="s">
-        <v>186</v>
-      </c>
       <c r="N76" s="12" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="O76" s="26" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="28.8">
       <c r="A77" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C77" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>567</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>568</v>
-      </c>
       <c r="F77" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="1"/>
       <c r="J77" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L77" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="28.8">
       <c r="A78" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C78" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="D78" s="22" t="s">
         <v>569</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="E78" s="22" t="s">
-        <v>571</v>
-      </c>
       <c r="F78" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="1"/>
       <c r="J78" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L78" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="O78" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="28.8">
       <c r="A79" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>572</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="E79" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>574</v>
-      </c>
       <c r="F79" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L79" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="28.8">
       <c r="A80" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C80" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>575</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E80" s="22" t="s">
-        <v>577</v>
-      </c>
       <c r="F80" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="1"/>
       <c r="J80" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L80" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="O80" s="26" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="E81" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="E81" s="24" t="s">
-        <v>580</v>
-      </c>
       <c r="F81" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="1"/>
       <c r="J81" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L81" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="O81" s="26" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="28.8">
       <c r="A82" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D82" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="E82" s="22" t="s">
-        <v>583</v>
-      </c>
       <c r="F82" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="1"/>
       <c r="J82" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L82" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O82" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="28.8">
       <c r="A83" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C83" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>584</v>
       </c>
-      <c r="D83" s="22" t="s">
+      <c r="E83" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>586</v>
-      </c>
       <c r="F83" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L83" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="O83" s="26" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="28.8">
       <c r="A84" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C84" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="D84" s="22" t="s">
         <v>587</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="E84" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>589</v>
-      </c>
       <c r="F84" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L84" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="O84" s="26" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="28.8">
       <c r="A85" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C85" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="D85" s="22" t="s">
+      <c r="E85" s="22" t="s">
         <v>591</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>592</v>
-      </c>
       <c r="F85" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L85" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="O85" s="26" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="86" spans="1:15">
       <c r="A86" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C86" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="D86" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="D86" s="22" t="s">
+      <c r="E86" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="E86" s="22" t="s">
-        <v>595</v>
-      </c>
       <c r="F86" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="O86" s="26" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="87" spans="1:15">
       <c r="A87" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C87" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="E87" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="E87" s="22" t="s">
-        <v>598</v>
-      </c>
       <c r="F87" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="1"/>
       <c r="J87" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="O87" s="26" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reporting credible interval for Bayesian models
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEBB220-0866-411A-B0FA-C0FAE5377451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EFEB1-DE09-4DD9-8406-00E0EFA297A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="843">
   <si>
     <t>context</t>
   </si>
@@ -2662,6 +2662,12 @@
   </si>
   <si>
     <t>Pearsons kjikvadrattest</t>
+  </si>
+  <si>
+    <t>CI = Credible Interval</t>
+  </si>
+  <si>
+    <t>Credible Interval</t>
   </si>
 </sst>
 </file>
@@ -3121,13 +3127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4398,134 +4404,78 @@
         <v>813</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
-      <c r="A37" t="s">
+    <row r="37" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="A37" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L37" t="s">
-        <v>743</v>
-      </c>
-      <c r="M37" t="s">
-        <v>785</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>644</v>
-      </c>
-      <c r="O37" s="26" t="s">
-        <v>696</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" t="s">
+      <c r="B37" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J38" t="s">
-        <v>51</v>
-      </c>
-      <c r="K38" t="s">
-        <v>52</v>
-      </c>
-      <c r="L38" t="s">
-        <v>53</v>
-      </c>
-      <c r="M38" t="s">
-        <v>54</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>645</v>
-      </c>
-      <c r="O38" s="25" t="s">
-        <v>697</v>
-      </c>
-      <c r="P38" s="12" t="s">
-        <v>218</v>
-      </c>
+      <c r="B38" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="G39" s="12"/>
+        <v>459</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>319</v>
+      </c>
       <c r="H39" s="4" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>193</v>
+        <v>217</v>
+      </c>
+      <c r="J39" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" t="s">
+        <v>743</v>
+      </c>
+      <c r="M39" t="s">
+        <v>785</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>193</v>
+        <v>644</v>
+      </c>
+      <c r="O39" s="26" t="s">
+        <v>696</v>
       </c>
       <c r="P39" s="12" t="s">
-        <v>193</v>
+        <v>814</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -4533,49 +4483,49 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J40" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="K40" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="L40" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="M40" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>646</v>
-      </c>
-      <c r="O40" s="26" t="s">
-        <v>698</v>
+        <v>645</v>
+      </c>
+      <c r="O40" s="25" t="s">
+        <v>697</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>815</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -4583,29 +4533,29 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>816</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -4613,49 +4563,49 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="J42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L42" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M42" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O42" s="26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="P42" s="12" t="s">
-        <v>59</v>
+        <v>815</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -4663,24 +4613,29 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="G43" s="12"/>
-      <c r="H43" s="4"/>
+      <c r="H43" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="I43" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="P43" s="12" t="s">
-        <v>198</v>
+        <v>816</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -4688,24 +4643,49 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="4"/>
+        <v>473</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="I44" s="1" t="s">
-        <v>194</v>
+        <v>59</v>
+      </c>
+      <c r="J44" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="O44" s="26" t="s">
+        <v>699</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -4713,54 +4693,74 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P45" s="12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="G46" s="12"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
         <v>196</v>
       </c>
-      <c r="P45" s="12" t="s">
+      <c r="C47" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>482</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="P47" s="12" t="s">
         <v>817</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" s="12" customFormat="1">
-      <c r="A46" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>632</v>
-      </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="14"/>
-      <c r="P46" s="12" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="12" customFormat="1">
-      <c r="A47" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>633</v>
-      </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="14"/>
-      <c r="P47" s="12" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="12" customFormat="1">
@@ -4768,78 +4768,50 @@
         <v>49</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="14"/>
-      <c r="L48" s="12" t="s">
+      <c r="P48" s="12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="12" customFormat="1">
+      <c r="A49" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="14"/>
+      <c r="P49" s="12" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="12" customFormat="1">
+      <c r="A50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="14"/>
+      <c r="L50" s="12" t="s">
         <v>744</v>
       </c>
-      <c r="M48" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>786</v>
       </c>
-      <c r="P48" s="12" t="s">
+      <c r="P50" s="12" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>483</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>484</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="N49" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="P49" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>487</v>
-      </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="N50" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="P50" s="12" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -4847,187 +4819,155 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="P51" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C53" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D53" s="24" t="s">
         <v>489</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E53" s="24" t="s">
         <v>490</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J53" t="s">
         <v>56</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K53" t="s">
         <v>55</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L53" t="s">
         <v>57</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M53" t="s">
         <v>58</v>
       </c>
-      <c r="N51" s="12" t="s">
+      <c r="N53" s="12" t="s">
         <v>648</v>
       </c>
-      <c r="O51" s="26" t="s">
+      <c r="O53" s="26" t="s">
         <v>700</v>
       </c>
-      <c r="P51" s="12" t="s">
+      <c r="P53" s="12" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="12" customFormat="1">
-      <c r="A52" s="12" t="s">
+    <row r="54" spans="1:16" s="12" customFormat="1">
+      <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="14"/>
-      <c r="L52" s="12" t="s">
+      <c r="C54" s="22"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="14"/>
+      <c r="L54" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="N52" s="12" t="s">
+      <c r="N54" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="O52" s="25" t="s">
+      <c r="O54" s="25" t="s">
         <v>701</v>
       </c>
-      <c r="P52" s="12" t="s">
+      <c r="P54" s="12" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="12" customFormat="1">
-      <c r="A53" s="12" t="s">
+    <row r="55" spans="1:16" s="12" customFormat="1">
+      <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="14"/>
-      <c r="L53" s="12" t="s">
+      <c r="C55" s="22"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="14"/>
+      <c r="L55" s="12" t="s">
         <v>745</v>
       </c>
-      <c r="M53" s="12" t="s">
+      <c r="M55" s="12" t="s">
         <v>787</v>
       </c>
-      <c r="N53" s="12" t="s">
+      <c r="N55" s="12" t="s">
         <v>649</v>
       </c>
-      <c r="P53" s="12" t="s">
+      <c r="P55" s="12" t="s">
         <v>820</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J54" t="s">
-        <v>104</v>
-      </c>
-      <c r="K54" t="s">
-        <v>105</v>
-      </c>
-      <c r="L54" t="s">
-        <v>106</v>
-      </c>
-      <c r="M54" t="s">
-        <v>107</v>
-      </c>
-      <c r="N54" s="12" t="s">
-        <v>650</v>
-      </c>
-      <c r="O54" s="26" t="s">
-        <v>702</v>
-      </c>
-      <c r="P54" s="12" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16">
-      <c r="A55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" t="s">
-        <v>254</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I55" s="1"/>
-      <c r="J55" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="L55" t="s">
-        <v>746</v>
-      </c>
-      <c r="N55" s="12" t="s">
-        <v>651</v>
-      </c>
-      <c r="O55" s="26" t="s">
-        <v>703</v>
-      </c>
-      <c r="P55" s="12" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -5035,49 +4975,49 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>497</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>374</v>
+        <v>492</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>372</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J56" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L56" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M56" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="O56" s="26" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -5085,39 +5025,39 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>500</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>375</v>
+        <v>495</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>373</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I57" s="1"/>
-      <c r="J57" s="11" t="s">
-        <v>280</v>
+      <c r="J57" s="12" t="s">
+        <v>279</v>
       </c>
       <c r="L57" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O57" s="26" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -5125,49 +5065,49 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>376</v>
+        <v>497</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>374</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J58" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="K58" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="L58" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="M58" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>654</v>
-      </c>
-      <c r="O58" s="25" t="s">
-        <v>706</v>
+        <v>652</v>
+      </c>
+      <c r="O58" s="26" t="s">
+        <v>704</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>223</v>
+        <v>823</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -5175,49 +5115,39 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>255</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>327</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>500</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="G59" s="12"/>
       <c r="H59" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="K59" t="s">
-        <v>101</v>
+        <v>274</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="L59" t="s">
-        <v>102</v>
-      </c>
-      <c r="M59" s="12" t="s">
-        <v>788</v>
+        <v>747</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>101</v>
+        <v>653</v>
       </c>
       <c r="O59" s="26" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -5225,49 +5155,49 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>240</v>
+        <v>503</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>376</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="J60" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="K60" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="L60" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="M60" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O60" s="25" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>826</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -5275,49 +5205,49 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>597</v>
+        <v>101</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>512</v>
+        <v>505</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>506</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="J61" t="s">
-        <v>603</v>
+        <v>600</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="K61" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="L61" t="s">
-        <v>605</v>
-      </c>
-      <c r="M61" t="s">
-        <v>87</v>
+        <v>102</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>788</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>656</v>
-      </c>
-      <c r="O61" s="25" t="s">
-        <v>709</v>
+        <v>101</v>
+      </c>
+      <c r="O61" s="26" t="s">
+        <v>707</v>
       </c>
       <c r="P61" s="12" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -5325,49 +5255,49 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>515</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>378</v>
+        <v>508</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J62" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K62" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L62" t="s">
-        <v>604</v>
+        <v>92</v>
       </c>
       <c r="M62" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="O62" s="25" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="P62" s="12" t="s">
-        <v>88</v>
+        <v>826</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -5375,49 +5305,49 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>597</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>518</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>243</v>
+        <v>511</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>377</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>90</v>
+        <v>601</v>
       </c>
       <c r="J63" t="s">
-        <v>91</v>
+        <v>603</v>
       </c>
       <c r="K63" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L63" t="s">
-        <v>90</v>
+        <v>605</v>
       </c>
       <c r="M63" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="O63" s="25" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="P63" s="12" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -5425,28 +5355,49 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>88</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>520</v>
-      </c>
-      <c r="G64" s="12"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="9" t="s">
-        <v>250</v>
+        <v>514</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J64" t="s">
+        <v>89</v>
+      </c>
+      <c r="K64" t="s">
+        <v>88</v>
+      </c>
+      <c r="L64" t="s">
+        <v>604</v>
+      </c>
+      <c r="M64" t="s">
+        <v>89</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>250</v>
+        <v>657</v>
+      </c>
+      <c r="O64" s="25" t="s">
+        <v>710</v>
       </c>
       <c r="P64" s="12" t="s">
-        <v>250</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -5454,44 +5405,49 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>523</v>
+        <v>518</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H65" s="4"/>
+        <v>331</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="I65" s="1" t="s">
-        <v>224</v>
+        <v>90</v>
       </c>
       <c r="J65" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="K65" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="L65" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M65" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O65" s="25" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="P65" s="12" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -5499,44 +5455,28 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>332</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="G66" s="12"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J66" t="s">
-        <v>114</v>
-      </c>
-      <c r="K66" t="s">
-        <v>115</v>
-      </c>
-      <c r="L66" t="s">
-        <v>116</v>
-      </c>
-      <c r="M66" t="s">
-        <v>117</v>
+      <c r="I66" s="1"/>
+      <c r="J66" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>659</v>
-      </c>
-      <c r="O66" s="25" t="s">
-        <v>712</v>
+        <v>250</v>
       </c>
       <c r="P66" s="12" t="s">
-        <v>830</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -5544,104 +5484,124 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H67" s="4"/>
+      <c r="I67" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J67" t="s">
+        <v>114</v>
+      </c>
+      <c r="K67" t="s">
+        <v>115</v>
+      </c>
+      <c r="L67" t="s">
+        <v>116</v>
+      </c>
+      <c r="M67" t="s">
+        <v>117</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="O67" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="P67" s="12" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H68" s="4"/>
+      <c r="I68" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J68" t="s">
+        <v>114</v>
+      </c>
+      <c r="K68" t="s">
+        <v>115</v>
+      </c>
+      <c r="L68" t="s">
+        <v>116</v>
+      </c>
+      <c r="M68" t="s">
+        <v>117</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="O68" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="P68" s="12" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
         <v>252</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C69" s="22" t="s">
         <v>524</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D69" s="22" t="s">
         <v>525</v>
       </c>
-      <c r="E67" s="24" t="s">
+      <c r="E69" s="24" t="s">
         <v>526</v>
       </c>
-      <c r="G67" s="12"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="L67" t="s">
-        <v>748</v>
-      </c>
-      <c r="N67" s="12" t="s">
-        <v>660</v>
-      </c>
-      <c r="O67" s="25" t="s">
-        <v>713</v>
-      </c>
-      <c r="P67" s="12" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="2" customFormat="1">
-      <c r="A68" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>527</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="F68" s="14"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="4"/>
-      <c r="J68" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="N68" s="12" t="s">
-        <v>661</v>
-      </c>
-      <c r="O68" s="26" t="s">
-        <v>714</v>
-      </c>
-      <c r="P68" s="12" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" s="2" customFormat="1">
-      <c r="A69" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="E69" s="24" t="s">
-        <v>532</v>
-      </c>
-      <c r="F69" s="14"/>
       <c r="G69" s="12"/>
       <c r="H69" s="4"/>
-      <c r="J69" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>751</v>
+      <c r="I69" s="1"/>
+      <c r="J69" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="L69" t="s">
+        <v>748</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>662</v>
-      </c>
-      <c r="O69" s="26" t="s">
-        <v>715</v>
+        <v>660</v>
+      </c>
+      <c r="O69" s="25" t="s">
+        <v>713</v>
       </c>
       <c r="P69" s="12" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="70" spans="1:16" s="2" customFormat="1">
@@ -5649,89 +5609,69 @@
         <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>596</v>
+        <v>248</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="F70" s="14"/>
-      <c r="G70" s="12" t="s">
-        <v>333</v>
-      </c>
+      <c r="G70" s="12"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>118</v>
+      <c r="J70" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>119</v>
+        <v>749</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O70" s="26" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" s="12" customFormat="1">
-      <c r="A71" s="12" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="2" customFormat="1">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>598</v>
-      </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="14" t="s">
-        <v>607</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>609</v>
-      </c>
-      <c r="I71" s="12" t="s">
-        <v>610</v>
-      </c>
-      <c r="J71" s="12" t="s">
-        <v>612</v>
-      </c>
-      <c r="K71" s="12" t="s">
-        <v>608</v>
-      </c>
-      <c r="L71" s="12" t="s">
-        <v>611</v>
-      </c>
-      <c r="M71" s="12" t="s">
-        <v>789</v>
+      <c r="B71" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="4"/>
+      <c r="J71" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>751</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>664</v>
-      </c>
-      <c r="O71" s="25" t="s">
-        <v>717</v>
+        <v>662</v>
+      </c>
+      <c r="O71" s="26" t="s">
+        <v>715</v>
       </c>
       <c r="P71" s="12" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="2" customFormat="1">
@@ -5739,143 +5679,139 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H72" s="4"/>
+      <c r="I72" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>663</v>
+      </c>
+      <c r="O72" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="P72" s="12" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" s="12" customFormat="1">
+      <c r="A73" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="I73" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="J73" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="K73" s="12" t="s">
+        <v>608</v>
+      </c>
+      <c r="L73" s="12" t="s">
+        <v>611</v>
+      </c>
+      <c r="M73" s="12" t="s">
+        <v>789</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="O73" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="P73" s="12" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F74" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G74" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="H72" s="4" t="s">
+      <c r="H74" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="M74" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N72" s="12" t="s">
+      <c r="N74" s="12" t="s">
         <v>665</v>
       </c>
-      <c r="O72" s="25" t="s">
+      <c r="O74" s="25" t="s">
         <v>718</v>
       </c>
-      <c r="P72" s="12" t="s">
+      <c r="P74" s="12" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" s="2" customFormat="1">
-      <c r="A73" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H73" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N73" s="12" t="s">
-        <v>666</v>
-      </c>
-      <c r="O73" s="26" t="s">
-        <v>719</v>
-      </c>
-      <c r="P73" s="12" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="12" customFormat="1">
-      <c r="A74" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>766</v>
-      </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="14" t="s">
-        <v>772</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>772</v>
-      </c>
-      <c r="H74" s="22" t="s">
-        <v>772</v>
-      </c>
-      <c r="I74" s="22" t="s">
-        <v>770</v>
-      </c>
-      <c r="J74" s="22" t="s">
-        <v>773</v>
-      </c>
-      <c r="K74" s="12" t="s">
-        <v>767</v>
-      </c>
-      <c r="L74" s="12" t="s">
-        <v>768</v>
-      </c>
-      <c r="M74" s="12" t="s">
-        <v>769</v>
-      </c>
-      <c r="N74" s="12" t="s">
-        <v>770</v>
-      </c>
-      <c r="O74" s="14" t="s">
-        <v>771</v>
-      </c>
-      <c r="P74" s="12" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="2" customFormat="1">
@@ -5883,69 +5819,93 @@
         <v>70</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>247</v>
+        <v>81</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="F75" s="14"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="4"/>
-      <c r="J75" s="6" t="s">
-        <v>285</v>
+        <v>541</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H75" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>752</v>
+        <v>84</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>667</v>
-      </c>
-      <c r="O75" s="25" t="s">
-        <v>720</v>
+        <v>666</v>
+      </c>
+      <c r="O75" s="26" t="s">
+        <v>719</v>
       </c>
       <c r="P75" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" s="2" customFormat="1">
-      <c r="A76" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="12" customFormat="1">
+      <c r="A76" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>546</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>547</v>
-      </c>
-      <c r="F76" s="14"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="4"/>
-      <c r="J76" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>753</v>
+      <c r="B76" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="14" t="s">
+        <v>772</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>772</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>772</v>
+      </c>
+      <c r="I76" s="22" t="s">
+        <v>770</v>
+      </c>
+      <c r="J76" s="22" t="s">
+        <v>773</v>
+      </c>
+      <c r="K76" s="12" t="s">
+        <v>767</v>
+      </c>
+      <c r="L76" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="M76" s="12" t="s">
+        <v>769</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>668</v>
-      </c>
-      <c r="O76" s="25" t="s">
-        <v>721</v>
+        <v>770</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>771</v>
       </c>
       <c r="P76" s="12" t="s">
-        <v>837</v>
+        <v>766</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="2" customFormat="1">
@@ -5953,49 +5913,34 @@
         <v>70</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>76</v>
+        <v>247</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="G77" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>78</v>
+        <v>544</v>
+      </c>
+      <c r="F77" s="14"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="4"/>
+      <c r="J77" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>80</v>
+        <v>752</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>669</v>
-      </c>
-      <c r="O77" s="26" t="s">
-        <v>722</v>
+        <v>667</v>
+      </c>
+      <c r="O77" s="25" t="s">
+        <v>720</v>
       </c>
       <c r="P77" s="12" t="s">
-        <v>838</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="2" customFormat="1">
@@ -6003,522 +5948,607 @@
         <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="F78" s="14"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="4"/>
+      <c r="J78" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="O78" s="25" t="s">
+        <v>721</v>
+      </c>
+      <c r="P78" s="12" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" s="2" customFormat="1">
+      <c r="A79" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="O79" s="26" t="s">
+        <v>722</v>
+      </c>
+      <c r="P79" s="12" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="2" customFormat="1">
+      <c r="A80" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C80" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="D80" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="E78" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="F78" s="20" t="s">
+      <c r="F80" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="G78" s="12" t="s">
+      <c r="G80" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="H78" s="4" t="s">
+      <c r="H80" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I80" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J80" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K80" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="N78" s="12" t="s">
+      <c r="N80" s="12" t="s">
         <v>670</v>
       </c>
-      <c r="O78" s="25" t="s">
+      <c r="O80" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="P78" s="12" t="s">
+      <c r="P80" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
-      <c r="A79" t="s">
+    <row r="81" spans="1:16">
+      <c r="A81" t="s">
         <v>171</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
         <v>172</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C81" s="22" t="s">
         <v>553</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="D81" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="E79" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>555</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F81" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="G79" s="12" t="s">
+      <c r="G81" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="H79" s="4" t="s">
+      <c r="H81" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J81" t="s">
         <v>173</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K81" t="s">
         <v>174</v>
       </c>
-      <c r="L79" t="s">
+      <c r="L81" t="s">
         <v>172</v>
       </c>
-      <c r="M79" t="s">
+      <c r="M81" t="s">
         <v>173</v>
       </c>
-      <c r="N79" s="12" t="s">
+      <c r="N81" s="12" t="s">
         <v>671</v>
       </c>
-      <c r="O79" s="25" t="s">
+      <c r="O81" s="25" t="s">
         <v>724</v>
       </c>
-      <c r="P79" s="12" t="s">
+      <c r="P81" s="12" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
-      <c r="A80" t="s">
+    <row r="82" spans="1:16">
+      <c r="A82" t="s">
         <v>171</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C82" s="22" t="s">
         <v>556</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="D82" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="F80" s="16" t="s">
+      <c r="F82" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="G80" s="12" t="s">
+      <c r="G82" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="H82" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J82" t="s">
         <v>176</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K82" t="s">
         <v>177</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L82" t="s">
         <v>178</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M82" t="s">
         <v>179</v>
       </c>
-      <c r="N80" s="12" t="s">
+      <c r="N82" s="12" t="s">
         <v>672</v>
       </c>
-      <c r="O80" s="26" t="s">
+      <c r="O82" s="26" t="s">
         <v>725</v>
       </c>
-      <c r="P80" s="12" t="s">
+      <c r="P82" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="28.8">
-      <c r="A81" s="12" t="s">
-        <v>631</v>
-      </c>
-      <c r="B81" t="s">
-        <v>183</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="D81" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H81" s="4"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L81" t="s">
-        <v>754</v>
-      </c>
-      <c r="O81" s="25" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="28.8">
-      <c r="A82" s="12" t="s">
-        <v>631</v>
-      </c>
-      <c r="B82" t="s">
-        <v>181</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="G82" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H82" s="4"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="L82" t="s">
-        <v>755</v>
-      </c>
-      <c r="O82" s="25" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="28.8">
+    <row r="83" spans="1:16" ht="28.8">
       <c r="A83" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="F83" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G83" s="12"/>
+        <v>561</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>339</v>
+      </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L83" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="28.8">
+        <v>754</v>
+      </c>
+      <c r="O83" s="25" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="28.8">
       <c r="A84" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L84" t="s">
-        <v>757</v>
-      </c>
-      <c r="O84" s="26" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15">
+        <v>755</v>
+      </c>
+      <c r="O84" s="25" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="28.8">
       <c r="A85" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B85" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="E85" s="24" t="s">
-        <v>573</v>
+        <v>566</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>567</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>342</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="G85" s="12"/>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L85" t="s">
-        <v>758</v>
-      </c>
-      <c r="O85" s="26" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="28.8">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="28.8">
       <c r="A86" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L86" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O86" s="26" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="28.8">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>579</v>
+        <v>572</v>
+      </c>
+      <c r="E87" s="24" t="s">
+        <v>573</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="1"/>
       <c r="J87" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L87" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="O87" s="26" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="28.8">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="28.8">
       <c r="A88" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="E88" s="22" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="1"/>
       <c r="J88" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L88" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="O88" s="26" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="28.8">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="28.8">
       <c r="A89" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="E89" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="F89" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="G89" s="13" t="s">
-        <v>346</v>
+        <v>579</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="1"/>
       <c r="J89" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L89" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="O89" s="26" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="28.8">
       <c r="A90" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="E90" s="22" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="1"/>
       <c r="J90" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="L90" s="12" t="s">
-        <v>762</v>
+        <v>294</v>
+      </c>
+      <c r="L90" t="s">
+        <v>761</v>
       </c>
       <c r="O90" s="26" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="28.8">
       <c r="A91" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="E91" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G91" s="12" t="s">
-        <v>348</v>
+        <v>585</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>346</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="1"/>
       <c r="J91" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="L91" t="s">
+        <v>764</v>
+      </c>
+      <c r="O91" s="26" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
+      <c r="A92" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H92" s="4"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="L92" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="O92" s="26" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
+      <c r="A93" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B93" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="H93" s="4"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L91" s="12" t="s">
+      <c r="L93" s="12" t="s">
         <v>763</v>
       </c>
-      <c r="O91" s="26" t="s">
+      <c r="O93" s="26" t="s">
         <v>735</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P91" xr:uid="{A4C0DE7B-B5FD-4B2E-A3DB-E7CF10EF5495}"/>
+  <autoFilter ref="A1:P93" xr:uid="{A4C0DE7B-B5FD-4B2E-A3DB-E7CF10EF5495}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Report credible interval for Bayesian models (#1203)
* reporting credible interval for Bayesian models

* increment version number
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEBB220-0866-411A-B0FA-C0FAE5377451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EFEB1-DE09-4DD9-8406-00E0EFA297A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="843">
   <si>
     <t>context</t>
   </si>
@@ -2662,6 +2662,12 @@
   </si>
   <si>
     <t>Pearsons kjikvadrattest</t>
+  </si>
+  <si>
+    <t>CI = Credible Interval</t>
+  </si>
+  <si>
+    <t>Credible Interval</t>
   </si>
 </sst>
 </file>
@@ -3121,13 +3127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4398,134 +4404,78 @@
         <v>813</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
-      <c r="A37" t="s">
+    <row r="37" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="A37" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J37" t="s">
-        <v>68</v>
-      </c>
-      <c r="K37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L37" t="s">
-        <v>743</v>
-      </c>
-      <c r="M37" t="s">
-        <v>785</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>644</v>
-      </c>
-      <c r="O37" s="26" t="s">
-        <v>696</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" t="s">
+      <c r="B37" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="J38" t="s">
-        <v>51</v>
-      </c>
-      <c r="K38" t="s">
-        <v>52</v>
-      </c>
-      <c r="L38" t="s">
-        <v>53</v>
-      </c>
-      <c r="M38" t="s">
-        <v>54</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>645</v>
-      </c>
-      <c r="O38" s="25" t="s">
-        <v>697</v>
-      </c>
-      <c r="P38" s="12" t="s">
-        <v>218</v>
-      </c>
+      <c r="B38" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="G39" s="12"/>
+        <v>459</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>319</v>
+      </c>
       <c r="H39" s="4" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>193</v>
+        <v>217</v>
+      </c>
+      <c r="J39" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" t="s">
+        <v>743</v>
+      </c>
+      <c r="M39" t="s">
+        <v>785</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>193</v>
+        <v>644</v>
+      </c>
+      <c r="O39" s="26" t="s">
+        <v>696</v>
       </c>
       <c r="P39" s="12" t="s">
-        <v>193</v>
+        <v>814</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -4533,49 +4483,49 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J40" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="K40" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="L40" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="M40" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>646</v>
-      </c>
-      <c r="O40" s="26" t="s">
-        <v>698</v>
+        <v>645</v>
+      </c>
+      <c r="O40" s="25" t="s">
+        <v>697</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>815</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -4583,29 +4533,29 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>816</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -4613,49 +4563,49 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="J42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="L42" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M42" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O42" s="26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="P42" s="12" t="s">
-        <v>59</v>
+        <v>815</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -4663,24 +4613,29 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="G43" s="12"/>
-      <c r="H43" s="4"/>
+      <c r="H43" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="I43" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="P43" s="12" t="s">
-        <v>198</v>
+        <v>816</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -4688,24 +4643,49 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>479</v>
-      </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="4"/>
+        <v>473</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="I44" s="1" t="s">
-        <v>194</v>
+        <v>59</v>
+      </c>
+      <c r="J44" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="O44" s="26" t="s">
+        <v>699</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -4713,54 +4693,74 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P45" s="12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="G46" s="12"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
         <v>196</v>
       </c>
-      <c r="P45" s="12" t="s">
+      <c r="C47" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>482</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="P47" s="12" t="s">
         <v>817</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" s="12" customFormat="1">
-      <c r="A46" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>632</v>
-      </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="14"/>
-      <c r="P46" s="12" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="12" customFormat="1">
-      <c r="A47" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>633</v>
-      </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="14"/>
-      <c r="P47" s="12" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="12" customFormat="1">
@@ -4768,78 +4768,50 @@
         <v>49</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="14"/>
-      <c r="L48" s="12" t="s">
+      <c r="P48" s="12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" s="12" customFormat="1">
+      <c r="A49" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="14"/>
+      <c r="P49" s="12" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" s="12" customFormat="1">
+      <c r="A50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="14"/>
+      <c r="L50" s="12" t="s">
         <v>744</v>
       </c>
-      <c r="M48" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>786</v>
       </c>
-      <c r="P48" s="12" t="s">
+      <c r="P50" s="12" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>483</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>484</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>485</v>
-      </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="N49" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="P49" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>487</v>
-      </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="N50" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="P50" s="12" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -4847,187 +4819,155 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="P51" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C53" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D53" s="24" t="s">
         <v>489</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E53" s="24" t="s">
         <v>490</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J53" t="s">
         <v>56</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K53" t="s">
         <v>55</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L53" t="s">
         <v>57</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M53" t="s">
         <v>58</v>
       </c>
-      <c r="N51" s="12" t="s">
+      <c r="N53" s="12" t="s">
         <v>648</v>
       </c>
-      <c r="O51" s="26" t="s">
+      <c r="O53" s="26" t="s">
         <v>700</v>
       </c>
-      <c r="P51" s="12" t="s">
+      <c r="P53" s="12" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="12" customFormat="1">
-      <c r="A52" s="12" t="s">
+    <row r="54" spans="1:16" s="12" customFormat="1">
+      <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="14"/>
-      <c r="L52" s="12" t="s">
+      <c r="C54" s="22"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="14"/>
+      <c r="L54" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="N52" s="12" t="s">
+      <c r="N54" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="O52" s="25" t="s">
+      <c r="O54" s="25" t="s">
         <v>701</v>
       </c>
-      <c r="P52" s="12" t="s">
+      <c r="P54" s="12" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="12" customFormat="1">
-      <c r="A53" s="12" t="s">
+    <row r="55" spans="1:16" s="12" customFormat="1">
+      <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="14"/>
-      <c r="L53" s="12" t="s">
+      <c r="C55" s="22"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="14"/>
+      <c r="L55" s="12" t="s">
         <v>745</v>
       </c>
-      <c r="M53" s="12" t="s">
+      <c r="M55" s="12" t="s">
         <v>787</v>
       </c>
-      <c r="N53" s="12" t="s">
+      <c r="N55" s="12" t="s">
         <v>649</v>
       </c>
-      <c r="P53" s="12" t="s">
+      <c r="P55" s="12" t="s">
         <v>820</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J54" t="s">
-        <v>104</v>
-      </c>
-      <c r="K54" t="s">
-        <v>105</v>
-      </c>
-      <c r="L54" t="s">
-        <v>106</v>
-      </c>
-      <c r="M54" t="s">
-        <v>107</v>
-      </c>
-      <c r="N54" s="12" t="s">
-        <v>650</v>
-      </c>
-      <c r="O54" s="26" t="s">
-        <v>702</v>
-      </c>
-      <c r="P54" s="12" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16">
-      <c r="A55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" t="s">
-        <v>254</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>493</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>494</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I55" s="1"/>
-      <c r="J55" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="L55" t="s">
-        <v>746</v>
-      </c>
-      <c r="N55" s="12" t="s">
-        <v>651</v>
-      </c>
-      <c r="O55" s="26" t="s">
-        <v>703</v>
-      </c>
-      <c r="P55" s="12" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -5035,49 +4975,49 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>497</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>374</v>
+        <v>492</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>372</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J56" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L56" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M56" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="O56" s="26" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -5085,39 +5025,39 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>500</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>375</v>
+        <v>495</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>373</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I57" s="1"/>
-      <c r="J57" s="11" t="s">
-        <v>280</v>
+      <c r="J57" s="12" t="s">
+        <v>279</v>
       </c>
       <c r="L57" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O57" s="26" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -5125,49 +5065,49 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>376</v>
+        <v>497</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>374</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J58" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="K58" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="L58" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="M58" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>654</v>
-      </c>
-      <c r="O58" s="25" t="s">
-        <v>706</v>
+        <v>652</v>
+      </c>
+      <c r="O58" s="26" t="s">
+        <v>704</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>223</v>
+        <v>823</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -5175,49 +5115,39 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>255</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>327</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>500</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="G59" s="12"/>
       <c r="H59" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="K59" t="s">
-        <v>101</v>
+        <v>274</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="L59" t="s">
-        <v>102</v>
-      </c>
-      <c r="M59" s="12" t="s">
-        <v>788</v>
+        <v>747</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>101</v>
+        <v>653</v>
       </c>
       <c r="O59" s="26" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -5225,49 +5155,49 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>240</v>
+        <v>503</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>376</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="J60" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="K60" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="L60" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="M60" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O60" s="25" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>826</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -5275,49 +5205,49 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>597</v>
+        <v>101</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>512</v>
+        <v>505</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>506</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="J61" t="s">
-        <v>603</v>
+        <v>600</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="K61" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="L61" t="s">
-        <v>605</v>
-      </c>
-      <c r="M61" t="s">
-        <v>87</v>
+        <v>102</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>788</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>656</v>
-      </c>
-      <c r="O61" s="25" t="s">
-        <v>709</v>
+        <v>101</v>
+      </c>
+      <c r="O61" s="26" t="s">
+        <v>707</v>
       </c>
       <c r="P61" s="12" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -5325,49 +5255,49 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>515</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>378</v>
+        <v>508</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J62" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K62" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L62" t="s">
-        <v>604</v>
+        <v>92</v>
       </c>
       <c r="M62" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="O62" s="25" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="P62" s="12" t="s">
-        <v>88</v>
+        <v>826</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -5375,49 +5305,49 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>597</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>518</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>243</v>
+        <v>511</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>377</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>90</v>
+        <v>601</v>
       </c>
       <c r="J63" t="s">
-        <v>91</v>
+        <v>603</v>
       </c>
       <c r="K63" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L63" t="s">
-        <v>90</v>
+        <v>605</v>
       </c>
       <c r="M63" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="O63" s="25" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="P63" s="12" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -5425,28 +5355,49 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>88</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>520</v>
-      </c>
-      <c r="G64" s="12"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="9" t="s">
-        <v>250</v>
+        <v>514</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J64" t="s">
+        <v>89</v>
+      </c>
+      <c r="K64" t="s">
+        <v>88</v>
+      </c>
+      <c r="L64" t="s">
+        <v>604</v>
+      </c>
+      <c r="M64" t="s">
+        <v>89</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>250</v>
+        <v>657</v>
+      </c>
+      <c r="O64" s="25" t="s">
+        <v>710</v>
       </c>
       <c r="P64" s="12" t="s">
-        <v>250</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -5454,44 +5405,49 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>523</v>
+        <v>518</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="H65" s="4"/>
+        <v>331</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="I65" s="1" t="s">
-        <v>224</v>
+        <v>90</v>
       </c>
       <c r="J65" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="K65" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="L65" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="M65" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O65" s="25" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="P65" s="12" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -5499,44 +5455,28 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>332</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="G66" s="12"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J66" t="s">
-        <v>114</v>
-      </c>
-      <c r="K66" t="s">
-        <v>115</v>
-      </c>
-      <c r="L66" t="s">
-        <v>116</v>
-      </c>
-      <c r="M66" t="s">
-        <v>117</v>
+      <c r="I66" s="1"/>
+      <c r="J66" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>659</v>
-      </c>
-      <c r="O66" s="25" t="s">
-        <v>712</v>
+        <v>250</v>
       </c>
       <c r="P66" s="12" t="s">
-        <v>830</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -5544,104 +5484,124 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H67" s="4"/>
+      <c r="I67" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J67" t="s">
+        <v>114</v>
+      </c>
+      <c r="K67" t="s">
+        <v>115</v>
+      </c>
+      <c r="L67" t="s">
+        <v>116</v>
+      </c>
+      <c r="M67" t="s">
+        <v>117</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="O67" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="P67" s="12" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H68" s="4"/>
+      <c r="I68" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J68" t="s">
+        <v>114</v>
+      </c>
+      <c r="K68" t="s">
+        <v>115</v>
+      </c>
+      <c r="L68" t="s">
+        <v>116</v>
+      </c>
+      <c r="M68" t="s">
+        <v>117</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="O68" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="P68" s="12" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
         <v>252</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C69" s="22" t="s">
         <v>524</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D69" s="22" t="s">
         <v>525</v>
       </c>
-      <c r="E67" s="24" t="s">
+      <c r="E69" s="24" t="s">
         <v>526</v>
       </c>
-      <c r="G67" s="12"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="L67" t="s">
-        <v>748</v>
-      </c>
-      <c r="N67" s="12" t="s">
-        <v>660</v>
-      </c>
-      <c r="O67" s="25" t="s">
-        <v>713</v>
-      </c>
-      <c r="P67" s="12" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="2" customFormat="1">
-      <c r="A68" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>527</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>528</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="F68" s="14"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="4"/>
-      <c r="J68" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="N68" s="12" t="s">
-        <v>661</v>
-      </c>
-      <c r="O68" s="26" t="s">
-        <v>714</v>
-      </c>
-      <c r="P68" s="12" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" s="2" customFormat="1">
-      <c r="A69" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="E69" s="24" t="s">
-        <v>532</v>
-      </c>
-      <c r="F69" s="14"/>
       <c r="G69" s="12"/>
       <c r="H69" s="4"/>
-      <c r="J69" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>751</v>
+      <c r="I69" s="1"/>
+      <c r="J69" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="L69" t="s">
+        <v>748</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>662</v>
-      </c>
-      <c r="O69" s="26" t="s">
-        <v>715</v>
+        <v>660</v>
+      </c>
+      <c r="O69" s="25" t="s">
+        <v>713</v>
       </c>
       <c r="P69" s="12" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="70" spans="1:16" s="2" customFormat="1">
@@ -5649,89 +5609,69 @@
         <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>596</v>
+        <v>248</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="F70" s="14"/>
-      <c r="G70" s="12" t="s">
-        <v>333</v>
-      </c>
+      <c r="G70" s="12"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>118</v>
+      <c r="J70" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>119</v>
+        <v>749</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O70" s="26" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" s="12" customFormat="1">
-      <c r="A71" s="12" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="2" customFormat="1">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>598</v>
-      </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="14" t="s">
-        <v>607</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>609</v>
-      </c>
-      <c r="I71" s="12" t="s">
-        <v>610</v>
-      </c>
-      <c r="J71" s="12" t="s">
-        <v>612</v>
-      </c>
-      <c r="K71" s="12" t="s">
-        <v>608</v>
-      </c>
-      <c r="L71" s="12" t="s">
-        <v>611</v>
-      </c>
-      <c r="M71" s="12" t="s">
-        <v>789</v>
+      <c r="B71" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="4"/>
+      <c r="J71" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>751</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>664</v>
-      </c>
-      <c r="O71" s="25" t="s">
-        <v>717</v>
+        <v>662</v>
+      </c>
+      <c r="O71" s="26" t="s">
+        <v>715</v>
       </c>
       <c r="P71" s="12" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="2" customFormat="1">
@@ -5739,143 +5679,139 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H72" s="4"/>
+      <c r="I72" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>663</v>
+      </c>
+      <c r="O72" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="P72" s="12" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" s="12" customFormat="1">
+      <c r="A73" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="I73" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="J73" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="K73" s="12" t="s">
+        <v>608</v>
+      </c>
+      <c r="L73" s="12" t="s">
+        <v>611</v>
+      </c>
+      <c r="M73" s="12" t="s">
+        <v>789</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="O73" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="P73" s="12" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>537</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F74" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G74" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="H72" s="4" t="s">
+      <c r="H74" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="M74" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N72" s="12" t="s">
+      <c r="N74" s="12" t="s">
         <v>665</v>
       </c>
-      <c r="O72" s="25" t="s">
+      <c r="O74" s="25" t="s">
         <v>718</v>
       </c>
-      <c r="P72" s="12" t="s">
+      <c r="P74" s="12" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" s="2" customFormat="1">
-      <c r="A73" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>541</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H73" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N73" s="12" t="s">
-        <v>666</v>
-      </c>
-      <c r="O73" s="26" t="s">
-        <v>719</v>
-      </c>
-      <c r="P73" s="12" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" s="12" customFormat="1">
-      <c r="A74" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>766</v>
-      </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="14" t="s">
-        <v>772</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>772</v>
-      </c>
-      <c r="H74" s="22" t="s">
-        <v>772</v>
-      </c>
-      <c r="I74" s="22" t="s">
-        <v>770</v>
-      </c>
-      <c r="J74" s="22" t="s">
-        <v>773</v>
-      </c>
-      <c r="K74" s="12" t="s">
-        <v>767</v>
-      </c>
-      <c r="L74" s="12" t="s">
-        <v>768</v>
-      </c>
-      <c r="M74" s="12" t="s">
-        <v>769</v>
-      </c>
-      <c r="N74" s="12" t="s">
-        <v>770</v>
-      </c>
-      <c r="O74" s="14" t="s">
-        <v>771</v>
-      </c>
-      <c r="P74" s="12" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="2" customFormat="1">
@@ -5883,69 +5819,93 @@
         <v>70</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>247</v>
+        <v>81</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="F75" s="14"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="4"/>
-      <c r="J75" s="6" t="s">
-        <v>285</v>
+        <v>541</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H75" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>752</v>
+        <v>84</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>667</v>
-      </c>
-      <c r="O75" s="25" t="s">
-        <v>720</v>
+        <v>666</v>
+      </c>
+      <c r="O75" s="26" t="s">
+        <v>719</v>
       </c>
       <c r="P75" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" s="2" customFormat="1">
-      <c r="A76" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="12" customFormat="1">
+      <c r="A76" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>546</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>547</v>
-      </c>
-      <c r="F76" s="14"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="4"/>
-      <c r="J76" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>753</v>
+      <c r="B76" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="14" t="s">
+        <v>772</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>772</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>772</v>
+      </c>
+      <c r="I76" s="22" t="s">
+        <v>770</v>
+      </c>
+      <c r="J76" s="22" t="s">
+        <v>773</v>
+      </c>
+      <c r="K76" s="12" t="s">
+        <v>767</v>
+      </c>
+      <c r="L76" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="M76" s="12" t="s">
+        <v>769</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>668</v>
-      </c>
-      <c r="O76" s="25" t="s">
-        <v>721</v>
+        <v>770</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>771</v>
       </c>
       <c r="P76" s="12" t="s">
-        <v>837</v>
+        <v>766</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="2" customFormat="1">
@@ -5953,49 +5913,34 @@
         <v>70</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>76</v>
+        <v>247</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="G77" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>78</v>
+        <v>544</v>
+      </c>
+      <c r="F77" s="14"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="4"/>
+      <c r="J77" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>80</v>
+        <v>752</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>669</v>
-      </c>
-      <c r="O77" s="26" t="s">
-        <v>722</v>
+        <v>667</v>
+      </c>
+      <c r="O77" s="25" t="s">
+        <v>720</v>
       </c>
       <c r="P77" s="12" t="s">
-        <v>838</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="2" customFormat="1">
@@ -6003,522 +5948,607 @@
         <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="F78" s="14"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="4"/>
+      <c r="J78" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="O78" s="25" t="s">
+        <v>721</v>
+      </c>
+      <c r="P78" s="12" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" s="2" customFormat="1">
+      <c r="A79" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="O79" s="26" t="s">
+        <v>722</v>
+      </c>
+      <c r="P79" s="12" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="2" customFormat="1">
+      <c r="A80" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C80" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="D80" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="E78" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="F78" s="20" t="s">
+      <c r="F80" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="G78" s="12" t="s">
+      <c r="G80" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="H78" s="4" t="s">
+      <c r="H80" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I80" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J80" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K80" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="N78" s="12" t="s">
+      <c r="N80" s="12" t="s">
         <v>670</v>
       </c>
-      <c r="O78" s="25" t="s">
+      <c r="O80" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="P78" s="12" t="s">
+      <c r="P80" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
-      <c r="A79" t="s">
+    <row r="81" spans="1:16">
+      <c r="A81" t="s">
         <v>171</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
         <v>172</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C81" s="22" t="s">
         <v>553</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="D81" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="E79" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>555</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F81" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="G79" s="12" t="s">
+      <c r="G81" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="H79" s="4" t="s">
+      <c r="H81" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J81" t="s">
         <v>173</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K81" t="s">
         <v>174</v>
       </c>
-      <c r="L79" t="s">
+      <c r="L81" t="s">
         <v>172</v>
       </c>
-      <c r="M79" t="s">
+      <c r="M81" t="s">
         <v>173</v>
       </c>
-      <c r="N79" s="12" t="s">
+      <c r="N81" s="12" t="s">
         <v>671</v>
       </c>
-      <c r="O79" s="25" t="s">
+      <c r="O81" s="25" t="s">
         <v>724</v>
       </c>
-      <c r="P79" s="12" t="s">
+      <c r="P81" s="12" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
-      <c r="A80" t="s">
+    <row r="82" spans="1:16">
+      <c r="A82" t="s">
         <v>171</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C82" s="22" t="s">
         <v>556</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="D82" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="F80" s="16" t="s">
+      <c r="F82" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="G80" s="12" t="s">
+      <c r="G82" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="H82" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J82" t="s">
         <v>176</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K82" t="s">
         <v>177</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L82" t="s">
         <v>178</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M82" t="s">
         <v>179</v>
       </c>
-      <c r="N80" s="12" t="s">
+      <c r="N82" s="12" t="s">
         <v>672</v>
       </c>
-      <c r="O80" s="26" t="s">
+      <c r="O82" s="26" t="s">
         <v>725</v>
       </c>
-      <c r="P80" s="12" t="s">
+      <c r="P82" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="28.8">
-      <c r="A81" s="12" t="s">
-        <v>631</v>
-      </c>
-      <c r="B81" t="s">
-        <v>183</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="D81" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H81" s="4"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L81" t="s">
-        <v>754</v>
-      </c>
-      <c r="O81" s="25" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="28.8">
-      <c r="A82" s="12" t="s">
-        <v>631</v>
-      </c>
-      <c r="B82" t="s">
-        <v>181</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="G82" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="H82" s="4"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="L82" t="s">
-        <v>755</v>
-      </c>
-      <c r="O82" s="25" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="28.8">
+    <row r="83" spans="1:16" ht="28.8">
       <c r="A83" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>567</v>
-      </c>
-      <c r="F83" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G83" s="12"/>
+        <v>561</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>339</v>
+      </c>
       <c r="H83" s="4"/>
       <c r="I83" s="1"/>
       <c r="J83" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L83" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="28.8">
+        <v>754</v>
+      </c>
+      <c r="O83" s="25" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="28.8">
       <c r="A84" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L84" t="s">
-        <v>757</v>
-      </c>
-      <c r="O84" s="26" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15">
+        <v>755</v>
+      </c>
+      <c r="O84" s="25" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="28.8">
       <c r="A85" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B85" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="E85" s="24" t="s">
-        <v>573</v>
+        <v>566</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>567</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>342</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="G85" s="12"/>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L85" t="s">
-        <v>758</v>
-      </c>
-      <c r="O85" s="26" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="28.8">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="28.8">
       <c r="A86" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L86" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O86" s="26" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="28.8">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>579</v>
+        <v>572</v>
+      </c>
+      <c r="E87" s="24" t="s">
+        <v>573</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="1"/>
       <c r="J87" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L87" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="O87" s="26" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="28.8">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="28.8">
       <c r="A88" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="E88" s="22" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="1"/>
       <c r="J88" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L88" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="O88" s="26" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="28.8">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="28.8">
       <c r="A89" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="E89" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="F89" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="G89" s="13" t="s">
-        <v>346</v>
+        <v>579</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="1"/>
       <c r="J89" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L89" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="O89" s="26" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="28.8">
       <c r="A90" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="E90" s="22" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="1"/>
       <c r="J90" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="L90" s="12" t="s">
-        <v>762</v>
+        <v>294</v>
+      </c>
+      <c r="L90" t="s">
+        <v>761</v>
       </c>
       <c r="O90" s="26" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="28.8">
       <c r="A91" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="E91" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="G91" s="12" t="s">
-        <v>348</v>
+        <v>585</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>346</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="1"/>
       <c r="J91" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="L91" t="s">
+        <v>764</v>
+      </c>
+      <c r="O91" s="26" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
+      <c r="A92" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H92" s="4"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="L92" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="O92" s="26" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
+      <c r="A93" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B93" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="H93" s="4"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L91" s="12" t="s">
+      <c r="L93" s="12" t="s">
         <v>763</v>
       </c>
-      <c r="O91" s="26" t="s">
+      <c r="O93" s="26" t="s">
         <v>735</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P91" xr:uid="{A4C0DE7B-B5FD-4B2E-A3DB-E7CF10EF5495}"/>
+  <autoFilter ref="A1:P93" xr:uid="{A4C0DE7B-B5FD-4B2E-A3DB-E7CF10EF5495}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Dutch (nl) to Excel file
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msberends/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EFEB1-DE09-4DD9-8406-00E0EFA297A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B86D9B-1C5F-A046-B45C-9CE55196A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34940" windowHeight="18700" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="911">
   <si>
     <t>context</t>
   </si>
@@ -2668,6 +2668,210 @@
   </si>
   <si>
     <t>Credible Interval</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>Pearson's chi-kwadraattoets</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallistoets</t>
+  </si>
+  <si>
+    <t>Fishers exacte toets</t>
+  </si>
+  <si>
+    <t>Eén-weg-variantieanalyse</t>
+  </si>
+  <si>
+    <t>p-waarde</t>
+  </si>
+  <si>
+    <t>Logistische regressie met willekeurige intercept</t>
+  </si>
+  <si>
+    <t>Statistiek</t>
+  </si>
+  <si>
+    <t>Statistische testen verricht</t>
+  </si>
+  <si>
+    <t>Gepaarde t-toets</t>
+  </si>
+  <si>
+    <t>McNemars chi-kwadraattoets met continuïteitscorrectie</t>
+  </si>
+  <si>
+    <t>McNemars chi-kwadraattoets</t>
+  </si>
+  <si>
+    <t>Mann-Whitney-Wilcoxontoets</t>
+  </si>
+  <si>
+    <t>t-toets</t>
+  </si>
+  <si>
+    <t>Bonferroni-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Benjamini- en Hochberg-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Benjamini- en Yekutieli-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>"False discovery rate"-detectie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Geen correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Hochberg-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Holm-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Hommel-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>q-waarde</t>
+  </si>
+  <si>
+    <t>Betrouwbaarheidsinterval</t>
+  </si>
+  <si>
+    <t>CI = betrouwbaarheidsinterval</t>
+  </si>
+  <si>
+    <t>CI = geloofwaardigheidsinterval</t>
+  </si>
+  <si>
+    <t>Geloofwaardigheidsinterval</t>
+  </si>
+  <si>
+    <t>Hazard-ratio</t>
+  </si>
+  <si>
+    <t>RR = Relatieve risico</t>
+  </si>
+  <si>
+    <t>% ontbrekend</t>
+  </si>
+  <si>
+    <t>% ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>% niet ontbrekend</t>
+  </si>
+  <si>
+    <t>% niet ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>Karakteristiek</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
+  </si>
+  <si>
+    <t>Mediaan</t>
+  </si>
+  <si>
+    <t>N ontbrekend</t>
+  </si>
+  <si>
+    <t>N ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>N niet ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>N niet ontbrekend</t>
+  </si>
+  <si>
+    <t>Aantal obs.</t>
+  </si>
+  <si>
+    <t>Bereik</t>
+  </si>
+  <si>
+    <t>Getoonde statistieken</t>
+  </si>
+  <si>
+    <t>Som</t>
+  </si>
+  <si>
+    <t>Totaal N</t>
+  </si>
+  <si>
+    <t>Totaal N (ongewogen)</t>
+  </si>
+  <si>
+    <t>Onbekend</t>
+  </si>
+  <si>
+    <t>Variantie</t>
+  </si>
+  <si>
+    <t>Percentiel</t>
+  </si>
+  <si>
+    <t>Tijd</t>
+  </si>
+  <si>
+    <t>t-toets aangepast aan complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Van der Waerden's normaalscorentoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Wald-onafhankelijkheidstoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Wilcoxon rank-sum test voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>onafhankelijkheidsbepaling met behulp van de exacte asymptotische verdeling voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>aangepaste Wald-onafhankelijkheidstoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>onafhankelijkheidstoets met zadelpuntbenadering voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>chi-kwadraattoets gecorrigeerd met een 'design effect'-schatting</t>
+  </si>
+  <si>
+    <t>chi-kwadraattoets met Rao en Scott tweede-ordecorrectie</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallistoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Moodstoets voor de mediaan voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Aangepaste R\U00B2</t>
+  </si>
+  <si>
+    <t>log-aannemelijkheidsfunctie</t>
+  </si>
+  <si>
+    <t>Residuele vrijheidsgraden</t>
+  </si>
+  <si>
+    <t>Null vrijheidsgraden</t>
+  </si>
+  <si>
+    <t>Null variantie</t>
+  </si>
+  <si>
+    <t>N events</t>
   </si>
 </sst>
 </file>
@@ -2773,7 +2977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2813,9 +3017,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2831,7 +3036,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3127,36 +3332,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="51.5546875" customWidth="1"/>
-    <col min="3" max="3" width="49" style="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" style="12" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5546875" style="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="38.44140625" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5546875" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51.5" customWidth="1"/>
+    <col min="3" max="3" width="49" style="22" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="53.5" style="22" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.5" style="3" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
-    <col min="10" max="10" width="67" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="51" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="52" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="52.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57.44140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="58.5546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="44.44140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="67" customWidth="1"/>
+    <col min="11" max="11" width="51" customWidth="1"/>
+    <col min="12" max="12" width="52" customWidth="1"/>
+    <col min="13" max="13" width="52.6640625" customWidth="1"/>
+    <col min="14" max="14" width="57.5" customWidth="1"/>
+    <col min="15" max="15" width="58.5" customWidth="1"/>
+    <col min="16" max="16" width="32.1640625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" ht="16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3205,8 +3411,11 @@
       <c r="P1" s="12" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>613</v>
       </c>
@@ -3216,8 +3425,11 @@
       <c r="O2" s="25" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="12" t="s">
         <v>613</v>
       </c>
@@ -3230,8 +3442,11 @@
       <c r="O3" s="12" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="12" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="12" t="s">
         <v>613</v>
       </c>
@@ -3244,8 +3459,11 @@
       <c r="O4" s="25" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="12" t="s">
         <v>613</v>
       </c>
@@ -3258,8 +3476,11 @@
       <c r="O5" s="25" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="12" t="s">
         <v>613</v>
       </c>
@@ -3269,8 +3490,11 @@
       <c r="L6" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="12" t="s">
         <v>613</v>
       </c>
@@ -3280,8 +3504,11 @@
       <c r="L7" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="12" t="s">
         <v>613</v>
       </c>
@@ -3291,16 +3518,22 @@
       <c r="L8" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="12" t="s">
         <v>613</v>
       </c>
       <c r="B9" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="12" t="s">
         <v>613</v>
       </c>
@@ -3310,8 +3543,11 @@
       <c r="L10" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="16">
       <c r="A11" t="s">
         <v>166</v>
       </c>
@@ -3355,8 +3591,11 @@
       <c r="P11" s="12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="16">
       <c r="A12" t="s">
         <v>630</v>
       </c>
@@ -3405,8 +3644,11 @@
       <c r="P12" s="12" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="16">
       <c r="A13" s="12" t="s">
         <v>630</v>
       </c>
@@ -3452,8 +3694,11 @@
       <c r="P13" s="12" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="16">
       <c r="A14" s="12" t="s">
         <v>630</v>
       </c>
@@ -3499,8 +3744,11 @@
       <c r="P14" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16">
       <c r="A15" s="12" t="s">
         <v>630</v>
       </c>
@@ -3549,8 +3797,11 @@
       <c r="P15" s="12" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="16">
       <c r="A16" s="12" t="s">
         <v>630</v>
       </c>
@@ -3599,8 +3850,11 @@
       <c r="P16" s="12" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="16">
       <c r="A17" s="12" t="s">
         <v>630</v>
       </c>
@@ -3644,8 +3898,11 @@
       <c r="P17" s="12" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="16">
       <c r="A18" s="12" t="s">
         <v>630</v>
       </c>
@@ -3694,8 +3951,11 @@
       <c r="P18" s="12" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16">
       <c r="A19" s="12" t="s">
         <v>630</v>
       </c>
@@ -3744,8 +4004,11 @@
       <c r="P19" s="12" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16">
       <c r="A20" s="12" t="s">
         <v>630</v>
       </c>
@@ -3794,8 +4057,11 @@
       <c r="P20" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" s="12" customFormat="1">
+      <c r="Q20" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="12" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>630</v>
       </c>
@@ -3813,8 +4079,11 @@
       <c r="P21" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="12" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16">
       <c r="A22" s="12" t="s">
         <v>630</v>
       </c>
@@ -3860,8 +4129,11 @@
       <c r="P22" s="12" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" s="12" customFormat="1">
+      <c r="Q22" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="12" customFormat="1">
       <c r="A23" s="12" t="s">
         <v>630</v>
       </c>
@@ -3879,8 +4151,11 @@
       <c r="P23" s="12" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" s="12" customFormat="1">
+      <c r="Q23" s="12" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="12" customFormat="1">
       <c r="A24" s="12" t="s">
         <v>630</v>
       </c>
@@ -3898,8 +4173,11 @@
       <c r="P24" s="12" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" s="12" customFormat="1">
+      <c r="Q24" s="12" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" s="12" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>630</v>
       </c>
@@ -3917,8 +4195,11 @@
       <c r="P25" s="12" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="12" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -3964,8 +4245,11 @@
       <c r="P26" s="12" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="16">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -4011,8 +4295,11 @@
       <c r="P27" s="12" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="12" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="16">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -4058,8 +4345,11 @@
       <c r="P28" s="12" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="12" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="16">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -4105,8 +4395,11 @@
       <c r="P29" s="12" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="27" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="16">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -4152,8 +4445,11 @@
       <c r="P30" s="12" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="16">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -4199,8 +4495,11 @@
       <c r="P31" s="12" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="12" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="16">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -4246,8 +4545,11 @@
       <c r="P32" s="12" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="12" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="16">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -4293,8 +4595,11 @@
       <c r="P33" s="12" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="12" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="16">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -4343,8 +4648,11 @@
       <c r="P34" s="12" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" ht="15">
+      <c r="Q34" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="16">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -4379,8 +4687,11 @@
       <c r="P35" s="12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="Q35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="12" customFormat="1" ht="16">
       <c r="A36" s="12" t="s">
         <v>49</v>
       </c>
@@ -4403,8 +4714,11 @@
       <c r="P36" s="12" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="Q36" s="12" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="12" customFormat="1" ht="16">
       <c r="A37" s="12" t="s">
         <v>49</v>
       </c>
@@ -4415,8 +4729,11 @@
       <c r="D37" s="23"/>
       <c r="E37" s="22"/>
       <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="Q37" s="12" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="12" customFormat="1" ht="16">
       <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
@@ -4427,8 +4744,11 @@
       <c r="D38" s="23"/>
       <c r="E38" s="22"/>
       <c r="F38" s="16"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="12" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="16">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -4477,8 +4797,11 @@
       <c r="P39" s="12" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="16">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -4527,8 +4850,11 @@
       <c r="P40" s="12" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="16">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -4557,8 +4883,11 @@
       <c r="P41" s="12" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="16">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -4607,8 +4936,11 @@
       <c r="P42" s="12" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="16">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -4637,8 +4969,11 @@
       <c r="P43" s="12" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="16">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -4687,8 +5022,11 @@
       <c r="P44" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="16">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -4712,8 +5050,11 @@
       <c r="P45" s="12" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="16">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4737,8 +5078,11 @@
       <c r="P46" s="12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="Q46" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="16">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -4762,8 +5106,11 @@
       <c r="P47" s="12" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" s="12" customFormat="1">
+      <c r="Q47" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" s="12" customFormat="1">
       <c r="A48" s="12" t="s">
         <v>49</v>
       </c>
@@ -4777,8 +5124,11 @@
       <c r="P48" s="12" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" s="12" customFormat="1">
+      <c r="Q48" s="12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
         <v>49</v>
       </c>
@@ -4792,8 +5142,11 @@
       <c r="P49" s="12" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" s="12" customFormat="1">
+      <c r="Q49" s="12" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" s="12" customFormat="1">
       <c r="A50" s="12" t="s">
         <v>49</v>
       </c>
@@ -4813,8 +5166,11 @@
       <c r="P50" s="12" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="Q50" s="12" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="16">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -4841,8 +5197,11 @@
       <c r="P51" s="12" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="Q51" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="16">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4871,8 +5230,11 @@
       <c r="P52" s="12" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="Q52" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="16">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -4921,8 +5283,11 @@
       <c r="P53" s="12" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" s="12" customFormat="1">
+      <c r="Q53" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="12" customFormat="1">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -4945,8 +5310,11 @@
       <c r="P54" s="12" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" s="12" customFormat="1">
+      <c r="Q54" s="12" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="12" customFormat="1">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
@@ -4969,8 +5337,11 @@
       <c r="P55" s="12" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="56" spans="1:16">
+      <c r="Q55" s="12" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="16">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -5019,8 +5390,11 @@
       <c r="P56" s="12" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="16">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -5059,8 +5433,11 @@
       <c r="P57" s="12" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57" s="12" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="16">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -5109,8 +5486,11 @@
       <c r="P58" s="12" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="16">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -5149,8 +5529,11 @@
       <c r="P59" s="12" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" s="12" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="16">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -5199,8 +5582,11 @@
       <c r="P60" s="12" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="16">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -5249,8 +5635,11 @@
       <c r="P61" s="12" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="16">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -5299,8 +5688,11 @@
       <c r="P62" s="12" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="16">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -5349,8 +5741,11 @@
       <c r="P63" s="12" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="16">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -5399,8 +5794,11 @@
       <c r="P64" s="12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="16">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -5449,8 +5847,11 @@
       <c r="P65" s="12" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="16">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -5478,8 +5879,11 @@
       <c r="P66" s="12" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="16">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -5523,8 +5927,11 @@
       <c r="P67" s="12" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="16">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -5568,8 +5975,11 @@
       <c r="P68" s="12" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="16">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -5603,8 +6013,11 @@
       <c r="P69" s="12" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" s="2" customFormat="1">
+      <c r="Q69" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A70" s="2" t="s">
         <v>70</v>
       </c>
@@ -5638,8 +6051,11 @@
       <c r="P70" s="12" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" s="2" customFormat="1">
+      <c r="Q70" s="12" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -5673,8 +6089,11 @@
       <c r="P71" s="12" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" s="2" customFormat="1">
+      <c r="Q71" s="12" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -5719,8 +6138,11 @@
       <c r="P72" s="12" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" s="12" customFormat="1">
+      <c r="Q72" s="2" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="12" customFormat="1">
       <c r="A73" s="12" t="s">
         <v>70</v>
       </c>
@@ -5763,8 +6185,11 @@
       <c r="P73" s="12" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" s="2" customFormat="1">
+      <c r="Q73" s="12" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -5813,8 +6238,11 @@
       <c r="P74" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" s="2" customFormat="1">
+      <c r="Q74" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A75" s="2" t="s">
         <v>70</v>
       </c>
@@ -5863,8 +6291,11 @@
       <c r="P75" s="12" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" s="12" customFormat="1">
+      <c r="Q75" s="2" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" s="12" customFormat="1" ht="16">
       <c r="A76" s="12" t="s">
         <v>70</v>
       </c>
@@ -5907,8 +6338,11 @@
       <c r="P76" s="12" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" s="2" customFormat="1">
+      <c r="Q76" s="12" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A77" s="2" t="s">
         <v>70</v>
       </c>
@@ -5942,8 +6376,11 @@
       <c r="P77" s="12" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" s="2" customFormat="1">
+      <c r="Q77" s="2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
@@ -5977,8 +6414,11 @@
       <c r="P78" s="12" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" s="2" customFormat="1">
+      <c r="Q78" s="2" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A79" s="2" t="s">
         <v>70</v>
       </c>
@@ -6027,8 +6467,11 @@
       <c r="P79" s="12" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" s="2" customFormat="1">
+      <c r="Q79" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" s="2" customFormat="1" ht="16">
       <c r="A80" s="2" t="s">
         <v>70</v>
       </c>
@@ -6077,8 +6520,11 @@
       <c r="P80" s="12" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="Q80" s="2" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="16">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -6127,8 +6573,11 @@
       <c r="P81" s="12" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" ht="16">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -6177,8 +6626,11 @@
       <c r="P82" s="12" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" ht="28.8">
+      <c r="Q82" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" ht="32">
       <c r="A83" s="12" t="s">
         <v>631</v>
       </c>
@@ -6211,8 +6663,11 @@
       <c r="O83" s="25" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" ht="28.8">
+      <c r="Q83" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" ht="32">
       <c r="A84" s="12" t="s">
         <v>631</v>
       </c>
@@ -6245,8 +6700,11 @@
       <c r="O84" s="25" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" ht="28.8">
+      <c r="Q84" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" ht="16">
       <c r="A85" s="12" t="s">
         <v>631</v>
       </c>
@@ -6274,8 +6732,11 @@
       <c r="L85" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" ht="28.8">
+      <c r="Q85" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" ht="16">
       <c r="A86" s="12" t="s">
         <v>631</v>
       </c>
@@ -6308,8 +6769,11 @@
       <c r="O86" s="26" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="Q86" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="16">
       <c r="A87" s="12" t="s">
         <v>631</v>
       </c>
@@ -6342,8 +6806,11 @@
       <c r="O87" s="26" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" ht="28.8">
+      <c r="Q87" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" ht="32">
       <c r="A88" s="12" t="s">
         <v>631</v>
       </c>
@@ -6376,8 +6843,11 @@
       <c r="O88" s="26" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" ht="28.8">
+      <c r="Q88" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="32">
       <c r="A89" s="12" t="s">
         <v>631</v>
       </c>
@@ -6410,8 +6880,11 @@
       <c r="O89" s="26" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" ht="28.8">
+      <c r="Q89" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" ht="32">
       <c r="A90" s="12" t="s">
         <v>631</v>
       </c>
@@ -6444,8 +6917,11 @@
       <c r="O90" s="26" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" ht="28.8">
+      <c r="Q90" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" ht="32">
       <c r="A91" s="12" t="s">
         <v>631</v>
       </c>
@@ -6478,8 +6954,11 @@
       <c r="O91" s="26" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="Q91" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="16">
       <c r="A92" s="12" t="s">
         <v>631</v>
       </c>
@@ -6512,8 +6991,11 @@
       <c r="O92" s="26" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="93" spans="1:16">
+      <c r="Q92" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="16">
       <c r="A93" s="12" t="s">
         <v>631</v>
       </c>
@@ -6545,6 +7027,9 @@
       </c>
       <c r="O93" s="26" t="s">
         <v>735</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Dutch language (#1302)
* Add Dutch (nl) to Excel file

* Update theme_gtsummary.R

* run internal_data

* redoc

* increment version number

Co-authored-by: Daniel Sjoberg <danield.sjoberg@gmail.com>
</commit_message>
<xml_diff>
--- a/data-raw/gtsummary_translated.xlsx
+++ b/data-raw/gtsummary_translated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EFEB1-DE09-4DD9-8406-00E0EFA297A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155BCB52-176D-45A4-B27F-55F98C027CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24D5C74B-D2E9-42BC-9756-BFD64AB81539}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="912">
   <si>
     <t>context</t>
   </si>
@@ -2668,6 +2668,213 @@
   </si>
   <si>
     <t>Credible Interval</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Aangepaste R\U00B2</t>
+  </si>
+  <si>
+    <t>log-aannemelijkheidsfunctie</t>
+  </si>
+  <si>
+    <t>Residuele vrijheidsgraden</t>
+  </si>
+  <si>
+    <t>Null variantie</t>
+  </si>
+  <si>
+    <t>Null vrijheidsgraden</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>Pearson's chi-kwadraattoets</t>
+  </si>
+  <si>
+    <t>Fishers exacte toets</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallistoets</t>
+  </si>
+  <si>
+    <t>Eén-weg-variantieanalyse</t>
+  </si>
+  <si>
+    <t>p-waarde</t>
+  </si>
+  <si>
+    <t>Logistische regressie met willekeurige intercept</t>
+  </si>
+  <si>
+    <t>Statistiek</t>
+  </si>
+  <si>
+    <t>Statistische testen verricht</t>
+  </si>
+  <si>
+    <t>t-toets</t>
+  </si>
+  <si>
+    <t>Mann-Whitney-Wilcoxontoets</t>
+  </si>
+  <si>
+    <t>Gepaarde t-toets</t>
+  </si>
+  <si>
+    <t>McNemars chi-kwadraattoets met continuïteitscorrectie</t>
+  </si>
+  <si>
+    <t>McNemars chi-kwadraattoets</t>
+  </si>
+  <si>
+    <t>Benjamini- en Hochberg-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Benjamini- en Yekutieli-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Bonferroni-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>"False discovery rate"-detectie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Hochberg-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Holm-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Hommel-correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>Geen correctie voor multipele toetsen</t>
+  </si>
+  <si>
+    <t>q-waarde</t>
+  </si>
+  <si>
+    <t>CI = geloofwaardigheidsinterval</t>
+  </si>
+  <si>
+    <t>Geloofwaardigheidsinterval</t>
+  </si>
+  <si>
+    <t>CI = betrouwbaarheidsinterval</t>
+  </si>
+  <si>
+    <t>Betrouwbaarheidsinterval</t>
+  </si>
+  <si>
+    <t>Hazard-ratio</t>
+  </si>
+  <si>
+    <t>RR = Relatieve risico</t>
+  </si>
+  <si>
+    <t>% ontbrekend</t>
+  </si>
+  <si>
+    <t>% ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>% niet ontbrekend</t>
+  </si>
+  <si>
+    <t>% niet ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>Karakteristiek</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
+  </si>
+  <si>
+    <t>Mediaan</t>
+  </si>
+  <si>
+    <t>N ontbrekend</t>
+  </si>
+  <si>
+    <t>N ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>N niet ontbrekend</t>
+  </si>
+  <si>
+    <t>N niet ontbrekend (ongewogen)</t>
+  </si>
+  <si>
+    <t>Aantal obs.</t>
+  </si>
+  <si>
+    <t>Bereik</t>
+  </si>
+  <si>
+    <t>Getoonde statistieken</t>
+  </si>
+  <si>
+    <t>Som</t>
+  </si>
+  <si>
+    <t>Totaal N</t>
+  </si>
+  <si>
+    <t>Totaal N (ongewogen)</t>
+  </si>
+  <si>
+    <t>Onbekend</t>
+  </si>
+  <si>
+    <t>Variantie</t>
+  </si>
+  <si>
+    <t>Percentiel</t>
+  </si>
+  <si>
+    <t>Tijd</t>
+  </si>
+  <si>
+    <t>aangepaste Wald-onafhankelijkheidstoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>chi-kwadraattoets gecorrigeerd met een 'design effect'-schatting</t>
+  </si>
+  <si>
+    <t>chi-kwadraattoets met Rao en Scott tweede-ordecorrectie</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallistoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Moodstoets voor de mediaan voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>onafhankelijkheidstoets met zadelpuntbenadering voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>onafhankelijkheidsbepaling met behulp van de exacte asymptotische verdeling voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>t-toets aangepast aan complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Van der Waerden's normaalscorentoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Wald-onafhankelijkheidstoets voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>Wilcoxon rank-sum test voor complexe enquêtesteekproeven</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>tot</t>
   </si>
 </sst>
 </file>
@@ -2773,7 +2980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2813,6 +3020,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3127,13 +3335,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}">
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -3154,9 +3362,10 @@
     <col min="14" max="14" width="57.44140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="58.5546875" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="44.44140625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="43.77734375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3205,8 +3414,11 @@
       <c r="P1" s="12" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="12" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>613</v>
       </c>
@@ -3217,7 +3429,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="12" t="s">
         <v>613</v>
       </c>
@@ -3230,8 +3442,11 @@
       <c r="O3" s="12" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="12" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="12" t="s">
         <v>613</v>
       </c>
@@ -3244,8 +3459,11 @@
       <c r="O4" s="25" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="12" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="12" t="s">
         <v>613</v>
       </c>
@@ -3258,8 +3476,11 @@
       <c r="O5" s="25" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="12" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="12" t="s">
         <v>613</v>
       </c>
@@ -3269,8 +3490,11 @@
       <c r="L6" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="12" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="12" t="s">
         <v>613</v>
       </c>
@@ -3280,8 +3504,11 @@
       <c r="L7" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="12" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="12" t="s">
         <v>613</v>
       </c>
@@ -3292,7 +3519,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="12" t="s">
         <v>613</v>
       </c>
@@ -3300,7 +3527,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="12" t="s">
         <v>613</v>
       </c>
@@ -3311,7 +3538,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>166</v>
       </c>
@@ -3355,8 +3582,11 @@
       <c r="P11" s="12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="12" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>630</v>
       </c>
@@ -3405,8 +3635,11 @@
       <c r="P12" s="12" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="12" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="12" t="s">
         <v>630</v>
       </c>
@@ -3452,8 +3685,11 @@
       <c r="P13" s="12" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="12" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="12" t="s">
         <v>630</v>
       </c>
@@ -3499,8 +3735,11 @@
       <c r="P14" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="12" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="12" t="s">
         <v>630</v>
       </c>
@@ -3549,8 +3788,11 @@
       <c r="P15" s="12" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="12" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="12" t="s">
         <v>630</v>
       </c>
@@ -3599,8 +3841,11 @@
       <c r="P16" s="12" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="12" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="12" t="s">
         <v>630</v>
       </c>
@@ -3644,8 +3889,11 @@
       <c r="P17" s="12" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="12" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="12" t="s">
         <v>630</v>
       </c>
@@ -3694,8 +3942,11 @@
       <c r="P18" s="12" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="12" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="12" t="s">
         <v>630</v>
       </c>
@@ -3744,8 +3995,11 @@
       <c r="P19" s="12" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="12" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="12" t="s">
         <v>630</v>
       </c>
@@ -3794,8 +4048,11 @@
       <c r="P20" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" s="12" customFormat="1">
+      <c r="Q20" s="12" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="12" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>630</v>
       </c>
@@ -3813,8 +4070,11 @@
       <c r="P21" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="12" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="12" t="s">
         <v>630</v>
       </c>
@@ -3860,8 +4120,11 @@
       <c r="P22" s="12" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" s="12" customFormat="1">
+      <c r="Q22" s="12" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="12" customFormat="1">
       <c r="A23" s="12" t="s">
         <v>630</v>
       </c>
@@ -3879,8 +4142,11 @@
       <c r="P23" s="12" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" s="12" customFormat="1">
+      <c r="Q23" s="12" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="12" customFormat="1">
       <c r="A24" s="12" t="s">
         <v>630</v>
       </c>
@@ -3898,8 +4164,11 @@
       <c r="P24" s="12" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" s="12" customFormat="1">
+      <c r="Q24" s="12" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" s="12" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>630</v>
       </c>
@@ -3917,8 +4186,11 @@
       <c r="P25" s="12" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="12" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -3964,8 +4236,11 @@
       <c r="P26" s="12" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -4011,8 +4286,11 @@
       <c r="P27" s="12" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="12" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -4058,8 +4336,11 @@
       <c r="P28" s="12" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="12" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -4105,8 +4386,11 @@
       <c r="P29" s="12" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="27" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -4152,8 +4436,11 @@
       <c r="P30" s="12" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="12" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -4199,8 +4486,11 @@
       <c r="P31" s="12" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="12" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -4246,8 +4536,11 @@
       <c r="P32" s="12" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="12" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -4293,8 +4586,11 @@
       <c r="P33" s="12" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="12" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -4343,8 +4639,11 @@
       <c r="P34" s="12" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" ht="15">
+      <c r="Q34" s="12" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -4379,8 +4678,11 @@
       <c r="P35" s="12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="Q35" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="12" customFormat="1" ht="15">
       <c r="A36" s="12" t="s">
         <v>49</v>
       </c>
@@ -4404,7 +4706,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="37" spans="1:17" s="12" customFormat="1" ht="15">
       <c r="A37" s="12" t="s">
         <v>49</v>
       </c>
@@ -4415,8 +4717,11 @@
       <c r="D37" s="23"/>
       <c r="E37" s="22"/>
       <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:16" s="12" customFormat="1" ht="15">
+      <c r="Q37" s="12" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="12" customFormat="1" ht="15">
       <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
@@ -4427,8 +4732,11 @@
       <c r="D38" s="23"/>
       <c r="E38" s="22"/>
       <c r="F38" s="16"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="12" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -4477,8 +4785,11 @@
       <c r="P39" s="12" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" s="12" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -4527,8 +4838,11 @@
       <c r="P40" s="12" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" s="12" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -4558,7 +4872,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -4607,8 +4921,11 @@
       <c r="P42" s="12" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" s="12" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -4638,7 +4955,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -4688,7 +5005,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -4713,7 +5030,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4738,7 +5055,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -4763,7 +5080,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="12" customFormat="1">
+    <row r="48" spans="1:17" s="12" customFormat="1">
       <c r="A48" s="12" t="s">
         <v>49</v>
       </c>
@@ -4778,7 +5095,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="12" customFormat="1">
+    <row r="49" spans="1:17" s="12" customFormat="1">
       <c r="A49" s="12" t="s">
         <v>49</v>
       </c>
@@ -4793,7 +5110,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="12" customFormat="1">
+    <row r="50" spans="1:17" s="12" customFormat="1">
       <c r="A50" s="12" t="s">
         <v>49</v>
       </c>
@@ -4813,8 +5130,11 @@
       <c r="P50" s="12" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="Q50" s="12" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -4842,7 +5162,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4872,7 +5192,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -4922,7 +5242,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="12" customFormat="1">
+    <row r="54" spans="1:17" s="12" customFormat="1">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -4946,7 +5266,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="12" customFormat="1">
+    <row r="55" spans="1:17" s="12" customFormat="1">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
@@ -4970,7 +5290,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -5019,8 +5339,11 @@
       <c r="P56" s="12" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56" s="12" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -5059,8 +5382,11 @@
       <c r="P57" s="12" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57" s="12" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -5109,8 +5435,11 @@
       <c r="P58" s="12" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58" s="12" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -5149,8 +5478,11 @@
       <c r="P59" s="12" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" s="12" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -5199,8 +5531,11 @@
       <c r="P60" s="12" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60" s="12" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -5250,7 +5585,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -5300,7 +5635,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -5349,8 +5684,11 @@
       <c r="P63" s="12" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63" s="12" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -5399,8 +5737,11 @@
       <c r="P64" s="12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64" s="12" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -5450,7 +5791,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -5479,7 +5820,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -5523,8 +5864,11 @@
       <c r="P67" s="12" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67" s="12" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -5568,8 +5912,11 @@
       <c r="P68" s="12" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" s="12" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -5603,8 +5950,11 @@
       <c r="P69" s="12" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" s="2" customFormat="1">
+      <c r="Q69" s="12" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="2" customFormat="1">
       <c r="A70" s="2" t="s">
         <v>70</v>
       </c>
@@ -5638,8 +5988,11 @@
       <c r="P70" s="12" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" s="2" customFormat="1">
+      <c r="Q70" s="12" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -5673,8 +6026,11 @@
       <c r="P71" s="12" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" s="2" customFormat="1">
+      <c r="Q71" s="12" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -5719,8 +6075,11 @@
       <c r="P72" s="12" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" s="12" customFormat="1">
+      <c r="Q72" s="12" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="12" customFormat="1">
       <c r="A73" s="12" t="s">
         <v>70</v>
       </c>
@@ -5763,8 +6122,11 @@
       <c r="P73" s="12" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" s="2" customFormat="1">
+      <c r="Q73" s="12" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="2" customFormat="1">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -5813,8 +6175,9 @@
       <c r="P74" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" s="2" customFormat="1">
+      <c r="Q74" s="12"/>
+    </row>
+    <row r="75" spans="1:17" s="2" customFormat="1">
       <c r="A75" s="2" t="s">
         <v>70</v>
       </c>
@@ -5863,8 +6226,11 @@
       <c r="P75" s="12" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" s="12" customFormat="1">
+      <c r="Q75" s="12" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" s="12" customFormat="1">
       <c r="A76" s="12" t="s">
         <v>70</v>
       </c>
@@ -5907,648 +6273,721 @@
       <c r="P76" s="12" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" s="2" customFormat="1">
-      <c r="A77" s="2" t="s">
+      <c r="Q76" s="12" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" s="12" customFormat="1">
+      <c r="A77" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>542</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="E77" s="22" t="s">
-        <v>544</v>
-      </c>
+      <c r="B77" s="12" t="s">
+        <v>910</v>
+      </c>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
       <c r="F77" s="14"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="4"/>
-      <c r="J77" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="N77" s="12" t="s">
-        <v>667</v>
-      </c>
-      <c r="O77" s="25" t="s">
-        <v>720</v>
-      </c>
-      <c r="P77" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" s="2" customFormat="1">
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="O77" s="14"/>
+      <c r="Q77" s="12" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="2" customFormat="1">
       <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>546</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>547</v>
+        <v>542</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>544</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="12"/>
       <c r="H78" s="4"/>
       <c r="J78" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="N78" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O78" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="P78" s="12" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" s="2" customFormat="1">
+        <v>285</v>
+      </c>
+      <c r="Q78" s="12" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" s="2" customFormat="1">
       <c r="A79" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>76</v>
+        <v>251</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="E79" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="G79" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>78</v>
+        <v>545</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="F79" s="14"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="4"/>
+      <c r="J79" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>80</v>
+        <v>753</v>
       </c>
       <c r="N79" s="12" t="s">
-        <v>669</v>
-      </c>
-      <c r="O79" s="26" t="s">
-        <v>722</v>
+        <v>668</v>
+      </c>
+      <c r="O79" s="25" t="s">
+        <v>721</v>
       </c>
       <c r="P79" s="12" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" s="2" customFormat="1">
+        <v>837</v>
+      </c>
+      <c r="Q79" s="12" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" s="2" customFormat="1">
       <c r="A80" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="O80" s="26" t="s">
+        <v>722</v>
+      </c>
+      <c r="P80" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="Q80" s="12" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" s="2" customFormat="1">
+      <c r="A81" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C81" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="D81" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F81" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="G80" s="12" t="s">
+      <c r="G81" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="H81" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I81" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J81" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K81" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="L81" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="N80" s="12" t="s">
+      <c r="N81" s="12" t="s">
         <v>670</v>
       </c>
-      <c r="O80" s="25" t="s">
+      <c r="O81" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="P80" s="12" t="s">
+      <c r="P81" s="12" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
-      <c r="A81" t="s">
-        <v>171</v>
-      </c>
-      <c r="B81" t="s">
-        <v>172</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="D81" s="22" t="s">
-        <v>554</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J81" t="s">
-        <v>173</v>
-      </c>
-      <c r="K81" t="s">
-        <v>174</v>
-      </c>
-      <c r="L81" t="s">
-        <v>172</v>
-      </c>
-      <c r="M81" t="s">
-        <v>173</v>
-      </c>
-      <c r="N81" s="12" t="s">
-        <v>671</v>
-      </c>
-      <c r="O81" s="25" t="s">
-        <v>724</v>
-      </c>
-      <c r="P81" s="12" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81" s="12" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
       <c r="A82" t="s">
         <v>171</v>
       </c>
       <c r="B82" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J82" t="s">
+        <v>173</v>
+      </c>
+      <c r="K82" t="s">
+        <v>174</v>
+      </c>
+      <c r="L82" t="s">
+        <v>172</v>
+      </c>
+      <c r="M82" t="s">
+        <v>173</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="O82" s="25" t="s">
+        <v>724</v>
+      </c>
+      <c r="P82" s="12" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q82" s="12" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" t="s">
         <v>175</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C83" s="22" t="s">
         <v>556</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="D83" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="E82" s="22" t="s">
+      <c r="E83" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="F82" s="16" t="s">
+      <c r="F83" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="G82" s="12" t="s">
+      <c r="G83" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H83" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I82" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J83" t="s">
         <v>176</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K83" t="s">
         <v>177</v>
       </c>
-      <c r="L82" t="s">
+      <c r="L83" t="s">
         <v>178</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M83" t="s">
         <v>179</v>
       </c>
-      <c r="N82" s="12" t="s">
+      <c r="N83" s="12" t="s">
         <v>672</v>
       </c>
-      <c r="O82" s="26" t="s">
+      <c r="O83" s="26" t="s">
         <v>725</v>
       </c>
-      <c r="P82" s="12" t="s">
+      <c r="P83" s="12" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" ht="28.8">
-      <c r="A83" s="12" t="s">
-        <v>631</v>
-      </c>
-      <c r="B83" t="s">
-        <v>183</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="D83" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="E83" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="F83" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="G83" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H83" s="4"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L83" t="s">
-        <v>754</v>
-      </c>
-      <c r="O83" s="25" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" ht="28.8">
+      <c r="Q83" s="12" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" ht="28.8">
       <c r="A84" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>564</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>385</v>
+        <v>561</v>
+      </c>
+      <c r="F84" s="21" t="s">
+        <v>384</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="1"/>
       <c r="J84" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L84" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O84" s="25" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" ht="28.8">
+        <v>726</v>
+      </c>
+      <c r="Q84" s="12" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" ht="28.8">
       <c r="A85" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G85" s="12"/>
+        <v>385</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>340</v>
+      </c>
       <c r="H85" s="4"/>
       <c r="I85" s="1"/>
       <c r="J85" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L85" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" ht="28.8">
+        <v>755</v>
+      </c>
+      <c r="O85" s="25" t="s">
+        <v>727</v>
+      </c>
+      <c r="Q85" s="12" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" ht="28.8">
       <c r="A86" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B86" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>341</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="G86" s="12"/>
       <c r="H86" s="4"/>
       <c r="I86" s="1"/>
       <c r="J86" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L86" t="s">
-        <v>757</v>
-      </c>
-      <c r="O86" s="26" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16">
+        <v>756</v>
+      </c>
+      <c r="Q86" s="12" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="28.8">
       <c r="A87" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B87" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="E87" s="24" t="s">
-        <v>573</v>
+        <v>569</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>570</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="1"/>
       <c r="J87" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L87" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="O87" s="26" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" ht="28.8">
+        <v>728</v>
+      </c>
+      <c r="Q87" s="12" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B88" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>576</v>
+        <v>572</v>
+      </c>
+      <c r="E88" s="24" t="s">
+        <v>573</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="1"/>
       <c r="J88" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L88" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="O88" s="26" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" ht="28.8">
+        <v>729</v>
+      </c>
+      <c r="Q88" s="12" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="28.8">
       <c r="A89" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E89" s="22" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G89" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="1"/>
       <c r="J89" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L89" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="O89" s="26" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="28.8">
+        <v>730</v>
+      </c>
+      <c r="Q89" s="12" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" ht="28.8">
       <c r="A90" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B90" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E90" s="22" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="1"/>
       <c r="J90" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L90" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="O90" s="26" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" ht="28.8">
+        <v>731</v>
+      </c>
+      <c r="Q90" s="12" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" ht="28.8">
       <c r="A91" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E91" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="F91" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="G91" s="13" t="s">
-        <v>346</v>
+        <v>582</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>345</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="1"/>
       <c r="J91" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L91" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="O91" s="26" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16">
+        <v>732</v>
+      </c>
+      <c r="Q91" s="12" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="28.8">
       <c r="A92" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E92" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="F92" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="G92" s="12" t="s">
-        <v>347</v>
+        <v>585</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="G92" s="13" t="s">
+        <v>346</v>
       </c>
       <c r="H92" s="4"/>
       <c r="I92" s="1"/>
       <c r="J92" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="L92" s="12" t="s">
-        <v>762</v>
+        <v>295</v>
+      </c>
+      <c r="L92" t="s">
+        <v>764</v>
       </c>
       <c r="O92" s="26" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16">
+        <v>733</v>
+      </c>
+      <c r="Q92" s="12" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17">
       <c r="A93" s="12" t="s">
         <v>631</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E93" s="22" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G93" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="1"/>
       <c r="J93" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="L93" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="O93" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q93" s="12" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="A94" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="H94" s="4"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L93" s="12" t="s">
+      <c r="L94" s="12" t="s">
         <v>763</v>
       </c>
-      <c r="O93" s="26" t="s">
+      <c r="O94" s="26" t="s">
         <v>735</v>
       </c>
+      <c r="Q94" s="12" t="s">
+        <v>909</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P93" xr:uid="{A4C0DE7B-B5FD-4B2E-A3DB-E7CF10EF5495}"/>
+  <autoFilter ref="A1:Q94" xr:uid="{D2D53F92-7994-419F-B91C-749F7CB570B6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>